<commit_message>
Add VSR auto-reload feature and update documentation
- Modified VSR Enhanced Tracker to check for new Long_Reversal_Daily files every 5 minutes
- No service restart required when new scan results arrive
- Added VSR tracker and SL watchdog dashboard to job manager
- Updated VSR dashboard guide with auto-reload feature
- Updated documentation index with new features
- New tickers are automatically detected and tracked within minutes
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="132">
   <si>
     <t>Ticker</t>
   </si>
@@ -61,282 +61,273 @@
     <t>PAYTM</t>
   </si>
   <si>
+    <t>DALBHARAT</t>
+  </si>
+  <si>
+    <t>AMBUJACEM</t>
+  </si>
+  <si>
+    <t>NMDC</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>KIMS</t>
+  </si>
+  <si>
+    <t>DIXON</t>
+  </si>
+  <si>
+    <t>LXCHEM</t>
+  </si>
+  <si>
+    <t>OLECTRA</t>
+  </si>
+  <si>
     <t>BIKAJI</t>
   </si>
   <si>
-    <t>AMBUJACEM</t>
-  </si>
-  <si>
-    <t>NMDC</t>
-  </si>
-  <si>
-    <t>KIMS</t>
-  </si>
-  <si>
-    <t>DIXON</t>
-  </si>
-  <si>
-    <t>OLECTRA</t>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>ANANDRATHI</t>
+  </si>
+  <si>
+    <t>NUVOCO</t>
+  </si>
+  <si>
+    <t>ASHAPURMIN</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>ELGIEQUIP</t>
+  </si>
+  <si>
+    <t>PRAKASH</t>
+  </si>
+  <si>
+    <t>SHK</t>
+  </si>
+  <si>
+    <t>UPL</t>
+  </si>
+  <si>
+    <t>GREENPLY</t>
+  </si>
+  <si>
+    <t>DELHIVERY</t>
+  </si>
+  <si>
+    <t>SWIGGY</t>
+  </si>
+  <si>
+    <t>CREDITACC</t>
+  </si>
+  <si>
+    <t>GLAND</t>
+  </si>
+  <si>
+    <t>TANLA</t>
+  </si>
+  <si>
+    <t>MEDANTA</t>
+  </si>
+  <si>
+    <t>PATANJALI</t>
+  </si>
+  <si>
+    <t>RAMCOCEM</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>SUMICHEM</t>
+  </si>
+  <si>
+    <t>NAVA</t>
+  </si>
+  <si>
+    <t>NLCINDIA</t>
+  </si>
+  <si>
+    <t>PEL</t>
+  </si>
+  <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>THERMAX</t>
+  </si>
+  <si>
+    <t>GLENMARK</t>
+  </si>
+  <si>
+    <t>AJANTPHARM</t>
+  </si>
+  <si>
+    <t>MRF</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>CRAFTSMAN</t>
+  </si>
+  <si>
+    <t>IIFL</t>
+  </si>
+  <si>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>FORCEMOT</t>
+  </si>
+  <si>
+    <t>BORORENEW</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>TATAMOTORS</t>
+  </si>
+  <si>
+    <t>METROPOLIS</t>
   </si>
   <si>
     <t>3MINDIA</t>
   </si>
   <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>NUVOCO</t>
-  </si>
-  <si>
-    <t>ASHAPURMIN</t>
-  </si>
-  <si>
-    <t>AGI</t>
-  </si>
-  <si>
-    <t>ELGIEQUIP</t>
-  </si>
-  <si>
-    <t>SHK</t>
-  </si>
-  <si>
-    <t>GREENPLY</t>
-  </si>
-  <si>
-    <t>UPL</t>
-  </si>
-  <si>
-    <t>SWIGGY</t>
-  </si>
-  <si>
-    <t>DELHIVERY</t>
-  </si>
-  <si>
-    <t>PRAKASH</t>
-  </si>
-  <si>
-    <t>CREDITACC</t>
-  </si>
-  <si>
-    <t>TANLA</t>
-  </si>
-  <si>
-    <t>PATANJALI</t>
-  </si>
-  <si>
-    <t>RAMCOCEM</t>
-  </si>
-  <si>
-    <t>GLAND</t>
-  </si>
-  <si>
-    <t>SUMICHEM</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
-  </si>
-  <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
-    <t>MEDANTA</t>
-  </si>
-  <si>
-    <t>SWANENERGY</t>
-  </si>
-  <si>
-    <t>NAVA</t>
-  </si>
-  <si>
-    <t>NLCINDIA</t>
-  </si>
-  <si>
-    <t>THERMAX</t>
-  </si>
-  <si>
-    <t>TORNTPHARM</t>
-  </si>
-  <si>
-    <t>AJANTPHARM</t>
-  </si>
-  <si>
-    <t>CUMMINSIND</t>
-  </si>
-  <si>
-    <t>MRF</t>
-  </si>
-  <si>
-    <t>CRAFTSMAN</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
-    <t>IIFL</t>
-  </si>
-  <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>FORCEMOT</t>
-  </si>
-  <si>
-    <t>BORORENEW</t>
-  </si>
-  <si>
-    <t>PTC</t>
-  </si>
-  <si>
-    <t>METROPOLIS</t>
-  </si>
-  <si>
     <t>ETERNAL</t>
   </si>
   <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>ZFCVINDIA</t>
-  </si>
-  <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
-    <t>LXCHEM</t>
-  </si>
-  <si>
     <t>VIJAYA</t>
   </si>
   <si>
+    <t>RAINBOW</t>
+  </si>
+  <si>
+    <t>PENIND</t>
+  </si>
+  <si>
     <t>GMDCLTD</t>
   </si>
   <si>
-    <t>PENIND</t>
-  </si>
-  <si>
     <t>IPCALAB</t>
   </si>
   <si>
-    <t>TATAMOTORS</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>MRPL</t>
+    <t>FINPIPE</t>
+  </si>
+  <si>
+    <t>HINDALCO</t>
+  </si>
+  <si>
+    <t>CGCL</t>
+  </si>
+  <si>
+    <t>MHRIL</t>
   </si>
   <si>
     <t>GPPL</t>
   </si>
   <si>
-    <t>MHRIL</t>
+    <t>ICICIBANK</t>
+  </si>
+  <si>
+    <t>BALKRISIND</t>
+  </si>
+  <si>
+    <t>BIRLACORPN</t>
   </si>
   <si>
     <t>NAVINFLUOR</t>
   </si>
   <si>
-    <t>ICICIBANK</t>
-  </si>
-  <si>
-    <t>BIRLACORPN</t>
+    <t>HDFCBANK</t>
+  </si>
+  <si>
+    <t>LALPATHLAB</t>
+  </si>
+  <si>
+    <t>ARE&amp;M</t>
+  </si>
+  <si>
+    <t>JMFINANCIL</t>
+  </si>
+  <si>
+    <t>APOLLOHOSP</t>
   </si>
   <si>
     <t>APOLLOTYRE</t>
   </si>
   <si>
-    <t>HDFCBANK</t>
-  </si>
-  <si>
-    <t>ARE&amp;M</t>
-  </si>
-  <si>
-    <t>RAINBOW</t>
+    <t>LAURUSLABS</t>
   </si>
   <si>
     <t>TIMKEN</t>
   </si>
   <si>
-    <t>BALKRISIND</t>
-  </si>
-  <si>
-    <t>JMFINANCIL</t>
-  </si>
-  <si>
-    <t>HINDALCO</t>
-  </si>
-  <si>
-    <t>CGCL</t>
-  </si>
-  <si>
-    <t>LALPATHLAB</t>
-  </si>
-  <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
     <t>M&amp;M</t>
   </si>
   <si>
     <t>JKCEMENT</t>
   </si>
   <si>
-    <t>VGUARD</t>
+    <t>BLUEDART</t>
   </si>
   <si>
     <t>ALKEM</t>
   </si>
   <si>
-    <t>APOLLOHOSP</t>
-  </si>
-  <si>
-    <t>ANDHRSUGAR</t>
-  </si>
-  <si>
     <t>KALYANKJIL</t>
   </si>
   <si>
     <t>SHREECEM</t>
   </si>
   <si>
+    <t>ASAHIINDIA</t>
+  </si>
+  <si>
     <t>TMB</t>
   </si>
   <si>
-    <t>CASTROLIND</t>
-  </si>
-  <si>
-    <t>JBCHEPHARM</t>
-  </si>
-  <si>
-    <t>BLUEDART</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
+    <t>Basic Materials</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
     <t>Consumer Defensive</t>
   </si>
   <si>
-    <t>Basic Materials</t>
-  </si>
-  <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Industrials</t>
-  </si>
-  <si>
     <t>Financial Services</t>
   </si>
   <si>
     <t>Consumer Cyclical</t>
   </si>
   <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
     <t>Utilities</t>
   </si>
   <si>
@@ -370,37 +361,37 @@
     <t>2025-07-11</t>
   </si>
   <si>
+    <t>2025-07-18</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
+    <t>2025-07-09</t>
+  </si>
+  <si>
     <t>2025-07-16</t>
   </si>
   <si>
-    <t>2025-07-07</t>
-  </si>
-  <si>
-    <t>2025-07-18</t>
-  </si>
-  <si>
-    <t>2025-07-08</t>
-  </si>
-  <si>
-    <t>2025-07-09</t>
-  </si>
-  <si>
     <t>2025-07-15</t>
   </si>
   <si>
     <t>2025-07-22</t>
   </si>
   <si>
+    <t>2025-07-24</t>
+  </si>
+  <si>
+    <t>2025-07-21</t>
+  </si>
+  <si>
+    <t>2025-07-17</t>
+  </si>
+  <si>
     <t>2025-07-10</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
-  </si>
-  <si>
-    <t>2025-07-21</t>
-  </si>
-  <si>
-    <t>2025-07-17</t>
   </si>
   <si>
     <t>G PATTERN CONFIRMED - FULL POSITION (100%)</t>
@@ -776,7 +767,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -831,19 +822,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -852,19 +843,19 @@
         <v>3</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K2">
-        <v>1109.3</v>
+        <v>1109.4</v>
       </c>
       <c r="L2">
-        <v>1041.92</v>
+        <v>1039.35</v>
       </c>
       <c r="M2">
-        <v>1244.06</v>
+        <v>1249.5</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -875,19 +866,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>45.78</v>
       </c>
       <c r="E3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -896,19 +887,19 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K3">
-        <v>795.2</v>
+        <v>2287.2</v>
       </c>
       <c r="L3">
-        <v>758.85</v>
+        <v>2176.49</v>
       </c>
       <c r="M3">
-        <v>867.9</v>
+        <v>2508.62</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -919,19 +910,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D4">
         <v>45.78</v>
       </c>
       <c r="E4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -943,16 +934,16 @@
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K4">
-        <v>620</v>
+        <v>621.15</v>
       </c>
       <c r="L4">
-        <v>599.72</v>
+        <v>600.87</v>
       </c>
       <c r="M4">
-        <v>660.5599999999999</v>
+        <v>661.71</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -963,19 +954,19 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D5">
         <v>39.76</v>
       </c>
       <c r="E5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G5">
         <v>81.27</v>
@@ -987,16 +978,16 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="K5">
-        <v>72.63</v>
+        <v>72.62</v>
       </c>
       <c r="L5">
-        <v>69.89</v>
+        <v>69.88</v>
       </c>
       <c r="M5">
-        <v>78.12</v>
+        <v>78.11</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -1007,40 +998,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D6">
-        <v>61.99</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="E6">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G6">
-        <v>61.99</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K6">
-        <v>777.55</v>
+        <v>840</v>
       </c>
       <c r="L6">
-        <v>737.35</v>
+        <v>797.64</v>
       </c>
       <c r="M6">
-        <v>857.95</v>
+        <v>924.71</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -1051,22 +1042,22 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D7">
-        <v>53.55</v>
+        <v>66.81</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G7">
-        <v>53.55</v>
+        <v>66.81</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1075,16 +1066,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K7">
-        <v>16715</v>
+        <v>792.65</v>
       </c>
       <c r="L7">
-        <v>16005.57</v>
+        <v>750.34</v>
       </c>
       <c r="M7">
-        <v>18133.86</v>
+        <v>877.26</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1095,40 +1086,40 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D8">
-        <v>90.06</v>
+        <v>53.55</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G8">
-        <v>90.06</v>
+        <v>53.55</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K8">
-        <v>1364.4</v>
+        <v>16717</v>
       </c>
       <c r="L8">
-        <v>1283.73</v>
+        <v>16007.57</v>
       </c>
       <c r="M8">
-        <v>1525.74</v>
+        <v>18135.86</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1139,40 +1130,40 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D9">
-        <v>38.55</v>
+        <v>52.17</v>
       </c>
       <c r="E9">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G9">
-        <v>92.47</v>
+        <v>52.17</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K9">
-        <v>31730</v>
+        <v>206.03</v>
       </c>
       <c r="L9">
-        <v>30400</v>
+        <v>195.59</v>
       </c>
       <c r="M9">
-        <v>34390</v>
+        <v>226.91</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1183,40 +1174,40 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D10">
-        <v>38.55</v>
+        <v>90.06</v>
       </c>
       <c r="E10">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>90.06</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K10">
-        <v>480.5</v>
+        <v>1433</v>
       </c>
       <c r="L10">
-        <v>433.28</v>
+        <v>1346.57</v>
       </c>
       <c r="M10">
-        <v>574.9400000000001</v>
+        <v>1605.86</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1227,40 +1218,40 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D11">
-        <v>38.55</v>
+        <v>39.76</v>
       </c>
       <c r="E11">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G11">
-        <v>96.08</v>
+        <v>100</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K11">
-        <v>2603.9</v>
+        <v>794.2</v>
       </c>
       <c r="L11">
-        <v>2398.37</v>
+        <v>757.85</v>
       </c>
       <c r="M11">
-        <v>3014.96</v>
+        <v>866.9</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1271,40 +1262,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D12">
-        <v>37.35</v>
+        <v>39.76</v>
       </c>
       <c r="E12">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G12">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K12">
-        <v>414.3</v>
+        <v>948.05</v>
       </c>
       <c r="L12">
-        <v>387.27</v>
+        <v>903.29</v>
       </c>
       <c r="M12">
-        <v>468.36</v>
+        <v>1037.58</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1315,16 +1306,16 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D13">
-        <v>37.35</v>
+        <v>38.55</v>
       </c>
       <c r="E13">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>119</v>
@@ -1336,19 +1327,19 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K13">
-        <v>579.4</v>
+        <v>493.3</v>
       </c>
       <c r="L13">
-        <v>529.1900000000001</v>
+        <v>446.08</v>
       </c>
       <c r="M13">
-        <v>679.8099999999999</v>
+        <v>587.74</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1359,40 +1350,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14">
-        <v>37.35</v>
+        <v>38.55</v>
       </c>
       <c r="E14">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G14">
-        <v>100</v>
+        <v>96.08</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K14">
-        <v>956.7</v>
+        <v>2634.3</v>
       </c>
       <c r="L14">
-        <v>875.3099999999999</v>
+        <v>2428.77</v>
       </c>
       <c r="M14">
-        <v>1119.49</v>
+        <v>3045.36</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1403,22 +1394,22 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D15">
-        <v>36.14</v>
+        <v>37.35</v>
       </c>
       <c r="E15">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G15">
-        <v>70.42</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1427,16 +1418,16 @@
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K15">
-        <v>595</v>
+        <v>415</v>
       </c>
       <c r="L15">
-        <v>560.4299999999999</v>
+        <v>387.97</v>
       </c>
       <c r="M15">
-        <v>664.14</v>
+        <v>469.06</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1447,19 +1438,19 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D16">
-        <v>33.73</v>
+        <v>37.35</v>
       </c>
       <c r="E16">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G16">
         <v>100</v>
@@ -1468,19 +1459,19 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K16">
-        <v>265.44</v>
+        <v>574</v>
       </c>
       <c r="L16">
-        <v>251.59</v>
+        <v>523.79</v>
       </c>
       <c r="M16">
-        <v>293.14</v>
+        <v>674.41</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1491,40 +1482,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D17">
-        <v>32.53</v>
+        <v>37.35</v>
       </c>
       <c r="E17">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G17">
-        <v>76.81</v>
+        <v>100</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K17">
-        <v>344.4</v>
+        <v>955</v>
       </c>
       <c r="L17">
-        <v>324.61</v>
+        <v>873.6</v>
       </c>
       <c r="M17">
-        <v>383.97</v>
+        <v>1117.8</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1535,40 +1526,40 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D18">
-        <v>32.53</v>
+        <v>36.14</v>
       </c>
       <c r="E18">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G18">
-        <v>85.23999999999999</v>
+        <v>70.42</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K18">
-        <v>719.05</v>
+        <v>590.5</v>
       </c>
       <c r="L18">
-        <v>687.03</v>
+        <v>555.9299999999999</v>
       </c>
       <c r="M18">
-        <v>783.09</v>
+        <v>659.64</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1579,22 +1570,22 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D19">
-        <v>30.12</v>
+        <v>34.94</v>
       </c>
       <c r="E19">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G19">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -1603,16 +1594,16 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K19">
-        <v>417.55</v>
+        <v>182.25</v>
       </c>
       <c r="L19">
-        <v>390.9</v>
+        <v>170.43</v>
       </c>
       <c r="M19">
-        <v>470.85</v>
+        <v>205.89</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1623,16 +1614,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D20">
-        <v>30.12</v>
+        <v>33.73</v>
       </c>
       <c r="E20">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
         <v>119</v>
@@ -1644,19 +1635,19 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K20">
-        <v>440.3</v>
+        <v>263.26</v>
       </c>
       <c r="L20">
-        <v>418.39</v>
+        <v>249.41</v>
       </c>
       <c r="M20">
-        <v>484.11</v>
+        <v>290.96</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1667,22 +1658,22 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D21">
-        <v>30.12</v>
+        <v>32.53</v>
       </c>
       <c r="E21">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1691,16 +1682,16 @@
         <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K21">
-        <v>179.89</v>
+        <v>720.9</v>
       </c>
       <c r="L21">
-        <v>168.3</v>
+        <v>688.88</v>
       </c>
       <c r="M21">
-        <v>203.08</v>
+        <v>784.9400000000001</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1711,40 +1702,40 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D22">
-        <v>28.92</v>
+        <v>32.53</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
         <v>119</v>
       </c>
       <c r="G22">
-        <v>70.42</v>
+        <v>76.81</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K22">
-        <v>1367.4</v>
+        <v>343.8</v>
       </c>
       <c r="L22">
-        <v>1268.41</v>
+        <v>324.01</v>
       </c>
       <c r="M22">
-        <v>1565.37</v>
+        <v>383.37</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1755,40 +1746,40 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D23">
-        <v>25.3</v>
+        <v>32.53</v>
       </c>
       <c r="E23">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G23">
-        <v>71.98999999999999</v>
+        <v>100</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K23">
-        <v>674.05</v>
+        <v>442.2</v>
       </c>
       <c r="L23">
-        <v>645.5700000000001</v>
+        <v>420.29</v>
       </c>
       <c r="M23">
-        <v>731</v>
+        <v>486.01</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1799,40 +1790,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D24">
-        <v>24.1</v>
+        <v>31.33</v>
       </c>
       <c r="E24">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>82.83</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K24">
-        <v>1913.4</v>
+        <v>416.6</v>
       </c>
       <c r="L24">
-        <v>1812.94</v>
+        <v>388.51</v>
       </c>
       <c r="M24">
-        <v>2114.31</v>
+        <v>472.77</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1843,19 +1834,19 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D25">
-        <v>22.89</v>
+        <v>30.12</v>
       </c>
       <c r="E25">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G25">
         <v>70.42</v>
@@ -1867,16 +1858,16 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K25">
-        <v>1177.5</v>
+        <v>1362</v>
       </c>
       <c r="L25">
-        <v>1112.18</v>
+        <v>1263.01</v>
       </c>
       <c r="M25">
-        <v>1308.14</v>
+        <v>1559.97</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1887,19 +1878,19 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D26">
-        <v>22.89</v>
+        <v>26.51</v>
       </c>
       <c r="E26">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G26">
         <v>86.45</v>
@@ -1911,16 +1902,16 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K26">
-        <v>2024.2</v>
+        <v>2035.9</v>
       </c>
       <c r="L26">
-        <v>1904.6</v>
+        <v>1916.3</v>
       </c>
       <c r="M26">
-        <v>2263.4</v>
+        <v>2275.1</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1931,40 +1922,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D27">
-        <v>20.48</v>
+        <v>25.3</v>
       </c>
       <c r="E27">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G27">
-        <v>100</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K27">
-        <v>595.1</v>
+        <v>673</v>
       </c>
       <c r="L27">
-        <v>556.54</v>
+        <v>645.4</v>
       </c>
       <c r="M27">
-        <v>672.21</v>
+        <v>728.2</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1975,19 +1966,19 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D28">
-        <v>19.28</v>
+        <v>25.3</v>
       </c>
       <c r="E28">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G28">
         <v>100</v>
@@ -1996,19 +1987,19 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K28">
-        <v>5555</v>
+        <v>1329.2</v>
       </c>
       <c r="L28">
-        <v>5318</v>
+        <v>1256.76</v>
       </c>
       <c r="M28">
-        <v>6029</v>
+        <v>1474.09</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -2019,19 +2010,19 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D29">
-        <v>19.28</v>
+        <v>24.1</v>
       </c>
       <c r="E29">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G29">
         <v>100</v>
@@ -2040,19 +2031,19 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K29">
-        <v>398.75</v>
+        <v>1903.6</v>
       </c>
       <c r="L29">
-        <v>379.68</v>
+        <v>1802.43</v>
       </c>
       <c r="M29">
-        <v>436.89</v>
+        <v>2105.94</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -2063,40 +2054,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D30">
-        <v>18.07</v>
+        <v>22.89</v>
       </c>
       <c r="E30">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G30">
-        <v>100</v>
+        <v>70.42</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K30">
-        <v>1323.5</v>
+        <v>1181.1</v>
       </c>
       <c r="L30">
-        <v>1254.92</v>
+        <v>1112.52</v>
       </c>
       <c r="M30">
-        <v>1460.65</v>
+        <v>1318.26</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -2107,40 +2098,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D31">
-        <v>16.87</v>
+        <v>22.89</v>
       </c>
       <c r="E31">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G31">
         <v>100</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K31">
-        <v>512.5</v>
+        <v>5560.5</v>
       </c>
       <c r="L31">
-        <v>473.45</v>
+        <v>5323.5</v>
       </c>
       <c r="M31">
-        <v>590.6</v>
+        <v>6034.5</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2151,22 +2142,22 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D32">
-        <v>16.87</v>
+        <v>20.48</v>
       </c>
       <c r="E32">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G32">
-        <v>75.42</v>
+        <v>100</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2175,16 +2166,16 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K32">
-        <v>636.35</v>
+        <v>595.15</v>
       </c>
       <c r="L32">
-        <v>601.7</v>
+        <v>556.59</v>
       </c>
       <c r="M32">
-        <v>705.65</v>
+        <v>672.26</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2195,40 +2186,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D33">
-        <v>15.66</v>
+        <v>16.87</v>
       </c>
       <c r="E33">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G33">
-        <v>70.78</v>
+        <v>75.42</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K33">
-        <v>244.69</v>
+        <v>635.5</v>
       </c>
       <c r="L33">
-        <v>232.33</v>
+        <v>600.85</v>
       </c>
       <c r="M33">
-        <v>269.42</v>
+        <v>704.8</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2239,40 +2230,40 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D34">
-        <v>14.46</v>
+        <v>15.66</v>
       </c>
       <c r="E34">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G34">
-        <v>100</v>
+        <v>70.78</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K34">
-        <v>3872.9</v>
+        <v>245.61</v>
       </c>
       <c r="L34">
-        <v>3632.53</v>
+        <v>233.25</v>
       </c>
       <c r="M34">
-        <v>4353.64</v>
+        <v>270.34</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2283,22 +2274,22 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35">
-        <v>13.25</v>
+        <v>14.46</v>
       </c>
       <c r="E35">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G35">
-        <v>82.65000000000001</v>
+        <v>100</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2307,16 +2298,16 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K35">
-        <v>3542</v>
+        <v>1299.5</v>
       </c>
       <c r="L35">
-        <v>3429.43</v>
+        <v>1226.68</v>
       </c>
       <c r="M35">
-        <v>3767.14</v>
+        <v>1445.14</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2327,22 +2318,22 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D36">
-        <v>10.84</v>
+        <v>14.46</v>
       </c>
       <c r="E36">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G36">
-        <v>93.48999999999999</v>
+        <v>100</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2351,16 +2342,16 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K36">
-        <v>2791.6</v>
+        <v>397.55</v>
       </c>
       <c r="L36">
-        <v>2651.31</v>
+        <v>378.48</v>
       </c>
       <c r="M36">
-        <v>3072.17</v>
+        <v>435.69</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2371,19 +2362,19 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D37">
-        <v>9.640000000000001</v>
+        <v>14.46</v>
       </c>
       <c r="E37">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G37">
         <v>100</v>
@@ -2395,16 +2386,16 @@
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K37">
-        <v>3606.9</v>
+        <v>3866.9</v>
       </c>
       <c r="L37">
-        <v>3465.92</v>
+        <v>3626.53</v>
       </c>
       <c r="M37">
-        <v>3888.85</v>
+        <v>4347.64</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2415,22 +2406,22 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D38">
-        <v>9.640000000000001</v>
+        <v>14.46</v>
       </c>
       <c r="E38">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="F38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G38">
-        <v>85.23999999999999</v>
+        <v>73.01000000000001</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2439,16 +2430,16 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K38">
-        <v>151100</v>
+        <v>2148.8</v>
       </c>
       <c r="L38">
-        <v>145496.12</v>
+        <v>1984.03</v>
       </c>
       <c r="M38">
-        <v>162307.75</v>
+        <v>2478.34</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2459,40 +2450,40 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D39">
-        <v>8.43</v>
+        <v>10.84</v>
       </c>
       <c r="E39">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G39">
-        <v>100</v>
+        <v>93.48999999999999</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K39">
-        <v>6307</v>
+        <v>2799.1</v>
       </c>
       <c r="L39">
-        <v>5997.6</v>
+        <v>2652.03</v>
       </c>
       <c r="M39">
-        <v>6925.81</v>
+        <v>3093.24</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2503,22 +2494,22 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D40">
-        <v>8.43</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E40">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G40">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -2527,16 +2518,16 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K40">
-        <v>38010</v>
+        <v>150710</v>
       </c>
       <c r="L40">
-        <v>36296.43</v>
+        <v>145458.98</v>
       </c>
       <c r="M40">
-        <v>41437.14</v>
+        <v>161212.04</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2547,22 +2538,22 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D41">
-        <v>7.23</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E41">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G41">
-        <v>100</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2571,16 +2562,16 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K41">
-        <v>528.4</v>
+        <v>3526.1</v>
       </c>
       <c r="L41">
-        <v>505.67</v>
+        <v>3413.46</v>
       </c>
       <c r="M41">
-        <v>573.86</v>
+        <v>3751.39</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2591,19 +2582,19 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D42">
-        <v>4.82</v>
+        <v>8.43</v>
       </c>
       <c r="E42">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G42">
         <v>100</v>
@@ -2615,16 +2606,16 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K42">
-        <v>485.5</v>
+        <v>38015</v>
       </c>
       <c r="L42">
-        <v>469.46</v>
+        <v>36301.43</v>
       </c>
       <c r="M42">
-        <v>517.5700000000001</v>
+        <v>41442.14</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2635,19 +2626,19 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D43">
-        <v>48.19</v>
+        <v>8.43</v>
       </c>
       <c r="E43">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F43" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G43">
         <v>100</v>
@@ -2656,19 +2647,19 @@
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K43">
-        <v>19850</v>
+        <v>6295</v>
       </c>
       <c r="L43">
-        <v>18009.71</v>
+        <v>5996.45</v>
       </c>
       <c r="M43">
-        <v>23530.57</v>
+        <v>6892.09</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2682,37 +2673,37 @@
         <v>102</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D44">
-        <v>45.78</v>
+        <v>7.23</v>
       </c>
       <c r="E44">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F44" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G44">
-        <v>92.11</v>
+        <v>100</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K44">
-        <v>645.6</v>
+        <v>529.4</v>
       </c>
       <c r="L44">
-        <v>590.1</v>
+        <v>506.67</v>
       </c>
       <c r="M44">
-        <v>756.6</v>
+        <v>574.86</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2723,40 +2714,40 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45">
-        <v>43.37</v>
+        <v>4.82</v>
       </c>
       <c r="E45">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G45">
-        <v>65.59999999999999</v>
+        <v>100</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K45">
-        <v>199.28</v>
+        <v>486.65</v>
       </c>
       <c r="L45">
-        <v>189.85</v>
+        <v>469.57</v>
       </c>
       <c r="M45">
-        <v>218.14</v>
+        <v>520.8</v>
       </c>
       <c r="N45">
         <v>2</v>
@@ -2767,40 +2758,40 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46">
-        <v>41.14</v>
+        <v>48.19</v>
       </c>
       <c r="E46">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G46">
-        <v>72.29000000000001</v>
+        <v>100</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K46">
-        <v>2025.6</v>
+        <v>19479</v>
       </c>
       <c r="L46">
-        <v>1863.96</v>
+        <v>17638.71</v>
       </c>
       <c r="M46">
-        <v>2348.89</v>
+        <v>23159.57</v>
       </c>
       <c r="N46">
         <v>2</v>
@@ -2814,37 +2805,37 @@
         <v>99</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D47">
-        <v>40.96</v>
+        <v>45.78</v>
       </c>
       <c r="E47">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G47">
-        <v>92.47</v>
+        <v>92.11</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K47">
-        <v>309.35</v>
+        <v>638.45</v>
       </c>
       <c r="L47">
-        <v>289.26</v>
+        <v>582.95</v>
       </c>
       <c r="M47">
-        <v>349.54</v>
+        <v>749.45</v>
       </c>
       <c r="N47">
         <v>2</v>
@@ -2855,40 +2846,40 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D48">
-        <v>40.96</v>
+        <v>43.37</v>
       </c>
       <c r="E48">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G48">
-        <v>100</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K48">
-        <v>952.55</v>
+        <v>199.2</v>
       </c>
       <c r="L48">
-        <v>907.79</v>
+        <v>189.77</v>
       </c>
       <c r="M48">
-        <v>1042.08</v>
+        <v>218.06</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -2899,40 +2890,40 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D49">
-        <v>40.12</v>
+        <v>41.33</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G49">
-        <v>64.40000000000001</v>
+        <v>41.33</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J49" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K49">
-        <v>13588</v>
+        <v>700.25</v>
       </c>
       <c r="L49">
-        <v>13083.2</v>
+        <v>680.64</v>
       </c>
       <c r="M49">
-        <v>14597.6</v>
+        <v>739.46</v>
       </c>
       <c r="N49">
         <v>2</v>
@@ -2943,22 +2934,22 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50">
+        <v>41.14</v>
+      </c>
+      <c r="E50">
+        <v>27</v>
+      </c>
+      <c r="F50" t="s">
         <v>116</v>
       </c>
-      <c r="D50">
-        <v>55.96</v>
-      </c>
-      <c r="E50">
-        <v>15</v>
-      </c>
-      <c r="F50" t="s">
-        <v>127</v>
-      </c>
       <c r="G50">
-        <v>55.96</v>
+        <v>72.29000000000001</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -2967,16 +2958,16 @@
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K50">
-        <v>988.95</v>
+        <v>2026</v>
       </c>
       <c r="L50">
-        <v>954.8</v>
+        <v>1864.36</v>
       </c>
       <c r="M50">
-        <v>1057.25</v>
+        <v>2349.29</v>
       </c>
       <c r="N50">
         <v>2</v>
@@ -2987,40 +2978,40 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D51">
-        <v>52.17</v>
+        <v>40.96</v>
       </c>
       <c r="E51">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G51">
-        <v>52.17</v>
+        <v>92.47</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J51" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K51">
-        <v>207</v>
+        <v>31840</v>
       </c>
       <c r="L51">
-        <v>196.65</v>
+        <v>30510</v>
       </c>
       <c r="M51">
-        <v>227.71</v>
+        <v>34500</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -3031,40 +3022,40 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D52">
-        <v>37.35</v>
+        <v>40.96</v>
       </c>
       <c r="E52">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F52" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G52">
-        <v>37.35</v>
+        <v>92.47</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J52" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="K52">
-        <v>1084.9</v>
+        <v>311.15</v>
       </c>
       <c r="L52">
-        <v>1025.64</v>
+        <v>291.06</v>
       </c>
       <c r="M52">
-        <v>1203.43</v>
+        <v>351.34</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -3075,40 +3066,40 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
         <v>113</v>
       </c>
       <c r="D53">
-        <v>34.94</v>
+        <v>63.19</v>
       </c>
       <c r="E53">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G53">
-        <v>44.58</v>
+        <v>63.19</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I53">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K53">
-        <v>452.85</v>
+        <v>993.55</v>
       </c>
       <c r="L53">
-        <v>418.24</v>
+        <v>958.62</v>
       </c>
       <c r="M53">
-        <v>522.0599999999999</v>
+        <v>1063.41</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -3119,40 +3110,40 @@
         <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D54">
-        <v>34.94</v>
+        <v>39.76</v>
       </c>
       <c r="E54">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F54" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="G54">
-        <v>54.76</v>
+        <v>39.76</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K54">
-        <v>260.03</v>
+        <v>1093.7</v>
       </c>
       <c r="L54">
-        <v>243.78</v>
+        <v>1032.83</v>
       </c>
       <c r="M54">
-        <v>292.53</v>
+        <v>1215.44</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -3163,22 +3154,22 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D55">
-        <v>32.53</v>
+        <v>36.14</v>
       </c>
       <c r="E55">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F55" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G55">
-        <v>32.53</v>
+        <v>38.55</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3187,16 +3178,16 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K55">
-        <v>1525.5</v>
+        <v>1617.6</v>
       </c>
       <c r="L55">
-        <v>1453.99</v>
+        <v>1534.87</v>
       </c>
       <c r="M55">
-        <v>1668.53</v>
+        <v>1783.06</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -3207,40 +3198,40 @@
         <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D56">
-        <v>27.71</v>
+        <v>34.94</v>
       </c>
       <c r="E56">
+        <v>28</v>
+      </c>
+      <c r="F56" t="s">
+        <v>124</v>
+      </c>
+      <c r="G56">
+        <v>54.76</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
         <v>3</v>
       </c>
-      <c r="F56" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56">
-        <v>27.71</v>
-      </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="I56">
-        <v>1</v>
-      </c>
       <c r="J56" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K56">
-        <v>699.6</v>
+        <v>262.15</v>
       </c>
       <c r="L56">
-        <v>680.58</v>
+        <v>245.9</v>
       </c>
       <c r="M56">
-        <v>737.64</v>
+        <v>294.65</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -3251,40 +3242,40 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D57">
-        <v>27.71</v>
+        <v>34.94</v>
       </c>
       <c r="E57">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F57" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G57">
-        <v>27.71</v>
+        <v>44.58</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J57" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K57">
-        <v>834.9</v>
+        <v>453.35</v>
       </c>
       <c r="L57">
-        <v>792.54</v>
+        <v>418.74</v>
       </c>
       <c r="M57">
-        <v>919.61</v>
+        <v>522.5599999999999</v>
       </c>
       <c r="N57">
         <v>2</v>
@@ -3295,40 +3286,40 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D58">
-        <v>24.1</v>
+        <v>32.53</v>
       </c>
       <c r="E58">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G58">
-        <v>61.63</v>
+        <v>32.53</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K58">
-        <v>154.55</v>
+        <v>1525</v>
       </c>
       <c r="L58">
-        <v>143.42</v>
+        <v>1453.49</v>
       </c>
       <c r="M58">
-        <v>176.81</v>
+        <v>1668.03</v>
       </c>
       <c r="N58">
         <v>2</v>
@@ -3339,40 +3330,40 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D59">
-        <v>22.89</v>
+        <v>29.28</v>
       </c>
       <c r="E59">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G59">
-        <v>22.89</v>
+        <v>38.92</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J59" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K59">
-        <v>166.1</v>
+        <v>210.11</v>
       </c>
       <c r="L59">
-        <v>158.91</v>
+        <v>207.1</v>
       </c>
       <c r="M59">
-        <v>180.48</v>
+        <v>216.13</v>
       </c>
       <c r="N59">
         <v>2</v>
@@ -3383,40 +3374,40 @@
         <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D60">
-        <v>22.89</v>
+        <v>27.89</v>
       </c>
       <c r="E60">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F60" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G60">
-        <v>52.35</v>
+        <v>27.89</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I60">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K60">
-        <v>369.05</v>
+        <v>698.9</v>
       </c>
       <c r="L60">
-        <v>350.04</v>
+        <v>675.42</v>
       </c>
       <c r="M60">
-        <v>407.07</v>
+        <v>745.86</v>
       </c>
       <c r="N60">
         <v>2</v>
@@ -3427,40 +3418,40 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D61">
-        <v>21.69</v>
+        <v>27.71</v>
       </c>
       <c r="E61">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="F61" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G61">
-        <v>66.81</v>
+        <v>27.71</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K61">
-        <v>5145</v>
+        <v>188.92</v>
       </c>
       <c r="L61">
-        <v>4861.07</v>
+        <v>177.86</v>
       </c>
       <c r="M61">
-        <v>5712.86</v>
+        <v>211.04</v>
       </c>
       <c r="N61">
         <v>2</v>
@@ -3471,40 +3462,40 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D62">
-        <v>21.69</v>
+        <v>22.89</v>
       </c>
       <c r="E62">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F62" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G62">
-        <v>63.37</v>
+        <v>52.35</v>
       </c>
       <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
         <v>3</v>
       </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
       <c r="J62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K62">
-        <v>1481.8</v>
+        <v>368.4</v>
       </c>
       <c r="L62">
-        <v>1449.01</v>
+        <v>349.98</v>
       </c>
       <c r="M62">
-        <v>1547.37</v>
+        <v>405.25</v>
       </c>
       <c r="N62">
         <v>2</v>
@@ -3515,40 +3506,40 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C63" t="s">
+        <v>112</v>
+      </c>
+      <c r="D63">
+        <v>22.89</v>
+      </c>
+      <c r="E63">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
         <v>115</v>
       </c>
-      <c r="D63">
-        <v>20.48</v>
-      </c>
-      <c r="E63">
-        <v>30</v>
-      </c>
-      <c r="F63" t="s">
-        <v>119</v>
-      </c>
       <c r="G63">
-        <v>43.37</v>
+        <v>22.89</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="I63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J63" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K63">
-        <v>1454.1</v>
+        <v>165.78</v>
       </c>
       <c r="L63">
-        <v>1378.74</v>
+        <v>158.59</v>
       </c>
       <c r="M63">
-        <v>1604.83</v>
+        <v>180.16</v>
       </c>
       <c r="N63">
         <v>2</v>
@@ -3559,40 +3550,40 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
         <v>111</v>
       </c>
       <c r="D64">
-        <v>19.28</v>
+        <v>21.69</v>
       </c>
       <c r="E64">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F64" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G64">
-        <v>28.92</v>
+        <v>63.37</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K64">
-        <v>464.5</v>
+        <v>1485.4</v>
       </c>
       <c r="L64">
-        <v>452.86</v>
+        <v>1452.57</v>
       </c>
       <c r="M64">
-        <v>487.78</v>
+        <v>1551.06</v>
       </c>
       <c r="N64">
         <v>2</v>
@@ -3603,40 +3594,40 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D65">
-        <v>19.28</v>
+        <v>21.69</v>
       </c>
       <c r="E65">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="F65" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G65">
-        <v>26.69</v>
+        <v>43.37</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K65">
-        <v>2011.2</v>
+        <v>2739.8</v>
       </c>
       <c r="L65">
-        <v>1979.19</v>
+        <v>2641.77</v>
       </c>
       <c r="M65">
-        <v>2075.23</v>
+        <v>2935.86</v>
       </c>
       <c r="N65">
         <v>2</v>
@@ -3647,22 +3638,22 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D66">
-        <v>18.07</v>
+        <v>20.48</v>
       </c>
       <c r="E66">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G66">
-        <v>28.07</v>
+        <v>43.37</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3671,16 +3662,16 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K66">
-        <v>1014.9</v>
+        <v>1453.8</v>
       </c>
       <c r="L66">
-        <v>978.89</v>
+        <v>1378.71</v>
       </c>
       <c r="M66">
-        <v>1086.91</v>
+        <v>1603.98</v>
       </c>
       <c r="N66">
         <v>2</v>
@@ -3691,40 +3682,40 @@
         <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D67">
-        <v>16.87</v>
+        <v>20.48</v>
       </c>
       <c r="E67">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G67">
-        <v>38.55</v>
+        <v>66.81</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K67">
-        <v>1611.1</v>
+        <v>5129.5</v>
       </c>
       <c r="L67">
-        <v>1528.37</v>
+        <v>4859.59</v>
       </c>
       <c r="M67">
-        <v>1776.56</v>
+        <v>5669.32</v>
       </c>
       <c r="N67">
         <v>2</v>
@@ -3735,40 +3726,40 @@
         <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C68" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D68">
-        <v>16.87</v>
+        <v>19.28</v>
       </c>
       <c r="E68">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G68">
-        <v>22.89</v>
+        <v>26.69</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K68">
-        <v>3544</v>
+        <v>2012</v>
       </c>
       <c r="L68">
-        <v>3389.84</v>
+        <v>1979.25</v>
       </c>
       <c r="M68">
-        <v>3852.31</v>
+        <v>2077.51</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -3779,22 +3770,22 @@
         <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D69">
-        <v>15.66</v>
+        <v>18.07</v>
       </c>
       <c r="E69">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="F69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G69">
-        <v>43.37</v>
+        <v>58.19</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3803,16 +3794,16 @@
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K69">
-        <v>2729.8</v>
+        <v>3096</v>
       </c>
       <c r="L69">
-        <v>2631.77</v>
+        <v>2940.19</v>
       </c>
       <c r="M69">
-        <v>2925.86</v>
+        <v>3407.63</v>
       </c>
       <c r="N69">
         <v>2</v>
@@ -3823,22 +3814,22 @@
         <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D70">
-        <v>14.46</v>
+        <v>18.07</v>
       </c>
       <c r="E70">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F70" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G70">
-        <v>37.35</v>
+        <v>28.07</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3847,16 +3838,16 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K70">
-        <v>175.85</v>
+        <v>1010.3</v>
       </c>
       <c r="L70">
-        <v>163.91</v>
+        <v>978.39</v>
       </c>
       <c r="M70">
-        <v>199.72</v>
+        <v>1074.11</v>
       </c>
       <c r="N70">
         <v>2</v>
@@ -3867,40 +3858,40 @@
         <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D71">
         <v>14.46</v>
       </c>
       <c r="E71">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F71" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G71">
-        <v>27.89</v>
+        <v>37.35</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K71">
-        <v>695.8</v>
+        <v>176.32</v>
       </c>
       <c r="L71">
-        <v>674.04</v>
+        <v>164.38</v>
       </c>
       <c r="M71">
-        <v>739.33</v>
+        <v>200.19</v>
       </c>
       <c r="N71">
         <v>2</v>
@@ -3911,40 +3902,40 @@
         <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C72" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D72">
-        <v>13.25</v>
+        <v>14.46</v>
       </c>
       <c r="E72">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="F72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G72">
-        <v>22.89</v>
+        <v>31.33</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K72">
-        <v>187.85</v>
+        <v>7427</v>
       </c>
       <c r="L72">
-        <v>176.79</v>
+        <v>7253.89</v>
       </c>
       <c r="M72">
-        <v>209.97</v>
+        <v>7773.22</v>
       </c>
       <c r="N72">
         <v>2</v>
@@ -3955,40 +3946,40 @@
         <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D73">
-        <v>12.05</v>
+        <v>13.25</v>
       </c>
       <c r="E73">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F73" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G73">
-        <v>58.19</v>
+        <v>28.92</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73">
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K73">
-        <v>3072</v>
+        <v>460.55</v>
       </c>
       <c r="L73">
-        <v>2918.29</v>
+        <v>452.47</v>
       </c>
       <c r="M73">
-        <v>3379.43</v>
+        <v>476.71</v>
       </c>
       <c r="N73">
         <v>2</v>
@@ -3999,19 +3990,19 @@
         <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C74" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D74">
         <v>12.05</v>
       </c>
       <c r="E74">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F74" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G74">
         <v>65.06</v>
@@ -4023,16 +4014,16 @@
         <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K74">
-        <v>826.15</v>
+        <v>827.1</v>
       </c>
       <c r="L74">
-        <v>793.6</v>
+        <v>794.55</v>
       </c>
       <c r="M74">
-        <v>891.25</v>
+        <v>892.2</v>
       </c>
       <c r="N74">
         <v>2</v>
@@ -4043,40 +4034,40 @@
         <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C75" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D75">
-        <v>10.84</v>
+        <v>12.05</v>
       </c>
       <c r="E75">
         <v>24</v>
       </c>
       <c r="F75" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G75">
-        <v>15.66</v>
+        <v>22.89</v>
       </c>
       <c r="H75">
         <v>0</v>
       </c>
       <c r="I75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K75">
-        <v>3251.1</v>
+        <v>3535</v>
       </c>
       <c r="L75">
-        <v>3151.19</v>
+        <v>3380.84</v>
       </c>
       <c r="M75">
-        <v>3450.91</v>
+        <v>3843.31</v>
       </c>
       <c r="N75">
         <v>2</v>
@@ -4087,40 +4078,40 @@
         <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C76" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D76">
         <v>10.84</v>
       </c>
       <c r="E76">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F76" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G76">
-        <v>22.89</v>
+        <v>15.66</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
       <c r="I76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J76" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K76">
-        <v>6584.5</v>
+        <v>3264.6</v>
       </c>
       <c r="L76">
-        <v>6276.09</v>
+        <v>3152.4</v>
       </c>
       <c r="M76">
-        <v>7201.31</v>
+        <v>3489</v>
       </c>
       <c r="N76">
         <v>2</v>
@@ -4131,10 +4122,10 @@
         <v>89</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D77">
         <v>10.84</v>
@@ -4143,10 +4134,10 @@
         <v>31</v>
       </c>
       <c r="F77" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G77">
-        <v>18.07</v>
+        <v>22.89</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -4155,16 +4146,16 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K77">
-        <v>405.05</v>
+        <v>6619.5</v>
       </c>
       <c r="L77">
-        <v>391.86</v>
+        <v>6301</v>
       </c>
       <c r="M77">
-        <v>431.43</v>
+        <v>7256.5</v>
       </c>
       <c r="N77">
         <v>2</v>
@@ -4175,40 +4166,40 @@
         <v>90</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D78">
         <v>9.640000000000001</v>
       </c>
       <c r="E78">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G78">
-        <v>21.69</v>
+        <v>20.48</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78">
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K78">
-        <v>4991.4</v>
+        <v>6899.5</v>
       </c>
       <c r="L78">
-        <v>4884.35</v>
+        <v>6675.62</v>
       </c>
       <c r="M78">
-        <v>5205.5</v>
+        <v>7347.27</v>
       </c>
       <c r="N78">
         <v>2</v>
@@ -4219,40 +4210,40 @@
         <v>91</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D79">
-        <v>8.43</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E79">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F79" t="s">
         <v>119</v>
       </c>
       <c r="G79">
-        <v>31.33</v>
+        <v>21.69</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79">
         <v>0</v>
       </c>
       <c r="J79" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K79">
-        <v>7423</v>
+        <v>5002.9</v>
       </c>
       <c r="L79">
-        <v>7253.51</v>
+        <v>4885.44</v>
       </c>
       <c r="M79">
-        <v>7761.98</v>
+        <v>5237.81</v>
       </c>
       <c r="N79">
         <v>2</v>
@@ -4263,40 +4254,40 @@
         <v>92</v>
       </c>
       <c r="B80" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D80">
-        <v>8.43</v>
+        <v>7.23</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F80" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G80">
-        <v>9.640000000000001</v>
+        <v>30.12</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80">
         <v>0</v>
       </c>
       <c r="J80" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K80">
-        <v>84.06999999999999</v>
+        <v>604.4</v>
       </c>
       <c r="L80">
-        <v>81.31999999999999</v>
+        <v>575.36</v>
       </c>
       <c r="M80">
-        <v>89.58</v>
+        <v>662.48</v>
       </c>
       <c r="N80">
         <v>2</v>
@@ -4307,10 +4298,10 @@
         <v>93</v>
       </c>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D81">
         <v>7.23</v>
@@ -4319,28 +4310,28 @@
         <v>25</v>
       </c>
       <c r="F81" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G81">
-        <v>30.12</v>
+        <v>48.73</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81">
         <v>0</v>
       </c>
       <c r="J81" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K81">
-        <v>604.95</v>
+        <v>31865</v>
       </c>
       <c r="L81">
-        <v>575.41</v>
+        <v>30895.2</v>
       </c>
       <c r="M81">
-        <v>664.02</v>
+        <v>33804.61</v>
       </c>
       <c r="N81">
         <v>2</v>
@@ -4351,40 +4342,40 @@
         <v>94</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D82">
-        <v>7.23</v>
+        <v>6.02</v>
       </c>
       <c r="E82">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F82" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G82">
-        <v>48.73</v>
+        <v>57.83</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82">
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K82">
-        <v>31855</v>
+        <v>855.55</v>
       </c>
       <c r="L82">
-        <v>30895.32</v>
+        <v>811.09</v>
       </c>
       <c r="M82">
-        <v>33774.37</v>
+        <v>944.47</v>
       </c>
       <c r="N82">
         <v>2</v>
@@ -4395,19 +4386,19 @@
         <v>95</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D83">
         <v>4.82</v>
       </c>
       <c r="E83">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F83" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G83">
         <v>41.14</v>
@@ -4419,150 +4410,18 @@
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K83">
-        <v>460.6</v>
+        <v>460.4</v>
       </c>
       <c r="L83">
-        <v>448.26</v>
+        <v>448.24</v>
       </c>
       <c r="M83">
-        <v>485.29</v>
+        <v>484.73</v>
       </c>
       <c r="N83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
-      <c r="A84" t="s">
-        <v>96</v>
-      </c>
-      <c r="B84" t="s">
-        <v>108</v>
-      </c>
-      <c r="C84" t="s">
-        <v>115</v>
-      </c>
-      <c r="D84">
-        <v>4.82</v>
-      </c>
-      <c r="E84">
-        <v>7</v>
-      </c>
-      <c r="F84" t="s">
-        <v>121</v>
-      </c>
-      <c r="G84">
-        <v>6.02</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84">
-        <v>0</v>
-      </c>
-      <c r="J84" t="s">
-        <v>134</v>
-      </c>
-      <c r="K84">
-        <v>228.19</v>
-      </c>
-      <c r="L84">
-        <v>218.96</v>
-      </c>
-      <c r="M84">
-        <v>246.65</v>
-      </c>
-      <c r="N84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
-      <c r="A85" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" t="s">
-        <v>106</v>
-      </c>
-      <c r="C85" t="s">
-        <v>115</v>
-      </c>
-      <c r="D85">
-        <v>4.82</v>
-      </c>
-      <c r="E85">
-        <v>15</v>
-      </c>
-      <c r="F85" t="s">
-        <v>127</v>
-      </c>
-      <c r="G85">
-        <v>10.84</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
-        <v>0</v>
-      </c>
-      <c r="J85" t="s">
-        <v>134</v>
-      </c>
-      <c r="K85">
-        <v>1689.4</v>
-      </c>
-      <c r="L85">
-        <v>1658.33</v>
-      </c>
-      <c r="M85">
-        <v>1751.54</v>
-      </c>
-      <c r="N85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
-      <c r="A86" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" t="s">
-        <v>103</v>
-      </c>
-      <c r="C86" t="s">
-        <v>115</v>
-      </c>
-      <c r="D86">
-        <v>4.82</v>
-      </c>
-      <c r="E86">
-        <v>10</v>
-      </c>
-      <c r="F86" t="s">
-        <v>123</v>
-      </c>
-      <c r="G86">
-        <v>20.48</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86">
-        <v>0</v>
-      </c>
-      <c r="J86" t="s">
-        <v>134</v>
-      </c>
-      <c r="K86">
-        <v>6892</v>
-      </c>
-      <c r="L86">
-        <v>6674.9</v>
-      </c>
-      <c r="M86">
-        <v>7326.19</v>
-      </c>
-      <c r="N86">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add enhanced market score with breadth integration
- Created EnhancedMarketScoreCalculator that combines reversal counts with market breadth
- Market score now weighted: 60% reversal signals, 40% breadth (configurable)
- Added weekly bias calculation for strategic direction alignment
- Enhanced dashboard to display breadth score and weekly trading bias
- Created market_score_config.json for tunable parameters
- Integrated enhanced score into market_regime_analyzer.py
- Dashboard now shows primary direction, strength, and allocation percentage
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="84">
   <si>
     <t>Ticker</t>
   </si>
@@ -61,210 +61,153 @@
     <t>PAYTM</t>
   </si>
   <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>UPL</t>
+  </si>
+  <si>
+    <t>NUVOCO</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>BORORENEW</t>
+  </si>
+  <si>
+    <t>SHK</t>
+  </si>
+  <si>
+    <t>SYRMA</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>AMBUJACEM</t>
+  </si>
+  <si>
     <t>IPCALAB</t>
   </si>
   <si>
+    <t>JINDALSTEL</t>
+  </si>
+  <si>
+    <t>3MINDIA</t>
+  </si>
+  <si>
+    <t>GLAND</t>
+  </si>
+  <si>
+    <t>KIMS</t>
+  </si>
+  <si>
+    <t>PATANJALI</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>ANANDRATHI</t>
+  </si>
+  <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>NMDC</t>
+  </si>
+  <si>
+    <t>MEDANTA</t>
+  </si>
+  <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>OLECTRA</t>
+  </si>
+  <si>
+    <t>SUPREMEIND</t>
+  </si>
+  <si>
     <t>ETERNAL</t>
   </si>
   <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>NUVOCO</t>
-  </si>
-  <si>
-    <t>UPL</t>
-  </si>
-  <si>
-    <t>BORORENEW</t>
-  </si>
-  <si>
-    <t>AGI</t>
-  </si>
-  <si>
-    <t>SHK</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>AMBUJACEM</t>
-  </si>
-  <si>
-    <t>METROPOLIS</t>
-  </si>
-  <si>
-    <t>BIKAJI</t>
-  </si>
-  <si>
-    <t>DELHIVERY</t>
-  </si>
-  <si>
-    <t>ASHAPURMIN</t>
-  </si>
-  <si>
-    <t>KIMS</t>
-  </si>
-  <si>
-    <t>GLAND</t>
-  </si>
-  <si>
-    <t>JINDALSTEL</t>
-  </si>
-  <si>
-    <t>GREENPLY</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
-    <t>PATANJALI</t>
-  </si>
-  <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>TORNTPHARM</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
-  </si>
-  <si>
-    <t>GLENMARK</t>
-  </si>
-  <si>
-    <t>NAVA</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
-    <t>MEDANTA</t>
-  </si>
-  <si>
-    <t>NMDC</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
-  </si>
-  <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>OLECTRA</t>
+    <t>HOMEFIRST</t>
   </si>
   <si>
     <t>TRIDENT</t>
   </si>
   <si>
+    <t>DIXON</t>
+  </si>
+  <si>
+    <t>LXCHEM</t>
+  </si>
+  <si>
+    <t>HINDALCO</t>
+  </si>
+  <si>
+    <t>ZYDUSLIFE</t>
+  </si>
+  <si>
     <t>LAURUSLABS</t>
   </si>
   <si>
-    <t>DIXON</t>
-  </si>
-  <si>
-    <t>METROBRAND</t>
-  </si>
-  <si>
-    <t>PTC</t>
-  </si>
-  <si>
-    <t>LXCHEM</t>
-  </si>
-  <si>
-    <t>VIJAYA</t>
-  </si>
-  <si>
-    <t>ECLERX</t>
-  </si>
-  <si>
-    <t>ICICIBANK</t>
-  </si>
-  <si>
-    <t>SURYAROSNI</t>
-  </si>
-  <si>
-    <t>PENIND</t>
-  </si>
-  <si>
-    <t>SUPREMEIND</t>
-  </si>
-  <si>
-    <t>HDFCBANK</t>
-  </si>
-  <si>
-    <t>HOMEFIRST</t>
-  </si>
-  <si>
-    <t>GMDCLTD</t>
-  </si>
-  <si>
     <t>LALPATHLAB</t>
   </si>
   <si>
-    <t>HINDALCO</t>
-  </si>
-  <si>
-    <t>RAINBOW</t>
-  </si>
-  <si>
-    <t>CGCL</t>
+    <t>JBCHEPHARM</t>
   </si>
   <si>
     <t>ALKEM</t>
   </si>
   <si>
+    <t>TFCILTD</t>
+  </si>
+  <si>
     <t>EIDPARRY</t>
   </si>
   <si>
-    <t>JBCHEPHARM</t>
+    <t>APOLLOHOSP</t>
   </si>
   <si>
     <t>TMB</t>
   </si>
   <si>
-    <t>APOLLOHOSP</t>
-  </si>
-  <si>
-    <t>JKCEMENT</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
+    <t>Consumer Cyclical</t>
+  </si>
+  <si>
     <t>Healthcare</t>
   </si>
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Consumer Cyclical</t>
-  </si>
-  <si>
     <t>Basic Materials</t>
   </si>
   <si>
-    <t>Consumer Defensive</t>
-  </si>
-  <si>
     <t>Industrials</t>
   </si>
   <si>
     <t>Financial Services</t>
   </si>
   <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>G_Pattern</t>
   </si>
   <si>
@@ -280,46 +223,34 @@
     <t>Power_H2_Volume</t>
   </si>
   <si>
-    <t>KC_Multi_H2</t>
-  </si>
-  <si>
     <t>2025-07-11</t>
   </si>
   <si>
+    <t>2025-07-16</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
     <t>2025-07-08</t>
   </si>
   <si>
+    <t>2025-07-21</t>
+  </si>
+  <si>
+    <t>2025-07-18</t>
+  </si>
+  <si>
+    <t>2025-07-25</t>
+  </si>
+  <si>
     <t>2025-07-22</t>
   </si>
   <si>
-    <t>2025-07-16</t>
-  </si>
-  <si>
-    <t>2025-07-07</t>
-  </si>
-  <si>
-    <t>2025-07-15</t>
-  </si>
-  <si>
-    <t>2025-07-21</t>
-  </si>
-  <si>
-    <t>2025-07-18</t>
-  </si>
-  <si>
     <t>2025-07-09</t>
-  </si>
-  <si>
-    <t>2025-07-17</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
-  </si>
-  <si>
-    <t>2025-07-25</t>
-  </si>
-  <si>
-    <t>2025-07-10</t>
   </si>
   <si>
     <t>G PATTERN CONFIRMED - FULL POSITION (100%)</t>
@@ -692,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -747,19 +678,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>63.86</v>
+        <v>59.04</v>
       </c>
       <c r="E2">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -771,16 +702,16 @@
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="K2">
-        <v>1094.05</v>
+        <v>1067</v>
       </c>
       <c r="L2">
-        <v>1023.69</v>
+        <v>992.6900000000001</v>
       </c>
       <c r="M2">
-        <v>1234.78</v>
+        <v>1215.61</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -791,40 +722,40 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D3">
-        <v>70.78</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G3">
-        <v>70.78</v>
+        <v>100</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="K3">
-        <v>1552.6</v>
+        <v>965.95</v>
       </c>
       <c r="L3">
-        <v>1478.13</v>
+        <v>920.09</v>
       </c>
       <c r="M3">
-        <v>1701.54</v>
+        <v>1057.66</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -835,22 +766,22 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D4">
-        <v>39.76</v>
+        <v>37.35</v>
       </c>
       <c r="E4">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="G4">
-        <v>92.47</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -859,16 +790,16 @@
         <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K4">
-        <v>309.6</v>
+        <v>496.2</v>
       </c>
       <c r="L4">
-        <v>289.51</v>
+        <v>445.93</v>
       </c>
       <c r="M4">
-        <v>349.77</v>
+        <v>596.74</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -879,40 +810,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D5">
-        <v>39.76</v>
+        <v>34.94</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K5">
-        <v>962.85</v>
+        <v>722.7</v>
       </c>
       <c r="L5">
-        <v>916.99</v>
+        <v>690.74</v>
       </c>
       <c r="M5">
-        <v>1054.56</v>
+        <v>786.61</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -923,40 +854,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D6">
-        <v>37.35</v>
+        <v>34.94</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K6">
-        <v>503.6</v>
+        <v>413.45</v>
       </c>
       <c r="L6">
-        <v>453.56</v>
+        <v>386.28</v>
       </c>
       <c r="M6">
-        <v>603.6900000000001</v>
+        <v>467.79</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -967,40 +898,40 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D7">
-        <v>37.35</v>
+        <v>33.73</v>
       </c>
       <c r="E7">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="G7">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K7">
-        <v>416</v>
+        <v>937</v>
       </c>
       <c r="L7">
-        <v>388.83</v>
+        <v>853.14</v>
       </c>
       <c r="M7">
-        <v>470.34</v>
+        <v>1104.71</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1011,22 +942,22 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>34.94</v>
+        <v>33.73</v>
       </c>
       <c r="E8">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G8">
-        <v>85.23999999999999</v>
+        <v>82.83</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1035,16 +966,16 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K8">
-        <v>725</v>
+        <v>847.8</v>
       </c>
       <c r="L8">
-        <v>693.39</v>
+        <v>805.29</v>
       </c>
       <c r="M8">
-        <v>788.21</v>
+        <v>932.8099999999999</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1055,19 +986,19 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D9">
-        <v>34.94</v>
+        <v>31.33</v>
       </c>
       <c r="E9">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="G9">
         <v>92.11</v>
@@ -1079,16 +1010,16 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K9">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="L9">
-        <v>583.8099999999999</v>
+        <v>567.5</v>
       </c>
       <c r="M9">
-        <v>749.37</v>
+        <v>740</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1099,40 +1030,40 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D10">
-        <v>33.73</v>
+        <v>30.12</v>
       </c>
       <c r="E10">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G10">
         <v>100</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K10">
-        <v>953.7</v>
+        <v>262</v>
       </c>
       <c r="L10">
-        <v>869.99</v>
+        <v>247.62</v>
       </c>
       <c r="M10">
-        <v>1121.13</v>
+        <v>290.76</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1143,40 +1074,40 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D11">
-        <v>31.33</v>
+        <v>30.12</v>
       </c>
       <c r="E11">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G11">
         <v>100</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K11">
-        <v>265.73</v>
+        <v>731.1</v>
       </c>
       <c r="L11">
-        <v>252.1</v>
+        <v>669.03</v>
       </c>
       <c r="M11">
-        <v>293</v>
+        <v>855.24</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1187,40 +1118,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D12">
-        <v>28.92</v>
+        <v>27.71</v>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="G12">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K12">
-        <v>841.05</v>
+        <v>682</v>
       </c>
       <c r="L12">
-        <v>799.48</v>
+        <v>649.25</v>
       </c>
       <c r="M12">
-        <v>924.1900000000001</v>
+        <v>747.5</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1231,19 +1162,19 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D13">
         <v>27.71</v>
       </c>
       <c r="E13">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G13">
         <v>100</v>
@@ -1255,16 +1186,16 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K13">
-        <v>614.3</v>
+        <v>613.95</v>
       </c>
       <c r="L13">
-        <v>594.64</v>
+        <v>593.6900000000001</v>
       </c>
       <c r="M13">
-        <v>653.61</v>
+        <v>654.46</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1275,40 +1206,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>26.51</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14">
-        <v>27.71</v>
-      </c>
-      <c r="E14">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>93</v>
-      </c>
       <c r="G14">
-        <v>72.29000000000001</v>
+        <v>70.78</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K14">
-        <v>2027.2</v>
+        <v>1519.7</v>
       </c>
       <c r="L14">
-        <v>1874.34</v>
+        <v>1438.6</v>
       </c>
       <c r="M14">
-        <v>2332.91</v>
+        <v>1681.9</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1319,19 +1250,19 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D15">
-        <v>25.3</v>
+        <v>24.1</v>
       </c>
       <c r="E15">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -1340,19 +1271,19 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K15">
-        <v>781.2</v>
+        <v>1001.2</v>
       </c>
       <c r="L15">
-        <v>741.5599999999999</v>
+        <v>966.01</v>
       </c>
       <c r="M15">
-        <v>860.48</v>
+        <v>1071.59</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1363,40 +1294,40 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D16">
-        <v>24.1</v>
+        <v>22.89</v>
       </c>
       <c r="E16">
         <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J16" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K16">
-        <v>438.65</v>
+        <v>31050</v>
       </c>
       <c r="L16">
-        <v>416.59</v>
+        <v>29766.56</v>
       </c>
       <c r="M16">
-        <v>482.78</v>
+        <v>33616.87</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1407,22 +1338,22 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D17">
-        <v>24.1</v>
+        <v>22.89</v>
       </c>
       <c r="E17">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1431,16 +1362,16 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K17">
-        <v>561</v>
+        <v>2023.7</v>
       </c>
       <c r="L17">
-        <v>509.11</v>
+        <v>1901.39</v>
       </c>
       <c r="M17">
-        <v>664.79</v>
+        <v>2268.33</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1451,19 +1382,19 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>22.89</v>
       </c>
       <c r="E18">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="G18">
         <v>87.65000000000001</v>
@@ -1475,16 +1406,16 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K18">
-        <v>764.6</v>
+        <v>761.45</v>
       </c>
       <c r="L18">
-        <v>721.64</v>
+        <v>717.76</v>
       </c>
       <c r="M18">
-        <v>850.51</v>
+        <v>848.8200000000001</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1495,22 +1426,22 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D19">
-        <v>22.89</v>
+        <v>21.69</v>
       </c>
       <c r="E19">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="G19">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1519,16 +1450,16 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K19">
-        <v>2017</v>
+        <v>1885</v>
       </c>
       <c r="L19">
-        <v>1898.23</v>
+        <v>1783.86</v>
       </c>
       <c r="M19">
-        <v>2254.54</v>
+        <v>2087.29</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1539,40 +1470,40 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="D20">
-        <v>22.89</v>
+        <v>16.87</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G20">
-        <v>100</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K20">
-        <v>1000</v>
+        <v>3605.5</v>
       </c>
       <c r="L20">
-        <v>965.88</v>
+        <v>3478.97</v>
       </c>
       <c r="M20">
-        <v>1068.24</v>
+        <v>3858.56</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1583,40 +1514,40 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D21">
-        <v>21.69</v>
+        <v>14.46</v>
       </c>
       <c r="E21">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="G21">
-        <v>76.81</v>
+        <v>96.08</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K21">
-        <v>338.1</v>
+        <v>2600.9</v>
       </c>
       <c r="L21">
-        <v>318.92</v>
+        <v>2392.57</v>
       </c>
       <c r="M21">
-        <v>376.45</v>
+        <v>3017.56</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1627,19 +1558,19 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D22">
-        <v>21.69</v>
+        <v>14.46</v>
       </c>
       <c r="E22">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F22" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G22">
         <v>100</v>
@@ -1648,19 +1579,19 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K22">
-        <v>680.85</v>
+        <v>394.15</v>
       </c>
       <c r="L22">
-        <v>649.4299999999999</v>
+        <v>377.56</v>
       </c>
       <c r="M22">
-        <v>743.6900000000001</v>
+        <v>427.33</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1671,19 +1602,19 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>13.25</v>
+      </c>
+      <c r="E23">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
         <v>73</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23">
-        <v>20.48</v>
-      </c>
-      <c r="E23">
-        <v>51</v>
-      </c>
-      <c r="F23" t="s">
-        <v>94</v>
       </c>
       <c r="G23">
         <v>100</v>
@@ -1692,19 +1623,19 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K23">
-        <v>1888.5</v>
+        <v>5556.5</v>
       </c>
       <c r="L23">
-        <v>1788.79</v>
+        <v>5325.93</v>
       </c>
       <c r="M23">
-        <v>2087.93</v>
+        <v>6017.64</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1715,40 +1646,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D24">
-        <v>18.07</v>
+        <v>8.43</v>
       </c>
       <c r="E24">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="G24">
-        <v>96.08</v>
+        <v>100</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K24">
-        <v>2634.1</v>
+        <v>37835</v>
       </c>
       <c r="L24">
-        <v>2428.4</v>
+        <v>36175.71</v>
       </c>
       <c r="M24">
-        <v>3045.5</v>
+        <v>41153.57</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1759,40 +1690,40 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D25">
-        <v>15.66</v>
+        <v>7.23</v>
       </c>
       <c r="E25">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="G25">
-        <v>82.65000000000001</v>
+        <v>81.27</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K25">
-        <v>3567.2</v>
+        <v>71.8</v>
       </c>
       <c r="L25">
-        <v>3444.37</v>
+        <v>69.73999999999999</v>
       </c>
       <c r="M25">
-        <v>3812.86</v>
+        <v>75.91</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1803,40 +1734,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26">
+        <v>7.23</v>
+      </c>
+      <c r="E26">
+        <v>49</v>
+      </c>
+      <c r="F26" t="s">
         <v>73</v>
-      </c>
-      <c r="C26" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26">
-        <v>14.46</v>
-      </c>
-      <c r="E26">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
       </c>
       <c r="G26">
         <v>100</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K26">
-        <v>720</v>
+        <v>1322.9</v>
       </c>
       <c r="L26">
-        <v>658.15</v>
+        <v>1260.29</v>
       </c>
       <c r="M26">
-        <v>843.7</v>
+        <v>1448.11</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1847,40 +1778,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D27">
-        <v>13.25</v>
+        <v>46.14</v>
       </c>
       <c r="E27">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="G27">
-        <v>73.01000000000001</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="K27">
-        <v>2154.8</v>
+        <v>1531.7</v>
       </c>
       <c r="L27">
-        <v>1994.41</v>
+        <v>1481.77</v>
       </c>
       <c r="M27">
-        <v>2475.58</v>
+        <v>1631.56</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1891,40 +1822,40 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D28">
-        <v>10.84</v>
+        <v>45.78</v>
       </c>
       <c r="E28">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F28" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="G28">
-        <v>75.42</v>
+        <v>90.06</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J28" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="K28">
-        <v>627.25</v>
+        <v>1472.3</v>
       </c>
       <c r="L28">
-        <v>595.6799999999999</v>
+        <v>1356.2</v>
       </c>
       <c r="M28">
-        <v>690.39</v>
+        <v>1704.5</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1935,40 +1866,40 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>41.33</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29" t="s">
         <v>76</v>
       </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29">
-        <v>8.43</v>
-      </c>
-      <c r="E29">
-        <v>60</v>
-      </c>
-      <c r="F29" t="s">
-        <v>93</v>
-      </c>
       <c r="G29">
-        <v>100</v>
+        <v>41.33</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="K29">
-        <v>37760</v>
+        <v>4289</v>
       </c>
       <c r="L29">
-        <v>36143.26</v>
+        <v>4169.74</v>
       </c>
       <c r="M29">
-        <v>40993.48</v>
+        <v>4527.51</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -1979,40 +1910,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D30">
-        <v>8.43</v>
+        <v>40.96</v>
       </c>
       <c r="E30">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="G30">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J30" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="K30">
-        <v>397.1</v>
+        <v>310.6</v>
       </c>
       <c r="L30">
-        <v>378.86</v>
+        <v>290.08</v>
       </c>
       <c r="M30">
-        <v>433.59</v>
+        <v>351.64</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -2023,40 +1954,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D31">
-        <v>7.23</v>
+        <v>52.17</v>
       </c>
       <c r="E31">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>52.17</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="K31">
-        <v>1328.5</v>
+        <v>1480.5</v>
       </c>
       <c r="L31">
-        <v>1261.07</v>
+        <v>1375.17</v>
       </c>
       <c r="M31">
-        <v>1463.37</v>
+        <v>1691.16</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2067,40 +1998,40 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="D32">
-        <v>7.23</v>
+        <v>38.92</v>
       </c>
       <c r="E32">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="G32">
-        <v>81.27</v>
+        <v>52.17</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="K32">
-        <v>71.93000000000001</v>
+        <v>31.91</v>
       </c>
       <c r="L32">
-        <v>69.77</v>
+        <v>30.85</v>
       </c>
       <c r="M32">
-        <v>76.25</v>
+        <v>34.03</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2111,40 +2042,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D33">
-        <v>7.23</v>
+        <v>26.51</v>
       </c>
       <c r="E33">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G33">
-        <v>100</v>
+        <v>61.99</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="K33">
-        <v>5560.5</v>
+        <v>16700</v>
       </c>
       <c r="L33">
-        <v>5332.29</v>
+        <v>16030.86</v>
       </c>
       <c r="M33">
-        <v>6016.93</v>
+        <v>18038.29</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2155,40 +2086,40 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D34">
-        <v>4.82</v>
+        <v>22.89</v>
       </c>
       <c r="E34">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F34" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G34">
-        <v>100</v>
+        <v>52.17</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J34" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="K34">
-        <v>485.05</v>
+        <v>205.56</v>
       </c>
       <c r="L34">
-        <v>470.83</v>
+        <v>195.95</v>
       </c>
       <c r="M34">
-        <v>513.49</v>
+        <v>224.79</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2199,40 +2130,40 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D35">
-        <v>40.96</v>
+        <v>15.66</v>
       </c>
       <c r="E35">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="G35">
-        <v>90.06</v>
+        <v>27.89</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="K35">
-        <v>1484</v>
+        <v>693.95</v>
       </c>
       <c r="L35">
-        <v>1369.83</v>
+        <v>675.12</v>
       </c>
       <c r="M35">
-        <v>1712.34</v>
+        <v>731.61</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2243,40 +2174,40 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D36">
-        <v>52.17</v>
+        <v>14.46</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G36">
-        <v>52.17</v>
+        <v>14.46</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K36">
-        <v>33.14</v>
+        <v>978.2</v>
       </c>
       <c r="L36">
-        <v>31.27</v>
+        <v>963.75</v>
       </c>
       <c r="M36">
-        <v>36.89</v>
+        <v>1007.09</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2287,40 +2218,40 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D37">
-        <v>37.89</v>
+        <v>13.25</v>
       </c>
       <c r="E37">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G37">
         <v>65.06</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K37">
-        <v>845.6</v>
+        <v>829.95</v>
       </c>
       <c r="L37">
-        <v>811.83</v>
+        <v>794.88</v>
       </c>
       <c r="M37">
-        <v>913.14</v>
+        <v>900.09</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2331,40 +2262,40 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="D38">
-        <v>33.73</v>
+        <v>12.05</v>
       </c>
       <c r="E38">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="F38" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="G38">
-        <v>61.99</v>
+        <v>58.19</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K38">
-        <v>16810</v>
+        <v>3081.8</v>
       </c>
       <c r="L38">
-        <v>16155.71</v>
+        <v>2919.86</v>
       </c>
       <c r="M38">
-        <v>18118.57</v>
+        <v>3405.69</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2375,40 +2306,40 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D39">
-        <v>30.12</v>
+        <v>10.84</v>
       </c>
       <c r="E39">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F39" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="G39">
-        <v>30.12</v>
+        <v>10.84</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K39">
-        <v>1264.4</v>
+        <v>1709.4</v>
       </c>
       <c r="L39">
-        <v>1185.66</v>
+        <v>1661.99</v>
       </c>
       <c r="M39">
-        <v>1421.89</v>
+        <v>1804.22</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2419,40 +2350,40 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D40">
-        <v>27.71</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E40">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G40">
-        <v>65.59999999999999</v>
+        <v>21.69</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K40">
-        <v>196.92</v>
+        <v>5011.6</v>
       </c>
       <c r="L40">
-        <v>187.27</v>
+        <v>4892.53</v>
       </c>
       <c r="M40">
-        <v>216.22</v>
+        <v>5249.74</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2463,40 +2394,40 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D41">
-        <v>26.51</v>
+        <v>7.23</v>
       </c>
       <c r="E41">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G41">
-        <v>52.17</v>
+        <v>39.76</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K41">
-        <v>207.24</v>
+        <v>289.7</v>
       </c>
       <c r="L41">
-        <v>196.76</v>
+        <v>272.79</v>
       </c>
       <c r="M41">
-        <v>228.2</v>
+        <v>323.51</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2507,40 +2438,40 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D42">
-        <v>25.3</v>
+        <v>6.02</v>
       </c>
       <c r="E42">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="G42">
-        <v>45.78</v>
+        <v>31.33</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K42">
-        <v>1076.55</v>
+        <v>1176.1</v>
       </c>
       <c r="L42">
-        <v>1006.32</v>
+        <v>1111.99</v>
       </c>
       <c r="M42">
-        <v>1217.01</v>
+        <v>1304.32</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2551,40 +2482,40 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D43">
-        <v>22.89</v>
+        <v>4.82</v>
       </c>
       <c r="E43">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F43" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="G43">
-        <v>61.81</v>
+        <v>31.33</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K43">
-        <v>3797</v>
+        <v>7459.5</v>
       </c>
       <c r="L43">
-        <v>3540.4</v>
+        <v>7261.05</v>
       </c>
       <c r="M43">
-        <v>4310.2</v>
+        <v>7856.41</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2595,746 +2526,42 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D44">
-        <v>21.69</v>
+        <v>4.82</v>
       </c>
       <c r="E44">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G44">
-        <v>63.37</v>
+        <v>41.14</v>
       </c>
       <c r="H44">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K44">
-        <v>1487.5</v>
+        <v>455.5</v>
       </c>
       <c r="L44">
-        <v>1453.56</v>
+        <v>448.71</v>
       </c>
       <c r="M44">
-        <v>1555.39</v>
+        <v>469.08</v>
       </c>
       <c r="N44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
-      <c r="A45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45">
-        <v>21.69</v>
-      </c>
-      <c r="E45">
-        <v>3</v>
-      </c>
-      <c r="F45" t="s">
-        <v>99</v>
-      </c>
-      <c r="G45">
-        <v>40.12</v>
-      </c>
-      <c r="H45">
-        <v>1</v>
-      </c>
-      <c r="I45">
-        <v>2</v>
-      </c>
-      <c r="J45" t="s">
-        <v>106</v>
-      </c>
-      <c r="K45">
-        <v>347.1</v>
-      </c>
-      <c r="L45">
-        <v>329.46</v>
-      </c>
-      <c r="M45">
-        <v>382.38</v>
-      </c>
-      <c r="N45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
-      <c r="A46" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" t="s">
-        <v>86</v>
-      </c>
-      <c r="D46">
-        <v>20.48</v>
-      </c>
-      <c r="E46">
-        <v>32</v>
-      </c>
-      <c r="F46" t="s">
-        <v>98</v>
-      </c>
-      <c r="G46">
-        <v>54.76</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>3</v>
-      </c>
-      <c r="J46" t="s">
-        <v>106</v>
-      </c>
-      <c r="K46">
-        <v>254.6</v>
-      </c>
-      <c r="L46">
-        <v>237.94</v>
-      </c>
-      <c r="M46">
-        <v>287.93</v>
-      </c>
-      <c r="N46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
-      <c r="A47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47">
-        <v>20.48</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>100</v>
-      </c>
-      <c r="G47">
-        <v>20.48</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
-      <c r="J47" t="s">
-        <v>106</v>
-      </c>
-      <c r="K47">
-        <v>4276.3</v>
-      </c>
-      <c r="L47">
-        <v>4169.37</v>
-      </c>
-      <c r="M47">
-        <v>4490.17</v>
-      </c>
-      <c r="N47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
-      <c r="A48" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48">
-        <v>19.28</v>
-      </c>
-      <c r="E48">
-        <v>24</v>
-      </c>
-      <c r="F48" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48">
-        <v>26.69</v>
-      </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48" t="s">
-        <v>106</v>
-      </c>
-      <c r="K48">
-        <v>2010</v>
-      </c>
-      <c r="L48">
-        <v>1981.16</v>
-      </c>
-      <c r="M48">
-        <v>2067.69</v>
-      </c>
-      <c r="N48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="A49" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49">
-        <v>19.28</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49">
-        <v>19.28</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-      <c r="J49" t="s">
-        <v>106</v>
-      </c>
-      <c r="K49">
-        <v>1437.2</v>
-      </c>
-      <c r="L49">
-        <v>1358.27</v>
-      </c>
-      <c r="M49">
-        <v>1595.05</v>
-      </c>
-      <c r="N49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
-      <c r="A50" t="s">
-        <v>62</v>
-      </c>
-      <c r="B50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50">
-        <v>19.28</v>
-      </c>
-      <c r="E50">
-        <v>31</v>
-      </c>
-      <c r="F50" t="s">
-        <v>96</v>
-      </c>
-      <c r="G50">
-        <v>44.58</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>3</v>
-      </c>
-      <c r="J50" t="s">
-        <v>106</v>
-      </c>
-      <c r="K50">
-        <v>443.5</v>
-      </c>
-      <c r="L50">
-        <v>408.79</v>
-      </c>
-      <c r="M50">
-        <v>512.9299999999999</v>
-      </c>
-      <c r="N50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
-      <c r="C51" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51">
-        <v>18.07</v>
-      </c>
-      <c r="E51">
-        <v>27</v>
-      </c>
-      <c r="F51" t="s">
-        <v>97</v>
-      </c>
-      <c r="G51">
-        <v>58.19</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <v>0</v>
-      </c>
-      <c r="J51" t="s">
-        <v>106</v>
-      </c>
-      <c r="K51">
-        <v>3098.9</v>
-      </c>
-      <c r="L51">
-        <v>2942.59</v>
-      </c>
-      <c r="M51">
-        <v>3411.53</v>
-      </c>
-      <c r="N51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
-      <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
-        <v>77</v>
-      </c>
-      <c r="C52" t="s">
-        <v>86</v>
-      </c>
-      <c r="D52">
-        <v>14.46</v>
-      </c>
-      <c r="E52">
-        <v>25</v>
-      </c>
-      <c r="F52" t="s">
-        <v>93</v>
-      </c>
-      <c r="G52">
-        <v>27.89</v>
-      </c>
-      <c r="H52">
-        <v>2</v>
-      </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-      <c r="J52" t="s">
-        <v>106</v>
-      </c>
-      <c r="K52">
-        <v>696.3</v>
-      </c>
-      <c r="L52">
-        <v>675.58</v>
-      </c>
-      <c r="M52">
-        <v>737.75</v>
-      </c>
-      <c r="N52">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
-      <c r="A53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" t="s">
-        <v>73</v>
-      </c>
-      <c r="C53" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53">
-        <v>13.25</v>
-      </c>
-      <c r="E53">
-        <v>8</v>
-      </c>
-      <c r="F53" t="s">
-        <v>93</v>
-      </c>
-      <c r="G53">
-        <v>38.55</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-      <c r="J53" t="s">
-        <v>106</v>
-      </c>
-      <c r="K53">
-        <v>1602.2</v>
-      </c>
-      <c r="L53">
-        <v>1521.09</v>
-      </c>
-      <c r="M53">
-        <v>1764.43</v>
-      </c>
-      <c r="N53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
-      <c r="A54" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C54" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54">
-        <v>10.84</v>
-      </c>
-      <c r="E54">
-        <v>43</v>
-      </c>
-      <c r="F54" t="s">
-        <v>89</v>
-      </c>
-      <c r="G54">
-        <v>32.53</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>1</v>
-      </c>
-      <c r="J54" t="s">
-        <v>106</v>
-      </c>
-      <c r="K54">
-        <v>186.14</v>
-      </c>
-      <c r="L54">
-        <v>175.26</v>
-      </c>
-      <c r="M54">
-        <v>207.91</v>
-      </c>
-      <c r="N54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
-      <c r="A55" t="s">
-        <v>67</v>
-      </c>
-      <c r="B55" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55">
-        <v>9.640000000000001</v>
-      </c>
-      <c r="E55">
-        <v>33</v>
-      </c>
-      <c r="F55" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55">
-        <v>21.69</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55" t="s">
-        <v>106</v>
-      </c>
-      <c r="K55">
-        <v>5016.5</v>
-      </c>
-      <c r="L55">
-        <v>4893.53</v>
-      </c>
-      <c r="M55">
-        <v>5262.43</v>
-      </c>
-      <c r="N55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
-      <c r="A56" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56">
-        <v>6.02</v>
-      </c>
-      <c r="E56">
-        <v>48</v>
-      </c>
-      <c r="F56" t="s">
-        <v>93</v>
-      </c>
-      <c r="G56">
-        <v>31.33</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56" t="s">
-        <v>106</v>
-      </c>
-      <c r="K56">
-        <v>1180</v>
-      </c>
-      <c r="L56">
-        <v>1112.4</v>
-      </c>
-      <c r="M56">
-        <v>1315.21</v>
-      </c>
-      <c r="N56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
-      <c r="A57" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" t="s">
-        <v>86</v>
-      </c>
-      <c r="D57">
-        <v>4.82</v>
-      </c>
-      <c r="E57">
-        <v>18</v>
-      </c>
-      <c r="F57" t="s">
-        <v>95</v>
-      </c>
-      <c r="G57">
-        <v>10.84</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57" t="s">
-        <v>106</v>
-      </c>
-      <c r="K57">
-        <v>1699.9</v>
-      </c>
-      <c r="L57">
-        <v>1661.44</v>
-      </c>
-      <c r="M57">
-        <v>1776.82</v>
-      </c>
-      <c r="N57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
-      <c r="A58" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" t="s">
-        <v>73</v>
-      </c>
-      <c r="C58" t="s">
-        <v>86</v>
-      </c>
-      <c r="D58">
-        <v>4.82</v>
-      </c>
-      <c r="E58">
-        <v>44</v>
-      </c>
-      <c r="F58" t="s">
-        <v>92</v>
-      </c>
-      <c r="G58">
-        <v>41.14</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="J58" t="s">
-        <v>106</v>
-      </c>
-      <c r="K58">
-        <v>457.7</v>
-      </c>
-      <c r="L58">
-        <v>449.01</v>
-      </c>
-      <c r="M58">
-        <v>475.08</v>
-      </c>
-      <c r="N58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
-      <c r="A59" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" t="s">
-        <v>74</v>
-      </c>
-      <c r="C59" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59">
-        <v>4.82</v>
-      </c>
-      <c r="E59">
-        <v>18</v>
-      </c>
-      <c r="F59" t="s">
-        <v>93</v>
-      </c>
-      <c r="G59">
-        <v>31.33</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="J59" t="s">
-        <v>106</v>
-      </c>
-      <c r="K59">
-        <v>7424.5</v>
-      </c>
-      <c r="L59">
-        <v>7258.86</v>
-      </c>
-      <c r="M59">
-        <v>7755.79</v>
-      </c>
-      <c r="N59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14">
-      <c r="A60" t="s">
-        <v>72</v>
-      </c>
-      <c r="B60" t="s">
-        <v>77</v>
-      </c>
-      <c r="C60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D60">
-        <v>4.82</v>
-      </c>
-      <c r="E60">
-        <v>35</v>
-      </c>
-      <c r="F60" t="s">
-        <v>101</v>
-      </c>
-      <c r="G60">
-        <v>22.89</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60" t="s">
-        <v>106</v>
-      </c>
-      <c r="K60">
-        <v>6629</v>
-      </c>
-      <c r="L60">
-        <v>6322.07</v>
-      </c>
-      <c r="M60">
-        <v>7242.86</v>
-      </c>
-      <c r="N60">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update market regime dashboards to show dynamic stock count from data
- Replace hardcoded '176 stocks tracked' with dynamic count from sma_breadth_historical_latest.json
- Currently showing 564 stocks (actual count from data)
- Created append_historical_breadth.py script for nightly updates
- No dashboard restart required - changes load dynamically via JavaScript
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="76">
   <si>
     <t>Ticker</t>
   </si>
@@ -61,193 +61,169 @@
     <t>PAYTM</t>
   </si>
   <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>ETERNAL</t>
+  </si>
+  <si>
+    <t>OLECTRA</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
     <t>SHYAMMETL</t>
   </si>
   <si>
-    <t>TI</t>
+    <t>SYRMA</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>KIMS</t>
+  </si>
+  <si>
+    <t>3MINDIA</t>
   </si>
   <si>
     <t>UPL</t>
   </si>
   <si>
+    <t>ANANDRATHI</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>GLAND</t>
+  </si>
+  <si>
+    <t>MEDANTA</t>
+  </si>
+  <si>
     <t>NUVOCO</t>
   </si>
   <si>
-    <t>AGI</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>BORORENEW</t>
-  </si>
-  <si>
-    <t>SHK</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
+    <t>JINDALSTEL</t>
   </si>
   <si>
     <t>AMBUJACEM</t>
   </si>
   <si>
-    <t>IPCALAB</t>
-  </si>
-  <si>
-    <t>JINDALSTEL</t>
-  </si>
-  <si>
-    <t>3MINDIA</t>
-  </si>
-  <si>
-    <t>GLAND</t>
-  </si>
-  <si>
-    <t>KIMS</t>
-  </si>
-  <si>
-    <t>PATANJALI</t>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>JAGSNPHARM</t>
+  </si>
+  <si>
+    <t>VIJAYA</t>
+  </si>
+  <si>
+    <t>STLTECH</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
   </si>
   <si>
     <t>TORNTPHARM</t>
   </si>
   <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
-    <t>NMDC</t>
-  </si>
-  <si>
-    <t>MEDANTA</t>
-  </si>
-  <si>
-    <t>CIPLA</t>
-  </si>
-  <si>
-    <t>OLECTRA</t>
-  </si>
-  <si>
-    <t>SUPREMEIND</t>
-  </si>
-  <si>
-    <t>ETERNAL</t>
-  </si>
-  <si>
-    <t>HOMEFIRST</t>
-  </si>
-  <si>
-    <t>TRIDENT</t>
+    <t>SBILIFE</t>
+  </si>
+  <si>
+    <t>ICICIBANK</t>
   </si>
   <si>
     <t>DIXON</t>
   </si>
   <si>
-    <t>LXCHEM</t>
-  </si>
-  <si>
-    <t>HINDALCO</t>
-  </si>
-  <si>
-    <t>ZYDUSLIFE</t>
-  </si>
-  <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
-    <t>LALPATHLAB</t>
+    <t>DABUR</t>
+  </si>
+  <si>
+    <t>ALKEM</t>
   </si>
   <si>
     <t>JBCHEPHARM</t>
   </si>
   <si>
-    <t>ALKEM</t>
-  </si>
-  <si>
-    <t>TFCILTD</t>
-  </si>
-  <si>
-    <t>EIDPARRY</t>
-  </si>
-  <si>
-    <t>APOLLOHOSP</t>
-  </si>
-  <si>
-    <t>TMB</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
     <t>Consumer Cyclical</t>
   </si>
   <si>
-    <t>Healthcare</t>
+    <t>Financial Services</t>
+  </si>
+  <si>
+    <t>Basic Materials</t>
   </si>
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Basic Materials</t>
-  </si>
-  <si>
-    <t>Industrials</t>
-  </si>
-  <si>
-    <t>Financial Services</t>
+    <t>Consumer Defensive</t>
   </si>
   <si>
     <t>G_Pattern</t>
   </si>
   <si>
+    <t>Building_G</t>
+  </si>
+  <si>
+    <t>KC_Breakout_Watch</t>
+  </si>
+  <si>
+    <t>Early_Setup</t>
+  </si>
+  <si>
     <t>H2_Momentum_Start</t>
   </si>
   <si>
-    <t>KC_Breakout_Watch</t>
-  </si>
-  <si>
-    <t>Early_Setup</t>
-  </si>
-  <si>
-    <t>Power_H2_Volume</t>
+    <t>KC_Multi_H2</t>
   </si>
   <si>
     <t>2025-07-11</t>
   </si>
   <si>
+    <t>2025-07-25</t>
+  </si>
+  <si>
     <t>2025-07-16</t>
   </si>
   <si>
+    <t>2025-07-22</t>
+  </si>
+  <si>
     <t>2025-07-07</t>
   </si>
   <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
     <t>2025-07-15</t>
   </si>
   <si>
-    <t>2025-07-08</t>
-  </si>
-  <si>
     <t>2025-07-21</t>
   </si>
   <si>
-    <t>2025-07-18</t>
-  </si>
-  <si>
-    <t>2025-07-25</t>
-  </si>
-  <si>
-    <t>2025-07-22</t>
+    <t>2025-07-28</t>
   </si>
   <si>
     <t>2025-07-09</t>
@@ -256,7 +232,7 @@
     <t>G PATTERN CONFIRMED - FULL POSITION (100%)</t>
   </si>
   <si>
-    <t>PATTERN EMERGING - INITIAL POSITION (25%)</t>
+    <t>G PATTERN DEVELOPING - DOUBLE POSITION (50%)</t>
   </si>
   <si>
     <t>HOLD AND MONITOR - PATTERN MATURE</t>
@@ -623,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -678,19 +654,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D2">
-        <v>59.04</v>
+        <v>67.47</v>
       </c>
       <c r="E2">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -702,16 +678,16 @@
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="K2">
-        <v>1067</v>
+        <v>1094.7</v>
       </c>
       <c r="L2">
-        <v>992.6900000000001</v>
+        <v>1017.73</v>
       </c>
       <c r="M2">
-        <v>1215.61</v>
+        <v>1248.64</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -722,40 +698,40 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D3">
-        <v>68.01000000000001</v>
+        <v>100</v>
       </c>
       <c r="E3">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="K3">
-        <v>965.95</v>
+        <v>1571.3</v>
       </c>
       <c r="L3">
-        <v>920.09</v>
+        <v>1518.07</v>
       </c>
       <c r="M3">
-        <v>1057.66</v>
+        <v>1677.76</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -766,19 +742,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
       </c>
       <c r="D4">
         <v>37.35</v>
       </c>
       <c r="E4">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -787,19 +763,19 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K4">
-        <v>496.2</v>
+        <v>509.2</v>
       </c>
       <c r="L4">
-        <v>445.93</v>
+        <v>455.4</v>
       </c>
       <c r="M4">
-        <v>596.74</v>
+        <v>616.8</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -810,40 +786,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
       <c r="D5">
-        <v>34.94</v>
+        <v>37.35</v>
       </c>
       <c r="E5">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G5">
-        <v>85.23999999999999</v>
+        <v>92.47</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K5">
-        <v>722.7</v>
+        <v>307.75</v>
       </c>
       <c r="L5">
-        <v>690.74</v>
+        <v>287.26</v>
       </c>
       <c r="M5">
-        <v>786.61</v>
+        <v>348.72</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -854,40 +830,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" t="s">
-        <v>66</v>
-      </c>
       <c r="D6">
-        <v>34.94</v>
+        <v>37.35</v>
       </c>
       <c r="E6">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G6">
-        <v>84.04000000000001</v>
+        <v>90.06</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K6">
-        <v>413.45</v>
+        <v>1445</v>
       </c>
       <c r="L6">
-        <v>386.28</v>
+        <v>1323.39</v>
       </c>
       <c r="M6">
-        <v>467.79</v>
+        <v>1688.23</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -898,40 +874,40 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D7">
-        <v>33.73</v>
+        <v>34.94</v>
       </c>
       <c r="E7">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>82.83</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K7">
-        <v>937</v>
+        <v>847.35</v>
       </c>
       <c r="L7">
-        <v>853.14</v>
+        <v>806.39</v>
       </c>
       <c r="M7">
-        <v>1104.71</v>
+        <v>929.26</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -942,40 +918,40 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>33.73</v>
       </c>
       <c r="E8">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G8">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K8">
-        <v>847.8</v>
+        <v>960</v>
       </c>
       <c r="L8">
-        <v>805.29</v>
+        <v>911</v>
       </c>
       <c r="M8">
-        <v>932.8099999999999</v>
+        <v>1058</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -986,40 +962,40 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D9">
-        <v>31.33</v>
+        <v>32.53</v>
       </c>
       <c r="E9">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G9">
-        <v>92.11</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K9">
-        <v>625</v>
+        <v>746</v>
       </c>
       <c r="L9">
-        <v>567.5</v>
+        <v>681.3200000000001</v>
       </c>
       <c r="M9">
-        <v>740</v>
+        <v>875.36</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1030,40 +1006,40 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D10">
-        <v>30.12</v>
+        <v>31.33</v>
       </c>
       <c r="E10">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G10">
         <v>100</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K10">
-        <v>262</v>
+        <v>954.65</v>
       </c>
       <c r="L10">
-        <v>247.62</v>
+        <v>867.34</v>
       </c>
       <c r="M10">
-        <v>290.76</v>
+        <v>1129.28</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1074,40 +1050,40 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>28.92</v>
+      </c>
+      <c r="E11">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
         <v>66</v>
       </c>
-      <c r="D11">
-        <v>30.12</v>
-      </c>
-      <c r="E11">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
       <c r="G11">
-        <v>100</v>
+        <v>87.65000000000001</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K11">
-        <v>731.1</v>
+        <v>771.55</v>
       </c>
       <c r="L11">
-        <v>669.03</v>
+        <v>727.09</v>
       </c>
       <c r="M11">
-        <v>855.24</v>
+        <v>860.46</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1118,40 +1094,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>25.3</v>
+      </c>
+      <c r="E12">
         <v>67</v>
       </c>
-      <c r="D12">
-        <v>27.71</v>
-      </c>
-      <c r="E12">
-        <v>44</v>
-      </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K12">
-        <v>682</v>
+        <v>31245</v>
       </c>
       <c r="L12">
-        <v>649.25</v>
+        <v>29876.41</v>
       </c>
       <c r="M12">
-        <v>747.5</v>
+        <v>33982.18</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1162,40 +1138,40 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D13">
-        <v>27.71</v>
+        <v>25.3</v>
       </c>
       <c r="E13">
         <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K13">
-        <v>613.95</v>
+        <v>728.8</v>
       </c>
       <c r="L13">
-        <v>593.6900000000001</v>
+        <v>696.79</v>
       </c>
       <c r="M13">
-        <v>654.46</v>
+        <v>792.83</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1206,40 +1182,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>22.89</v>
+      </c>
+      <c r="E14">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
         <v>67</v>
       </c>
-      <c r="D14">
-        <v>26.51</v>
-      </c>
-      <c r="E14">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14">
+        <v>96.08</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
         <v>73</v>
       </c>
-      <c r="G14">
-        <v>70.78</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
-      <c r="J14" t="s">
-        <v>81</v>
-      </c>
       <c r="K14">
-        <v>1519.7</v>
+        <v>2655</v>
       </c>
       <c r="L14">
-        <v>1438.6</v>
+        <v>2440.3</v>
       </c>
       <c r="M14">
-        <v>1681.9</v>
+        <v>3084.4</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1250,40 +1226,40 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>24.1</v>
+        <v>16.87</v>
       </c>
       <c r="E15">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G15">
         <v>100</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K15">
-        <v>1001.2</v>
+        <v>691</v>
       </c>
       <c r="L15">
-        <v>966.01</v>
+        <v>652.6799999999999</v>
       </c>
       <c r="M15">
-        <v>1071.59</v>
+        <v>767.64</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1294,40 +1270,40 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D16">
-        <v>22.89</v>
+        <v>16.87</v>
       </c>
       <c r="E16">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16">
+        <v>86.45</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
         <v>73</v>
       </c>
-      <c r="G16">
-        <v>92.47</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>4</v>
-      </c>
-      <c r="J16" t="s">
-        <v>81</v>
-      </c>
       <c r="K16">
-        <v>31050</v>
+        <v>2055.2</v>
       </c>
       <c r="L16">
-        <v>29766.56</v>
+        <v>1931.4</v>
       </c>
       <c r="M16">
-        <v>33616.87</v>
+        <v>2302.8</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1338,40 +1314,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D17">
-        <v>22.89</v>
+        <v>15.66</v>
       </c>
       <c r="E17">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G17">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K17">
-        <v>2023.7</v>
+        <v>1359.1</v>
       </c>
       <c r="L17">
-        <v>1901.39</v>
+        <v>1279.46</v>
       </c>
       <c r="M17">
-        <v>2268.33</v>
+        <v>1518.39</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1382,40 +1358,40 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D18">
-        <v>22.89</v>
+        <v>14.46</v>
       </c>
       <c r="E18">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18">
+        <v>84.04000000000001</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
         <v>73</v>
       </c>
-      <c r="G18">
-        <v>87.65000000000001</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>81</v>
-      </c>
       <c r="K18">
-        <v>761.45</v>
+        <v>411.1</v>
       </c>
       <c r="L18">
-        <v>717.76</v>
+        <v>382.74</v>
       </c>
       <c r="M18">
-        <v>848.8200000000001</v>
+        <v>467.81</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1426,40 +1402,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D19">
-        <v>21.69</v>
+        <v>13.25</v>
       </c>
       <c r="E19">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G19">
         <v>100</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K19">
-        <v>1885</v>
+        <v>978.75</v>
       </c>
       <c r="L19">
-        <v>1783.86</v>
+        <v>951.05</v>
       </c>
       <c r="M19">
-        <v>2087.29</v>
+        <v>1034.15</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1470,40 +1446,40 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20">
+        <v>13.25</v>
+      </c>
+      <c r="E20">
         <v>66</v>
       </c>
-      <c r="D20">
-        <v>16.87</v>
-      </c>
-      <c r="E20">
-        <v>56</v>
-      </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G20">
-        <v>82.65000000000001</v>
+        <v>100</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K20">
-        <v>3605.5</v>
+        <v>612.7</v>
       </c>
       <c r="L20">
-        <v>3478.97</v>
+        <v>593.13</v>
       </c>
       <c r="M20">
-        <v>3858.56</v>
+        <v>651.84</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1514,40 +1490,40 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21">
+        <v>10.84</v>
+      </c>
+      <c r="E21">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21">
-        <v>14.46</v>
-      </c>
-      <c r="E21">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
       <c r="G21">
-        <v>96.08</v>
+        <v>100</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K21">
-        <v>2600.9</v>
+        <v>487.05</v>
       </c>
       <c r="L21">
-        <v>2392.57</v>
+        <v>470.77</v>
       </c>
       <c r="M21">
-        <v>3017.56</v>
+        <v>519.62</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1558,19 +1534,19 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D22">
-        <v>14.46</v>
+        <v>7.23</v>
       </c>
       <c r="E22">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G22">
         <v>100</v>
@@ -1582,16 +1558,16 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K22">
-        <v>394.15</v>
+        <v>5559</v>
       </c>
       <c r="L22">
-        <v>377.56</v>
+        <v>5332.5</v>
       </c>
       <c r="M22">
-        <v>427.33</v>
+        <v>6012</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1602,19 +1578,19 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D23">
-        <v>13.25</v>
+        <v>7.23</v>
       </c>
       <c r="E23">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G23">
         <v>100</v>
@@ -1626,16 +1602,16 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K23">
-        <v>5556.5</v>
+        <v>38250</v>
       </c>
       <c r="L23">
-        <v>5325.93</v>
+        <v>36624.29</v>
       </c>
       <c r="M23">
-        <v>6017.64</v>
+        <v>41501.43</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1646,40 +1622,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24">
+        <v>48.19</v>
+      </c>
+      <c r="E24">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
         <v>67</v>
       </c>
-      <c r="D24">
-        <v>8.43</v>
-      </c>
-      <c r="E24">
-        <v>64</v>
-      </c>
-      <c r="F24" t="s">
-        <v>71</v>
-      </c>
       <c r="G24">
-        <v>100</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J24" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K24">
-        <v>37835</v>
+        <v>293.4</v>
       </c>
       <c r="L24">
-        <v>36175.71</v>
+        <v>261.03</v>
       </c>
       <c r="M24">
-        <v>41153.57</v>
+        <v>358.14</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1690,40 +1666,40 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
         <v>57</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
       <c r="D25">
-        <v>7.23</v>
+        <v>45.78</v>
       </c>
       <c r="E25">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G25">
-        <v>81.27</v>
+        <v>45.78</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K25">
-        <v>71.8</v>
+        <v>1150.3</v>
       </c>
       <c r="L25">
-        <v>69.73999999999999</v>
+        <v>1064.79</v>
       </c>
       <c r="M25">
-        <v>75.91</v>
+        <v>1321.31</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1734,40 +1710,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>7.23</v>
+        <v>43.37</v>
       </c>
       <c r="E26">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>77.83</v>
       </c>
       <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
         <v>1</v>
       </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
       <c r="J26" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="K26">
-        <v>1322.9</v>
+        <v>127.2</v>
       </c>
       <c r="L26">
-        <v>1260.29</v>
+        <v>114.14</v>
       </c>
       <c r="M26">
-        <v>1448.11</v>
+        <v>153.32</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1778,40 +1754,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D27">
-        <v>46.14</v>
+        <v>43.37</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G27">
-        <v>71.98999999999999</v>
+        <v>65.06</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K27">
-        <v>1531.7</v>
+        <v>889.6</v>
       </c>
       <c r="L27">
-        <v>1481.77</v>
+        <v>846.6799999999999</v>
       </c>
       <c r="M27">
-        <v>1631.56</v>
+        <v>975.4400000000001</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1822,40 +1798,40 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>40.3</v>
+      </c>
+      <c r="E28">
         <v>62</v>
       </c>
-      <c r="C28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28">
-        <v>45.78</v>
-      </c>
-      <c r="E28">
-        <v>34</v>
-      </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G28">
-        <v>90.06</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K28">
-        <v>1472.3</v>
+        <v>3622</v>
       </c>
       <c r="L28">
-        <v>1356.2</v>
+        <v>3495.7</v>
       </c>
       <c r="M28">
-        <v>1704.5</v>
+        <v>3874.6</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1866,40 +1842,40 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D29">
-        <v>41.33</v>
+        <v>31.33</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="G29">
-        <v>41.33</v>
+        <v>31.33</v>
       </c>
       <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
         <v>1</v>
       </c>
-      <c r="I29">
-        <v>3</v>
-      </c>
       <c r="J29" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K29">
-        <v>4289</v>
+        <v>1850.1</v>
       </c>
       <c r="L29">
-        <v>4169.74</v>
+        <v>1802.06</v>
       </c>
       <c r="M29">
-        <v>4527.51</v>
+        <v>1946.17</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -1910,40 +1886,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D30">
-        <v>40.96</v>
+        <v>24.1</v>
       </c>
       <c r="E30">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G30">
-        <v>92.47</v>
+        <v>63.37</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K30">
-        <v>310.6</v>
+        <v>1488.3</v>
       </c>
       <c r="L30">
-        <v>290.08</v>
+        <v>1452.93</v>
       </c>
       <c r="M30">
-        <v>351.64</v>
+        <v>1559.04</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -1954,22 +1930,22 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D31">
-        <v>52.17</v>
+        <v>20.48</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G31">
-        <v>52.17</v>
+        <v>61.99</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -1978,16 +1954,16 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K31">
-        <v>1480.5</v>
+        <v>16764</v>
       </c>
       <c r="L31">
-        <v>1375.17</v>
+        <v>16084.29</v>
       </c>
       <c r="M31">
-        <v>1691.16</v>
+        <v>18123.43</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -1998,40 +1974,40 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32">
+        <v>12.05</v>
+      </c>
+      <c r="E32">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s">
         <v>65</v>
       </c>
-      <c r="D32">
-        <v>38.92</v>
-      </c>
-      <c r="E32">
-        <v>8</v>
-      </c>
-      <c r="F32" t="s">
-        <v>78</v>
-      </c>
       <c r="G32">
-        <v>52.17</v>
+        <v>60.24</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K32">
-        <v>31.91</v>
+        <v>520.95</v>
       </c>
       <c r="L32">
-        <v>30.85</v>
+        <v>507.11</v>
       </c>
       <c r="M32">
-        <v>34.03</v>
+        <v>548.63</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2042,40 +2018,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D33">
-        <v>26.51</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E33">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="G33">
-        <v>61.99</v>
+        <v>21.69</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K33">
-        <v>16700</v>
+        <v>5049.1</v>
       </c>
       <c r="L33">
-        <v>16030.86</v>
+        <v>4903.61</v>
       </c>
       <c r="M33">
-        <v>18038.29</v>
+        <v>5340.08</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2086,482 +2062,42 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D34">
-        <v>22.89</v>
+        <v>4.82</v>
       </c>
       <c r="E34">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34">
-        <v>52.17</v>
+        <v>10.84</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K34">
-        <v>205.56</v>
+        <v>1708.5</v>
       </c>
       <c r="L34">
-        <v>195.95</v>
+        <v>1665.06</v>
       </c>
       <c r="M34">
-        <v>224.79</v>
+        <v>1795.38</v>
       </c>
       <c r="N34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35">
-        <v>15.66</v>
-      </c>
-      <c r="E35">
-        <v>30</v>
-      </c>
-      <c r="F35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35">
-        <v>27.89</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>83</v>
-      </c>
-      <c r="K35">
-        <v>693.95</v>
-      </c>
-      <c r="L35">
-        <v>675.12</v>
-      </c>
-      <c r="M35">
-        <v>731.61</v>
-      </c>
-      <c r="N35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36">
-        <v>14.46</v>
-      </c>
-      <c r="E36">
-        <v>5</v>
-      </c>
-      <c r="F36" t="s">
-        <v>71</v>
-      </c>
-      <c r="G36">
-        <v>14.46</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>83</v>
-      </c>
-      <c r="K36">
-        <v>978.2</v>
-      </c>
-      <c r="L36">
-        <v>963.75</v>
-      </c>
-      <c r="M36">
-        <v>1007.09</v>
-      </c>
-      <c r="N36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37">
-        <v>13.25</v>
-      </c>
-      <c r="E37">
-        <v>65</v>
-      </c>
-      <c r="F37" t="s">
-        <v>71</v>
-      </c>
-      <c r="G37">
-        <v>65.06</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>83</v>
-      </c>
-      <c r="K37">
-        <v>829.95</v>
-      </c>
-      <c r="L37">
-        <v>794.88</v>
-      </c>
-      <c r="M37">
-        <v>900.09</v>
-      </c>
-      <c r="N37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D38">
-        <v>12.05</v>
-      </c>
-      <c r="E38">
-        <v>32</v>
-      </c>
-      <c r="F38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38">
-        <v>58.19</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>83</v>
-      </c>
-      <c r="K38">
-        <v>3081.8</v>
-      </c>
-      <c r="L38">
-        <v>2919.86</v>
-      </c>
-      <c r="M38">
-        <v>3405.69</v>
-      </c>
-      <c r="N38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
-      <c r="A39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39">
-        <v>10.84</v>
-      </c>
-      <c r="E39">
-        <v>23</v>
-      </c>
-      <c r="F39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39">
-        <v>10.84</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>83</v>
-      </c>
-      <c r="K39">
-        <v>1709.4</v>
-      </c>
-      <c r="L39">
-        <v>1661.99</v>
-      </c>
-      <c r="M39">
-        <v>1804.22</v>
-      </c>
-      <c r="N39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
-      <c r="A40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40">
-        <v>9.640000000000001</v>
-      </c>
-      <c r="E40">
-        <v>38</v>
-      </c>
-      <c r="F40" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40">
-        <v>21.69</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40">
-        <v>5011.6</v>
-      </c>
-      <c r="L40">
-        <v>4892.53</v>
-      </c>
-      <c r="M40">
-        <v>5249.74</v>
-      </c>
-      <c r="N40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>67</v>
-      </c>
-      <c r="D41">
-        <v>7.23</v>
-      </c>
-      <c r="E41">
-        <v>44</v>
-      </c>
-      <c r="F41" t="s">
-        <v>71</v>
-      </c>
-      <c r="G41">
-        <v>39.76</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>83</v>
-      </c>
-      <c r="K41">
-        <v>289.7</v>
-      </c>
-      <c r="L41">
-        <v>272.79</v>
-      </c>
-      <c r="M41">
-        <v>323.51</v>
-      </c>
-      <c r="N41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>67</v>
-      </c>
-      <c r="D42">
-        <v>6.02</v>
-      </c>
-      <c r="E42">
-        <v>53</v>
-      </c>
-      <c r="F42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42">
-        <v>31.33</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42" t="s">
-        <v>83</v>
-      </c>
-      <c r="K42">
-        <v>1176.1</v>
-      </c>
-      <c r="L42">
-        <v>1111.99</v>
-      </c>
-      <c r="M42">
-        <v>1304.32</v>
-      </c>
-      <c r="N42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
-      <c r="A43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43">
-        <v>4.82</v>
-      </c>
-      <c r="E43">
-        <v>23</v>
-      </c>
-      <c r="F43" t="s">
-        <v>71</v>
-      </c>
-      <c r="G43">
-        <v>31.33</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43" t="s">
-        <v>83</v>
-      </c>
-      <c r="K43">
-        <v>7459.5</v>
-      </c>
-      <c r="L43">
-        <v>7261.05</v>
-      </c>
-      <c r="M43">
-        <v>7856.41</v>
-      </c>
-      <c r="N43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
-      <c r="A44" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44">
-        <v>4.82</v>
-      </c>
-      <c r="E44">
-        <v>48</v>
-      </c>
-      <c r="F44" t="s">
-        <v>70</v>
-      </c>
-      <c r="G44">
-        <v>41.14</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44" t="s">
-        <v>83</v>
-      </c>
-      <c r="K44">
-        <v>455.5</v>
-      </c>
-      <c r="L44">
-        <v>448.71</v>
-      </c>
-      <c r="M44">
-        <v>469.08</v>
-      </c>
-      <c r="N44">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add hourly reversal scanners with 30-minute scheduled runs
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="90">
   <si>
     <t>Ticker</t>
   </si>
@@ -58,103 +58,145 @@
     <t>Risk_Reward</t>
   </si>
   <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
+    <t>GLAND</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>AMBER</t>
+  </si>
+  <si>
+    <t>PPLPHARMA</t>
+  </si>
+  <si>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
     <t>PAYTM</t>
   </si>
   <si>
-    <t>CIPLA</t>
-  </si>
-  <si>
-    <t>TI</t>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>TATACHEM</t>
+  </si>
+  <si>
+    <t>STLTECH</t>
+  </si>
+  <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>OLECTRA</t>
+  </si>
+  <si>
+    <t>SYRMA</t>
   </si>
   <si>
     <t>ETERNAL</t>
   </si>
   <si>
-    <t>OLECTRA</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
+    <t>ANANDRATHI</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
   </si>
   <si>
     <t>AGI</t>
   </si>
   <si>
-    <t>KIMS</t>
-  </si>
-  <si>
-    <t>3MINDIA</t>
-  </si>
-  <si>
     <t>UPL</t>
   </si>
   <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
-    <t>GLAND</t>
-  </si>
-  <si>
-    <t>MEDANTA</t>
+    <t>SUMICHEM</t>
   </si>
   <si>
     <t>NUVOCO</t>
   </si>
   <si>
+    <t>ASIANPAINT</t>
+  </si>
+  <si>
+    <t>RAMCOCEM</t>
+  </si>
+  <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>AJANTPHARM</t>
+  </si>
+  <si>
     <t>AMBUJACEM</t>
   </si>
   <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
+    <t>APARINDS</t>
   </si>
   <si>
     <t>JAGSNPHARM</t>
   </si>
   <si>
+    <t>JBCHEPHARM</t>
+  </si>
+  <si>
     <t>VIJAYA</t>
   </si>
   <si>
-    <t>STLTECH</t>
-  </si>
-  <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
-    <t>TORNTPHARM</t>
-  </si>
-  <si>
-    <t>SBILIFE</t>
-  </si>
-  <si>
-    <t>ICICIBANK</t>
+    <t>SUNPHARMA</t>
+  </si>
+  <si>
+    <t>EIDPARRY</t>
   </si>
   <si>
     <t>DIXON</t>
   </si>
   <si>
-    <t>DABUR</t>
+    <t>COROMANDEL</t>
+  </si>
+  <si>
+    <t>BIRLACORPN</t>
+  </si>
+  <si>
+    <t>INDIGOPNTS</t>
   </si>
   <si>
     <t>ALKEM</t>
   </si>
   <si>
-    <t>JBCHEPHARM</t>
+    <t>HINDUNILVR</t>
+  </si>
+  <si>
+    <t>ESCORTS</t>
+  </si>
+  <si>
+    <t>DRREDDY</t>
+  </si>
+  <si>
+    <t>APOLLOHOSP</t>
+  </si>
+  <si>
+    <t>PIIND</t>
+  </si>
+  <si>
+    <t>ZYDUSLIFE</t>
   </si>
   <si>
     <t>Unknown</t>
@@ -163,12 +205,12 @@
     <t>Healthcare</t>
   </si>
   <si>
+    <t>Consumer Cyclical</t>
+  </si>
+  <si>
     <t>Industrials</t>
   </si>
   <si>
-    <t>Consumer Cyclical</t>
-  </si>
-  <si>
     <t>Financial Services</t>
   </si>
   <si>
@@ -181,58 +223,58 @@
     <t>Consumer Defensive</t>
   </si>
   <si>
-    <t>G_Pattern</t>
-  </si>
-  <si>
     <t>Building_G</t>
   </si>
   <si>
+    <t>H2_Momentum_Start</t>
+  </si>
+  <si>
+    <t>Power_H2_Volume</t>
+  </si>
+  <si>
     <t>KC_Breakout_Watch</t>
   </si>
   <si>
     <t>Early_Setup</t>
   </si>
   <si>
-    <t>H2_Momentum_Start</t>
-  </si>
-  <si>
-    <t>KC_Multi_H2</t>
+    <t>2025-07-15</t>
+  </si>
+  <si>
+    <t>2025-07-25</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
+    <t>2025-07-16</t>
   </si>
   <si>
     <t>2025-07-11</t>
   </si>
   <si>
-    <t>2025-07-25</t>
-  </si>
-  <si>
-    <t>2025-07-16</t>
-  </si>
-  <si>
     <t>2025-07-22</t>
   </si>
   <si>
-    <t>2025-07-07</t>
-  </si>
-  <si>
     <t>2025-07-08</t>
   </si>
   <si>
-    <t>2025-07-15</t>
-  </si>
-  <si>
     <t>2025-07-21</t>
   </si>
   <si>
-    <t>2025-07-28</t>
-  </si>
-  <si>
     <t>2025-07-09</t>
   </si>
   <si>
-    <t>G PATTERN CONFIRMED - FULL POSITION (100%)</t>
+    <t>2025-07-29</t>
+  </si>
+  <si>
+    <t>2025-07-18</t>
   </si>
   <si>
     <t>G PATTERN DEVELOPING - DOUBLE POSITION (50%)</t>
+  </si>
+  <si>
+    <t>PATTERN EMERGING - INITIAL POSITION (25%)</t>
   </si>
   <si>
     <t>HOLD AND MONITOR - PATTERN MATURE</t>
@@ -599,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -654,40 +696,40 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="D2">
-        <v>67.47</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="K2">
-        <v>1094.7</v>
+        <v>3760.4</v>
       </c>
       <c r="L2">
-        <v>1017.73</v>
+        <v>3618.31</v>
       </c>
       <c r="M2">
-        <v>1248.64</v>
+        <v>4044.57</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -698,19 +740,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>53.01</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -722,16 +764,16 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="K3">
-        <v>1571.3</v>
+        <v>1575.7</v>
       </c>
       <c r="L3">
-        <v>1518.07</v>
+        <v>1522</v>
       </c>
       <c r="M3">
-        <v>1677.76</v>
+        <v>1683.1</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -742,40 +784,40 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D4">
-        <v>37.35</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="E4">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="K4">
-        <v>509.2</v>
+        <v>909.65</v>
       </c>
       <c r="L4">
-        <v>455.4</v>
+        <v>864.53</v>
       </c>
       <c r="M4">
-        <v>616.8</v>
+        <v>999.89</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -786,40 +828,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D5">
-        <v>37.35</v>
+        <v>66.81</v>
       </c>
       <c r="E5">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G5">
-        <v>92.47</v>
+        <v>86.45</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="K5">
-        <v>307.75</v>
+        <v>2086.8</v>
       </c>
       <c r="L5">
-        <v>287.26</v>
+        <v>1959.29</v>
       </c>
       <c r="M5">
-        <v>348.72</v>
+        <v>2341.83</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -830,40 +872,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D6">
-        <v>37.35</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="E6">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G6">
-        <v>90.06</v>
+        <v>100</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="K6">
-        <v>1445</v>
+        <v>39805</v>
       </c>
       <c r="L6">
-        <v>1323.39</v>
+        <v>37945.71</v>
       </c>
       <c r="M6">
-        <v>1688.23</v>
+        <v>43523.57</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -874,40 +916,40 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D7">
-        <v>34.94</v>
+        <v>50.96</v>
       </c>
       <c r="E7">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G7">
-        <v>82.83</v>
+        <v>79.04000000000001</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K7">
-        <v>847.35</v>
+        <v>7789</v>
       </c>
       <c r="L7">
-        <v>806.39</v>
+        <v>7255.81</v>
       </c>
       <c r="M7">
-        <v>929.26</v>
+        <v>8855.379999999999</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -918,40 +960,40 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D8">
-        <v>33.73</v>
+        <v>38.92</v>
       </c>
       <c r="E8">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K8">
-        <v>960</v>
+        <v>205.98</v>
       </c>
       <c r="L8">
-        <v>911</v>
+        <v>202.31</v>
       </c>
       <c r="M8">
-        <v>1058</v>
+        <v>213.31</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -962,19 +1004,19 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D9">
-        <v>32.53</v>
+        <v>38.55</v>
       </c>
       <c r="E9">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -983,19 +1025,19 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K9">
-        <v>746</v>
+        <v>507</v>
       </c>
       <c r="L9">
-        <v>681.3200000000001</v>
+        <v>483.79</v>
       </c>
       <c r="M9">
-        <v>875.36</v>
+        <v>553.4299999999999</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1006,19 +1048,19 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D10">
-        <v>31.33</v>
+        <v>37.35</v>
       </c>
       <c r="E10">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -1030,16 +1072,16 @@
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K10">
-        <v>954.65</v>
+        <v>512.8</v>
       </c>
       <c r="L10">
-        <v>867.34</v>
+        <v>456.33</v>
       </c>
       <c r="M10">
-        <v>1129.28</v>
+        <v>625.74</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1050,40 +1092,40 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D11">
-        <v>28.92</v>
+        <v>37.35</v>
       </c>
       <c r="E11">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G11">
-        <v>87.65000000000001</v>
+        <v>100</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K11">
-        <v>771.55</v>
+        <v>1070.05</v>
       </c>
       <c r="L11">
-        <v>727.09</v>
+        <v>990.41</v>
       </c>
       <c r="M11">
-        <v>860.46</v>
+        <v>1229.34</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1094,40 +1136,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D12">
-        <v>25.3</v>
+        <v>37.35</v>
       </c>
       <c r="E12">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G12">
-        <v>92.47</v>
+        <v>82.83</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K12">
-        <v>31245</v>
+        <v>851.4</v>
       </c>
       <c r="L12">
-        <v>29876.41</v>
+        <v>810.89</v>
       </c>
       <c r="M12">
-        <v>33982.18</v>
+        <v>932.41</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1138,40 +1180,40 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D13">
-        <v>25.3</v>
+        <v>36.14</v>
       </c>
       <c r="E13">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="G13">
-        <v>85.23999999999999</v>
+        <v>75.23999999999999</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K13">
-        <v>728.8</v>
+        <v>999</v>
       </c>
       <c r="L13">
-        <v>696.79</v>
+        <v>946.11</v>
       </c>
       <c r="M13">
-        <v>792.83</v>
+        <v>1104.77</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1182,40 +1224,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D14">
-        <v>22.89</v>
+        <v>36.14</v>
       </c>
       <c r="E14">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G14">
-        <v>96.08</v>
+        <v>77.83</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K14">
-        <v>2655</v>
+        <v>128.23</v>
       </c>
       <c r="L14">
-        <v>2440.3</v>
+        <v>114.48</v>
       </c>
       <c r="M14">
-        <v>3084.4</v>
+        <v>155.74</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1226,40 +1268,40 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D15">
-        <v>16.87</v>
+        <v>34.94</v>
       </c>
       <c r="E15">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="G15">
         <v>100</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K15">
-        <v>691</v>
+        <v>972</v>
       </c>
       <c r="L15">
-        <v>652.6799999999999</v>
+        <v>919.59</v>
       </c>
       <c r="M15">
-        <v>767.64</v>
+        <v>1076.81</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1270,40 +1312,40 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D16">
-        <v>16.87</v>
+        <v>32.53</v>
       </c>
       <c r="E16">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G16">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K16">
-        <v>2055.2</v>
+        <v>709.55</v>
       </c>
       <c r="L16">
-        <v>1931.4</v>
+        <v>669.36</v>
       </c>
       <c r="M16">
-        <v>2302.8</v>
+        <v>789.92</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1314,40 +1356,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>31.33</v>
+      </c>
+      <c r="E17">
         <v>48</v>
       </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17">
-        <v>15.66</v>
-      </c>
-      <c r="E17">
-        <v>55</v>
-      </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>90.06</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K17">
-        <v>1359.1</v>
+        <v>1434.3</v>
       </c>
       <c r="L17">
-        <v>1279.46</v>
+        <v>1307.5</v>
       </c>
       <c r="M17">
-        <v>1518.39</v>
+        <v>1687.9</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1358,22 +1400,22 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D18">
-        <v>14.46</v>
+        <v>31.33</v>
       </c>
       <c r="E18">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G18">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1382,16 +1424,16 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K18">
-        <v>411.1</v>
+        <v>747.5</v>
       </c>
       <c r="L18">
-        <v>382.74</v>
+        <v>687.65</v>
       </c>
       <c r="M18">
-        <v>467.81</v>
+        <v>867.2</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1402,40 +1444,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D19">
-        <v>13.25</v>
+        <v>24.1</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K19">
-        <v>978.75</v>
+        <v>305.5</v>
       </c>
       <c r="L19">
-        <v>951.05</v>
+        <v>284.46</v>
       </c>
       <c r="M19">
-        <v>1034.15</v>
+        <v>347.59</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1446,40 +1488,40 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D20">
-        <v>13.25</v>
+        <v>22.89</v>
       </c>
       <c r="E20">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G20">
-        <v>100</v>
+        <v>96.08</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K20">
-        <v>612.7</v>
+        <v>2677.7</v>
       </c>
       <c r="L20">
-        <v>593.13</v>
+        <v>2460.51</v>
       </c>
       <c r="M20">
-        <v>651.84</v>
+        <v>3112.07</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1490,19 +1532,19 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D21">
-        <v>10.84</v>
+        <v>22.89</v>
       </c>
       <c r="E21">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -1514,16 +1556,16 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K21">
-        <v>487.05</v>
+        <v>5630.5</v>
       </c>
       <c r="L21">
-        <v>470.77</v>
+        <v>5396.07</v>
       </c>
       <c r="M21">
-        <v>519.62</v>
+        <v>6099.36</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1534,19 +1576,19 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22">
+        <v>20.48</v>
+      </c>
+      <c r="E22">
         <v>58</v>
       </c>
-      <c r="D22">
-        <v>7.23</v>
-      </c>
-      <c r="E22">
-        <v>65</v>
-      </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G22">
         <v>100</v>
@@ -1555,19 +1597,19 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K22">
-        <v>5559</v>
+        <v>960</v>
       </c>
       <c r="L22">
-        <v>5332.5</v>
+        <v>872.34</v>
       </c>
       <c r="M22">
-        <v>6012</v>
+        <v>1135.33</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1578,40 +1620,40 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D23">
-        <v>7.23</v>
+        <v>19.28</v>
       </c>
       <c r="E23">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G23">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="K23">
-        <v>38250</v>
+        <v>725.8</v>
       </c>
       <c r="L23">
-        <v>36624.29</v>
+        <v>693.4400000000001</v>
       </c>
       <c r="M23">
-        <v>41501.43</v>
+        <v>790.51</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1622,40 +1664,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24">
+        <v>15.66</v>
+      </c>
+      <c r="E24">
         <v>57</v>
       </c>
-      <c r="D24">
-        <v>48.19</v>
-      </c>
-      <c r="E24">
-        <v>38</v>
-      </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G24">
-        <v>68.01000000000001</v>
+        <v>100</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="K24">
-        <v>293.4</v>
+        <v>606.5</v>
       </c>
       <c r="L24">
-        <v>261.03</v>
+        <v>568.04</v>
       </c>
       <c r="M24">
-        <v>358.14</v>
+        <v>683.41</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1666,40 +1708,40 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D25">
-        <v>45.78</v>
+        <v>14.46</v>
       </c>
       <c r="E25">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G25">
-        <v>45.78</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="K25">
-        <v>1150.3</v>
+        <v>414.55</v>
       </c>
       <c r="L25">
-        <v>1064.79</v>
+        <v>383.2</v>
       </c>
       <c r="M25">
-        <v>1321.31</v>
+        <v>477.25</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1710,40 +1752,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="D26">
-        <v>43.37</v>
+        <v>14.46</v>
       </c>
       <c r="E26">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G26">
-        <v>77.83</v>
+        <v>91.27</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="K26">
-        <v>127.2</v>
+        <v>2408.2</v>
       </c>
       <c r="L26">
-        <v>114.14</v>
+        <v>2355.82</v>
       </c>
       <c r="M26">
-        <v>153.32</v>
+        <v>2512.96</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1754,40 +1796,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D27">
-        <v>43.37</v>
+        <v>14.46</v>
       </c>
       <c r="E27">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="G27">
-        <v>65.06</v>
+        <v>70.42</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="K27">
-        <v>889.6</v>
+        <v>1190.5</v>
       </c>
       <c r="L27">
-        <v>846.6799999999999</v>
+        <v>1121.95</v>
       </c>
       <c r="M27">
-        <v>975.4400000000001</v>
+        <v>1327.61</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1798,40 +1840,40 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D28">
-        <v>40.3</v>
+        <v>13.25</v>
       </c>
       <c r="E28">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F28" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="G28">
-        <v>82.65000000000001</v>
+        <v>100</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="K28">
-        <v>3622</v>
+        <v>984.6</v>
       </c>
       <c r="L28">
-        <v>3495.7</v>
+        <v>953.59</v>
       </c>
       <c r="M28">
-        <v>3874.6</v>
+        <v>1046.62</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1842,40 +1884,40 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="D29">
-        <v>31.33</v>
+        <v>12.05</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G29">
-        <v>31.33</v>
+        <v>100</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="K29">
-        <v>1850.1</v>
+        <v>397.15</v>
       </c>
       <c r="L29">
-        <v>1802.06</v>
+        <v>379.05</v>
       </c>
       <c r="M29">
-        <v>1946.17</v>
+        <v>433.36</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -1886,40 +1928,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D30">
-        <v>24.1</v>
+        <v>12.05</v>
       </c>
       <c r="E30">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G30">
-        <v>63.37</v>
+        <v>93.48999999999999</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="K30">
-        <v>1488.3</v>
+        <v>2825</v>
       </c>
       <c r="L30">
-        <v>1452.93</v>
+        <v>2676.41</v>
       </c>
       <c r="M30">
-        <v>1559.04</v>
+        <v>3122.19</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -1930,40 +1972,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D31">
-        <v>20.48</v>
+        <v>7.23</v>
       </c>
       <c r="E31">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G31">
-        <v>61.99</v>
+        <v>100</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="K31">
-        <v>16764</v>
+        <v>609</v>
       </c>
       <c r="L31">
-        <v>16084.29</v>
+        <v>593.84</v>
       </c>
       <c r="M31">
-        <v>18123.43</v>
+        <v>639.3200000000001</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -1974,40 +2016,40 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D32">
-        <v>12.05</v>
+        <v>42.17</v>
       </c>
       <c r="E32">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G32">
-        <v>60.24</v>
+        <v>44.58</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="K32">
-        <v>520.95</v>
+        <v>9751.5</v>
       </c>
       <c r="L32">
-        <v>507.11</v>
+        <v>9033.57</v>
       </c>
       <c r="M32">
-        <v>548.63</v>
+        <v>11187.36</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2018,40 +2060,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D33">
-        <v>9.640000000000001</v>
+        <v>34.94</v>
       </c>
       <c r="E33">
         <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="G33">
-        <v>21.69</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J33" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="K33">
-        <v>5049.1</v>
+        <v>285.27</v>
       </c>
       <c r="L33">
-        <v>4903.61</v>
+        <v>250.89</v>
       </c>
       <c r="M33">
-        <v>5340.08</v>
+        <v>354.03</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2062,42 +2104,658 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34">
+        <v>33.73</v>
+      </c>
+      <c r="E34">
+        <v>36</v>
+      </c>
+      <c r="F34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34">
+        <v>33.73</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>89</v>
+      </c>
+      <c r="K34">
+        <v>1797</v>
+      </c>
+      <c r="L34">
+        <v>1731.7</v>
+      </c>
+      <c r="M34">
+        <v>1927.6</v>
+      </c>
+      <c r="N34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35">
+        <v>31.33</v>
+      </c>
+      <c r="E35">
+        <v>36</v>
+      </c>
+      <c r="F35" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35">
+        <v>45.78</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35">
+        <v>1125.35</v>
+      </c>
+      <c r="L35">
+        <v>1040.88</v>
+      </c>
+      <c r="M35">
+        <v>1294.29</v>
+      </c>
+      <c r="N35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="C34" t="s">
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36">
+        <v>26.69</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36">
+        <v>33.92</v>
+      </c>
+      <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>89</v>
+      </c>
+      <c r="K36">
+        <v>1711.9</v>
+      </c>
+      <c r="L36">
+        <v>1678.83</v>
+      </c>
+      <c r="M36">
+        <v>1778.03</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37">
+        <v>25.3</v>
+      </c>
+      <c r="E37">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G37">
+        <v>31.33</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K37">
+        <v>1212.1</v>
+      </c>
+      <c r="L37">
+        <v>1142.59</v>
+      </c>
+      <c r="M37">
+        <v>1351.13</v>
+      </c>
+      <c r="N37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38">
+        <v>24.1</v>
+      </c>
+      <c r="E38">
+        <v>73</v>
+      </c>
+      <c r="F38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38">
+        <v>61.99</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>89</v>
+      </c>
+      <c r="K38">
+        <v>16774</v>
+      </c>
+      <c r="L38">
+        <v>16117.29</v>
+      </c>
+      <c r="M38">
+        <v>18087.43</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39">
+        <v>22.89</v>
+      </c>
+      <c r="E39">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39">
+        <v>22.89</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39">
+        <v>2493</v>
+      </c>
+      <c r="L39">
+        <v>2339.77</v>
+      </c>
+      <c r="M39">
+        <v>2799.46</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40">
+        <v>21.69</v>
+      </c>
+      <c r="E40">
+        <v>36</v>
+      </c>
+      <c r="F40" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40">
+        <v>43.37</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>89</v>
+      </c>
+      <c r="K40">
+        <v>1509.2</v>
+      </c>
+      <c r="L40">
+        <v>1419.43</v>
+      </c>
+      <c r="M40">
+        <v>1688.74</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41">
+        <v>16.87</v>
+      </c>
+      <c r="E41">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41">
+        <v>16.87</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41" t="s">
+        <v>89</v>
+      </c>
+      <c r="K41">
+        <v>1207.6</v>
+      </c>
+      <c r="L41">
+        <v>1168.18</v>
+      </c>
+      <c r="M41">
+        <v>1286.44</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42">
+        <v>14.46</v>
+      </c>
+      <c r="E42">
+        <v>52</v>
+      </c>
+      <c r="F42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42">
+        <v>21.69</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42">
+        <v>5081.9</v>
+      </c>
+      <c r="L42">
+        <v>4916.12</v>
+      </c>
+      <c r="M42">
+        <v>5413.45</v>
+      </c>
+      <c r="N42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43">
+        <v>13.25</v>
+      </c>
+      <c r="E43">
+        <v>47</v>
+      </c>
+      <c r="F43" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43">
+        <v>63.86</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>89</v>
+      </c>
+      <c r="K43">
+        <v>2451.8</v>
+      </c>
+      <c r="L43">
+        <v>2414.24</v>
+      </c>
+      <c r="M43">
+        <v>2526.92</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44">
+        <v>10.84</v>
+      </c>
+      <c r="E44">
+        <v>21</v>
+      </c>
+      <c r="F44" t="s">
+        <v>84</v>
+      </c>
+      <c r="G44">
+        <v>15.66</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>89</v>
+      </c>
+      <c r="K44">
+        <v>3485.8</v>
+      </c>
+      <c r="L44">
+        <v>3356.66</v>
+      </c>
+      <c r="M44">
+        <v>3744.09</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45">
+        <v>10.84</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45">
+        <v>19.28</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>89</v>
+      </c>
+      <c r="K45">
+        <v>1295.4</v>
+      </c>
+      <c r="L45">
+        <v>1263.72</v>
+      </c>
+      <c r="M45">
+        <v>1358.76</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
         <v>58</v>
       </c>
-      <c r="D34">
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="E46">
+        <v>28</v>
+      </c>
+      <c r="F46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G46">
+        <v>31.33</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>89</v>
+      </c>
+      <c r="K46">
+        <v>7459</v>
+      </c>
+      <c r="L46">
+        <v>7272.64</v>
+      </c>
+      <c r="M46">
+        <v>7831.71</v>
+      </c>
+      <c r="N46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>76</v>
+      </c>
+      <c r="G47">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47">
+        <v>4245.4</v>
+      </c>
+      <c r="L47">
+        <v>4070.26</v>
+      </c>
+      <c r="M47">
+        <v>4595.68</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48">
         <v>4.82</v>
       </c>
-      <c r="E34">
-        <v>29</v>
-      </c>
-      <c r="F34" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34">
-        <v>10.84</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>75</v>
-      </c>
-      <c r="K34">
-        <v>1708.5</v>
-      </c>
-      <c r="L34">
-        <v>1665.06</v>
-      </c>
-      <c r="M34">
-        <v>1795.38</v>
-      </c>
-      <c r="N34">
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>76</v>
+      </c>
+      <c r="G48">
+        <v>14.46</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48">
+        <v>996</v>
+      </c>
+      <c r="L48">
+        <v>967.0599999999999</v>
+      </c>
+      <c r="M48">
+        <v>1053.88</v>
+      </c>
+      <c r="N48">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix hourly tracker services and add orange theme to dashboards
- Fixed hourly tracker service initialization issues with Kite API
- Created hourly_tracker_service_fixed.py with proper config loading
- Updated hourly_tracker_dashboard.py regex pattern to match service logs
- Created new hourly short tracker service for Short_Reversal_Hourly
- Created hourly short tracker dashboard at port 3004
- Updated dashboard_manager.py to include port 3004
- Added both hourly services to job_manager_dashboard.py
- Changed color scheme from red/green to orange for dashboards 3003 & 3004
- Fixed NaN JSON error in short momentum dashboard
- Updated Activity.md with all changes

Services:
- hourly_tracker_service_fixed.py (long positions)
- hourly_short_tracker_service.py (short positions)

Dashboards:
- Port 3002: Hourly tracker (long)
- Port 3003: Short momentum (orange theme)
- Port 3004: Hourly short tracker (orange theme)
- Port 9090: Job manager (updated with new services)
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="109">
   <si>
     <t>Ticker</t>
   </si>
@@ -58,154 +58,205 @@
     <t>Risk_Reward</t>
   </si>
   <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>AMBER</t>
+  </si>
+  <si>
     <t>TORNTPHARM</t>
   </si>
   <si>
     <t>CIPLA</t>
   </si>
   <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>COROMANDEL</t>
+  </si>
+  <si>
+    <t>TATACHEM</t>
+  </si>
+  <si>
+    <t>EIDPARRY</t>
+  </si>
+  <si>
+    <t>SUMICHEM</t>
+  </si>
+  <si>
+    <t>CRAFTSMAN</t>
+  </si>
+  <si>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>GATEWAY</t>
+  </si>
+  <si>
     <t>LAURUSLABS</t>
   </si>
   <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>SYRMA</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>ETERNAL</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>UPL</t>
+  </si>
+  <si>
     <t>GLAND</t>
   </si>
   <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
-    <t>AMBER</t>
-  </si>
-  <si>
-    <t>PPLPHARMA</t>
-  </si>
-  <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>PAYTM</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>TATACHEM</t>
-  </si>
-  <si>
-    <t>STLTECH</t>
-  </si>
-  <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
-    <t>OLECTRA</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
-  </si>
-  <si>
-    <t>ETERNAL</t>
-  </si>
-  <si>
     <t>ANANDRATHI</t>
   </si>
   <si>
-    <t>HDFCAMC</t>
+    <t>PATANJALI</t>
+  </si>
+  <si>
+    <t>JGCHEM</t>
   </si>
   <si>
     <t>AGI</t>
   </si>
   <si>
-    <t>UPL</t>
-  </si>
-  <si>
-    <t>SUMICHEM</t>
-  </si>
-  <si>
     <t>NUVOCO</t>
   </si>
   <si>
-    <t>ASIANPAINT</t>
-  </si>
-  <si>
-    <t>RAMCOCEM</t>
+    <t>PCBL</t>
+  </si>
+  <si>
+    <t>EPACK</t>
+  </si>
+  <si>
+    <t>VIPIND</t>
+  </si>
+  <si>
+    <t>METROPOLIS</t>
   </si>
   <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
-    <t>AJANTPHARM</t>
+    <t>NMDC</t>
   </si>
   <si>
     <t>AMBUJACEM</t>
   </si>
   <si>
+    <t>STARHEALTH</t>
+  </si>
+  <si>
+    <t>GODFRYPHLP</t>
+  </si>
+  <si>
+    <t>VISHNU</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>POWERINDIA</t>
+  </si>
+  <si>
+    <t>DBL</t>
+  </si>
+  <si>
+    <t>PIIND</t>
+  </si>
+  <si>
+    <t>PAGEIND</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>SUNPHARMA</t>
+  </si>
+  <si>
     <t>APARINDS</t>
   </si>
   <si>
-    <t>JAGSNPHARM</t>
-  </si>
-  <si>
     <t>JBCHEPHARM</t>
   </si>
   <si>
-    <t>VIJAYA</t>
-  </si>
-  <si>
-    <t>SUNPHARMA</t>
-  </si>
-  <si>
-    <t>EIDPARRY</t>
+    <t>BSOFT</t>
+  </si>
+  <si>
+    <t>PGHH</t>
+  </si>
+  <si>
+    <t>MPHASIS</t>
+  </si>
+  <si>
+    <t>NIACL</t>
+  </si>
+  <si>
+    <t>HEG</t>
+  </si>
+  <si>
+    <t>AUBANK</t>
+  </si>
+  <si>
+    <t>EICHERMOT</t>
+  </si>
+  <si>
+    <t>GPIL</t>
+  </si>
+  <si>
+    <t>BERGEPAINT</t>
+  </si>
+  <si>
+    <t>FLUOROCHEM</t>
+  </si>
+  <si>
+    <t>ERIS</t>
+  </si>
+  <si>
+    <t>LALPATHLAB</t>
+  </si>
+  <si>
+    <t>DMART</t>
   </si>
   <si>
     <t>DIXON</t>
   </si>
   <si>
-    <t>COROMANDEL</t>
-  </si>
-  <si>
-    <t>BIRLACORPN</t>
-  </si>
-  <si>
-    <t>INDIGOPNTS</t>
-  </si>
-  <si>
-    <t>ALKEM</t>
-  </si>
-  <si>
-    <t>HINDUNILVR</t>
-  </si>
-  <si>
-    <t>ESCORTS</t>
-  </si>
-  <si>
-    <t>DRREDDY</t>
-  </si>
-  <si>
-    <t>APOLLOHOSP</t>
-  </si>
-  <si>
-    <t>PIIND</t>
+    <t>DABUR</t>
+  </si>
+  <si>
+    <t>CESC</t>
+  </si>
+  <si>
+    <t>GMMPFAUDLR</t>
   </si>
   <si>
     <t>ZYDUSLIFE</t>
   </si>
   <si>
+    <t>Consumer Cyclical</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
     <t>Healthcare</t>
   </si>
   <si>
-    <t>Consumer Cyclical</t>
+    <t>Basic Materials</t>
   </si>
   <si>
     <t>Industrials</t>
@@ -214,13 +265,13 @@
     <t>Financial Services</t>
   </si>
   <si>
-    <t>Basic Materials</t>
+    <t>Consumer Defensive</t>
   </si>
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Consumer Defensive</t>
+    <t>Utilities</t>
   </si>
   <si>
     <t>Building_G</t>
@@ -238,37 +289,43 @@
     <t>Early_Setup</t>
   </si>
   <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
     <t>2025-07-15</t>
   </si>
   <si>
     <t>2025-07-25</t>
   </si>
   <si>
-    <t>2025-07-07</t>
+    <t>2025-07-29</t>
+  </si>
+  <si>
+    <t>2025-07-22</t>
   </si>
   <si>
     <t>2025-07-16</t>
   </si>
   <si>
+    <t>2025-07-30</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
     <t>2025-07-11</t>
   </si>
   <si>
-    <t>2025-07-22</t>
-  </si>
-  <si>
-    <t>2025-07-08</t>
+    <t>2025-07-09</t>
   </si>
   <si>
     <t>2025-07-21</t>
   </si>
   <si>
-    <t>2025-07-09</t>
-  </si>
-  <si>
-    <t>2025-07-29</t>
-  </si>
-  <si>
     <t>2025-07-18</t>
+  </si>
+  <si>
+    <t>2025-07-17</t>
   </si>
   <si>
     <t>G PATTERN DEVELOPING - DOUBLE POSITION (50%)</t>
@@ -641,7 +698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -696,19 +753,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>97.11</v>
       </c>
       <c r="E2">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -720,16 +777,16 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="K2">
-        <v>3760.4</v>
+        <v>40395</v>
       </c>
       <c r="L2">
-        <v>3618.31</v>
+        <v>38442.86</v>
       </c>
       <c r="M2">
-        <v>4044.57</v>
+        <v>44299.29</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -740,40 +797,40 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D3">
-        <v>53.01</v>
+        <v>64.04000000000001</v>
       </c>
       <c r="E3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>79.04000000000001</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="K3">
-        <v>1575.7</v>
+        <v>8012.5</v>
       </c>
       <c r="L3">
-        <v>1522</v>
+        <v>7452.29</v>
       </c>
       <c r="M3">
-        <v>1683.1</v>
+        <v>9132.93</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -784,40 +841,40 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D4">
-        <v>68.01000000000001</v>
+        <v>54.22</v>
       </c>
       <c r="E4">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G4">
-        <v>68.01000000000001</v>
+        <v>100</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="K4">
-        <v>909.65</v>
+        <v>3739</v>
       </c>
       <c r="L4">
-        <v>864.53</v>
+        <v>3593.57</v>
       </c>
       <c r="M4">
-        <v>999.89</v>
+        <v>4029.86</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -828,40 +885,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D5">
-        <v>66.81</v>
+        <v>49.4</v>
       </c>
       <c r="E5">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="G5">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="K5">
-        <v>2086.8</v>
+        <v>1560.2</v>
       </c>
       <c r="L5">
-        <v>1959.29</v>
+        <v>1507.49</v>
       </c>
       <c r="M5">
-        <v>2341.83</v>
+        <v>1665.63</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -872,19 +929,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D6">
-        <v>64.40000000000001</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="E6">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G6">
         <v>100</v>
@@ -893,19 +950,19 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="K6">
-        <v>39805</v>
+        <v>722.55</v>
       </c>
       <c r="L6">
-        <v>37945.71</v>
+        <v>680.96</v>
       </c>
       <c r="M6">
-        <v>43523.57</v>
+        <v>805.74</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -916,40 +973,40 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="D7">
-        <v>50.96</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="E7">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="G7">
-        <v>79.04000000000001</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="K7">
-        <v>7789</v>
+        <v>2612.6</v>
       </c>
       <c r="L7">
-        <v>7255.81</v>
+        <v>2446.41</v>
       </c>
       <c r="M7">
-        <v>8855.379999999999</v>
+        <v>2944.97</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -960,40 +1017,40 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D8">
-        <v>38.92</v>
+        <v>55.96</v>
       </c>
       <c r="E8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="G8">
-        <v>82.65000000000001</v>
+        <v>75.23999999999999</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="K8">
-        <v>205.98</v>
+        <v>1006.1</v>
       </c>
       <c r="L8">
-        <v>202.31</v>
+        <v>950.14</v>
       </c>
       <c r="M8">
-        <v>213.31</v>
+        <v>1118.01</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1004,40 +1061,40 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D9">
-        <v>38.55</v>
+        <v>53.55</v>
       </c>
       <c r="E9">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>53.55</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="K9">
-        <v>507</v>
+        <v>1227.4</v>
       </c>
       <c r="L9">
-        <v>483.79</v>
+        <v>1158.96</v>
       </c>
       <c r="M9">
-        <v>553.4299999999999</v>
+        <v>1364.29</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1048,40 +1105,40 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D10">
-        <v>37.35</v>
+        <v>94.88</v>
       </c>
       <c r="E10">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G10">
         <v>100</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K10">
-        <v>512.8</v>
+        <v>638.5</v>
       </c>
       <c r="L10">
-        <v>456.33</v>
+        <v>596.04</v>
       </c>
       <c r="M10">
-        <v>625.74</v>
+        <v>723.4299999999999</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1092,40 +1149,40 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D11">
-        <v>37.35</v>
+        <v>94.88</v>
       </c>
       <c r="E11">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G11">
         <v>100</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K11">
-        <v>1070.05</v>
+        <v>6796</v>
       </c>
       <c r="L11">
-        <v>990.41</v>
+        <v>6325.43</v>
       </c>
       <c r="M11">
-        <v>1229.34</v>
+        <v>7737.14</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1136,22 +1193,22 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D12">
-        <v>37.35</v>
+        <v>92.47</v>
       </c>
       <c r="E12">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G12">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1160,16 +1217,16 @@
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K12">
-        <v>851.4</v>
+        <v>521.35</v>
       </c>
       <c r="L12">
-        <v>810.89</v>
+        <v>495.26</v>
       </c>
       <c r="M12">
-        <v>932.41</v>
+        <v>573.54</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1180,40 +1237,40 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D13">
-        <v>36.14</v>
+        <v>91.27</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="G13">
-        <v>75.23999999999999</v>
+        <v>91.27</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K13">
-        <v>999</v>
+        <v>73.09</v>
       </c>
       <c r="L13">
-        <v>946.11</v>
+        <v>68.45</v>
       </c>
       <c r="M13">
-        <v>1104.77</v>
+        <v>82.38</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1224,40 +1281,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D14">
-        <v>36.14</v>
+        <v>38.55</v>
       </c>
       <c r="E14">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G14">
-        <v>77.83</v>
+        <v>89.88</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K14">
-        <v>128.23</v>
+        <v>887.75</v>
       </c>
       <c r="L14">
-        <v>114.48</v>
+        <v>839.9400000000001</v>
       </c>
       <c r="M14">
-        <v>155.74</v>
+        <v>983.38</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1268,19 +1325,19 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D15">
-        <v>34.94</v>
+        <v>37.35</v>
       </c>
       <c r="E15">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -1289,19 +1346,19 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K15">
-        <v>972</v>
+        <v>986.45</v>
       </c>
       <c r="L15">
-        <v>919.59</v>
+        <v>930.16</v>
       </c>
       <c r="M15">
-        <v>1076.81</v>
+        <v>1099.04</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1312,19 +1369,19 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D16">
-        <v>32.53</v>
+        <v>31.33</v>
       </c>
       <c r="E16">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G16">
         <v>100</v>
@@ -1333,19 +1390,19 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K16">
-        <v>709.55</v>
+        <v>753.2</v>
       </c>
       <c r="L16">
-        <v>669.36</v>
+        <v>695.8099999999999</v>
       </c>
       <c r="M16">
-        <v>789.92</v>
+        <v>867.99</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1356,40 +1413,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17">
+        <v>30.12</v>
+      </c>
+      <c r="E17">
         <v>73</v>
       </c>
-      <c r="D17">
-        <v>31.33</v>
-      </c>
-      <c r="E17">
-        <v>48</v>
-      </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G17">
-        <v>90.06</v>
+        <v>100</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K17">
-        <v>1434.3</v>
+        <v>494</v>
       </c>
       <c r="L17">
-        <v>1307.5</v>
+        <v>433.16</v>
       </c>
       <c r="M17">
-        <v>1687.9</v>
+        <v>615.6900000000001</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1400,40 +1457,40 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D18">
-        <v>31.33</v>
+        <v>24.1</v>
       </c>
       <c r="E18">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="G18">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K18">
-        <v>747.5</v>
+        <v>306.8</v>
       </c>
       <c r="L18">
-        <v>687.65</v>
+        <v>285.73</v>
       </c>
       <c r="M18">
-        <v>867.2</v>
+        <v>348.94</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1444,40 +1501,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D19">
-        <v>24.1</v>
+        <v>21.69</v>
       </c>
       <c r="E19">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="G19">
-        <v>92.47</v>
+        <v>82.83</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K19">
-        <v>305.5</v>
+        <v>837.6</v>
       </c>
       <c r="L19">
-        <v>284.46</v>
+        <v>802.6</v>
       </c>
       <c r="M19">
-        <v>347.59</v>
+        <v>907.61</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1488,40 +1545,40 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D20">
-        <v>22.89</v>
+        <v>20.48</v>
       </c>
       <c r="E20">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="G20">
-        <v>96.08</v>
+        <v>100</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K20">
-        <v>2677.7</v>
+        <v>5661.5</v>
       </c>
       <c r="L20">
-        <v>2460.51</v>
+        <v>5426.36</v>
       </c>
       <c r="M20">
-        <v>3112.07</v>
+        <v>6131.79</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1532,40 +1589,40 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>22.89</v>
+        <v>19.28</v>
       </c>
       <c r="E21">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K21">
-        <v>5630.5</v>
+        <v>721.95</v>
       </c>
       <c r="L21">
-        <v>5396.07</v>
+        <v>690.23</v>
       </c>
       <c r="M21">
-        <v>6099.36</v>
+        <v>785.39</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1576,40 +1633,40 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D22">
-        <v>20.48</v>
+        <v>16.87</v>
       </c>
       <c r="E22">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K22">
-        <v>960</v>
+        <v>2065.3</v>
       </c>
       <c r="L22">
-        <v>872.34</v>
+        <v>1929.87</v>
       </c>
       <c r="M22">
-        <v>1135.33</v>
+        <v>2336.16</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1620,40 +1677,40 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D23">
-        <v>19.28</v>
+        <v>16.87</v>
       </c>
       <c r="E23">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G23">
-        <v>85.23999999999999</v>
+        <v>96.08</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K23">
-        <v>725.8</v>
+        <v>2686.4</v>
       </c>
       <c r="L23">
-        <v>693.4400000000001</v>
+        <v>2464.09</v>
       </c>
       <c r="M23">
-        <v>790.51</v>
+        <v>3131.03</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1664,19 +1721,19 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D24">
-        <v>15.66</v>
+        <v>14.46</v>
       </c>
       <c r="E24">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="G24">
         <v>100</v>
@@ -1688,16 +1745,16 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K24">
-        <v>606.5</v>
+        <v>1902</v>
       </c>
       <c r="L24">
-        <v>568.04</v>
+        <v>1797.45</v>
       </c>
       <c r="M24">
-        <v>683.41</v>
+        <v>2111.1</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1708,40 +1765,40 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D25">
         <v>14.46</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="G25">
-        <v>84.04000000000001</v>
+        <v>86.45</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K25">
-        <v>414.55</v>
+        <v>501.8</v>
       </c>
       <c r="L25">
-        <v>383.2</v>
+        <v>468.74</v>
       </c>
       <c r="M25">
-        <v>477.25</v>
+        <v>567.9299999999999</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1752,40 +1809,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D26">
         <v>14.46</v>
       </c>
       <c r="E26">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G26">
-        <v>91.27</v>
+        <v>100</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K26">
-        <v>2408.2</v>
+        <v>962.75</v>
       </c>
       <c r="L26">
-        <v>2355.82</v>
+        <v>875.5700000000001</v>
       </c>
       <c r="M26">
-        <v>2512.96</v>
+        <v>1137.11</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1796,22 +1853,22 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D27">
         <v>14.46</v>
       </c>
       <c r="E27">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="G27">
-        <v>70.42</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -1820,16 +1877,16 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K27">
-        <v>1190.5</v>
+        <v>418.55</v>
       </c>
       <c r="L27">
-        <v>1121.95</v>
+        <v>387.16</v>
       </c>
       <c r="M27">
-        <v>1327.61</v>
+        <v>481.32</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1840,43 +1897,43 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D28">
         <v>13.25</v>
       </c>
       <c r="E28">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="G28">
-        <v>100</v>
+        <v>70.78</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K28">
-        <v>984.6</v>
+        <v>394.2</v>
       </c>
       <c r="L28">
-        <v>953.59</v>
+        <v>399.29</v>
       </c>
       <c r="M28">
-        <v>1046.62</v>
+        <v>384.01</v>
       </c>
       <c r="N28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1884,40 +1941,40 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D29">
-        <v>12.05</v>
+        <v>13.25</v>
       </c>
       <c r="E29">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="G29">
-        <v>100</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K29">
-        <v>397.15</v>
+        <v>370.35</v>
       </c>
       <c r="L29">
-        <v>379.05</v>
+        <v>354.18</v>
       </c>
       <c r="M29">
-        <v>433.36</v>
+        <v>402.69</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -1928,40 +1985,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D30">
-        <v>12.05</v>
+        <v>13.25</v>
       </c>
       <c r="E30">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="G30">
-        <v>93.48999999999999</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K30">
-        <v>2825</v>
+        <v>464.45</v>
       </c>
       <c r="L30">
-        <v>2676.41</v>
+        <v>440.62</v>
       </c>
       <c r="M30">
-        <v>3122.19</v>
+        <v>512.12</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -1972,40 +2029,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D31">
-        <v>7.23</v>
+        <v>12.05</v>
       </c>
       <c r="E31">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>72.29000000000001</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="K31">
-        <v>609</v>
+        <v>2020.5</v>
       </c>
       <c r="L31">
-        <v>593.84</v>
+        <v>1890.26</v>
       </c>
       <c r="M31">
-        <v>639.3200000000001</v>
+        <v>2280.98</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2016,40 +2073,40 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D32">
-        <v>42.17</v>
+        <v>10.84</v>
       </c>
       <c r="E32">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
       <c r="G32">
-        <v>44.58</v>
+        <v>100</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="K32">
-        <v>9751.5</v>
+        <v>981.75</v>
       </c>
       <c r="L32">
-        <v>9033.57</v>
+        <v>955.4</v>
       </c>
       <c r="M32">
-        <v>11187.36</v>
+        <v>1034.46</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2060,40 +2117,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D33">
-        <v>34.94</v>
+        <v>8.43</v>
       </c>
       <c r="E33">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="G33">
-        <v>68.01000000000001</v>
+        <v>81.27</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="K33">
-        <v>285.27</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="L33">
-        <v>250.89</v>
+        <v>70.03</v>
       </c>
       <c r="M33">
-        <v>354.03</v>
+        <v>75.91</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2104,40 +2161,40 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D34">
-        <v>33.73</v>
+        <v>7.23</v>
       </c>
       <c r="E34">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="G34">
-        <v>33.73</v>
+        <v>100</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="K34">
-        <v>1797</v>
+        <v>617.75</v>
       </c>
       <c r="L34">
-        <v>1731.7</v>
+        <v>597.6900000000001</v>
       </c>
       <c r="M34">
-        <v>1927.6</v>
+        <v>657.86</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2148,40 +2205,40 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D35">
-        <v>31.33</v>
+        <v>44.94</v>
       </c>
       <c r="E35">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="G35">
-        <v>45.78</v>
+        <v>44.94</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="K35">
-        <v>1125.35</v>
+        <v>445.5</v>
       </c>
       <c r="L35">
-        <v>1040.88</v>
+        <v>426.18</v>
       </c>
       <c r="M35">
-        <v>1294.29</v>
+        <v>484.15</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2192,40 +2249,40 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="D36">
-        <v>26.69</v>
+        <v>40.12</v>
       </c>
       <c r="E36">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="G36">
-        <v>33.92</v>
+        <v>90.06</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="K36">
-        <v>1711.9</v>
+        <v>9434.5</v>
       </c>
       <c r="L36">
-        <v>1678.83</v>
+        <v>8740.809999999999</v>
       </c>
       <c r="M36">
-        <v>1778.03</v>
+        <v>10821.89</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2236,40 +2293,40 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D37">
-        <v>25.3</v>
+        <v>91.27</v>
       </c>
       <c r="E37">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="G37">
-        <v>31.33</v>
+        <v>91.27</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K37">
-        <v>1212.1</v>
+        <v>579.6</v>
       </c>
       <c r="L37">
-        <v>1142.59</v>
+        <v>540.95</v>
       </c>
       <c r="M37">
-        <v>1351.13</v>
+        <v>656.9</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2280,40 +2337,40 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D38">
-        <v>24.1</v>
+        <v>82.83</v>
       </c>
       <c r="E38">
-        <v>73</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="G38">
-        <v>61.99</v>
+        <v>82.83</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K38">
-        <v>16774</v>
+        <v>3660.1</v>
       </c>
       <c r="L38">
-        <v>16117.29</v>
+        <v>3544.04</v>
       </c>
       <c r="M38">
-        <v>18087.43</v>
+        <v>3892.21</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2324,40 +2381,40 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D39">
-        <v>22.89</v>
+        <v>53.37</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="G39">
-        <v>22.89</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K39">
-        <v>2493</v>
+        <v>20810</v>
       </c>
       <c r="L39">
-        <v>2339.77</v>
+        <v>19117.86</v>
       </c>
       <c r="M39">
-        <v>2799.46</v>
+        <v>24194.29</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2368,40 +2425,40 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D40">
-        <v>21.69</v>
+        <v>38.92</v>
       </c>
       <c r="E40">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="G40">
-        <v>43.37</v>
+        <v>38.92</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K40">
-        <v>1509.2</v>
+        <v>485.55</v>
       </c>
       <c r="L40">
-        <v>1419.43</v>
+        <v>479.65</v>
       </c>
       <c r="M40">
-        <v>1688.74</v>
+        <v>497.35</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2412,40 +2469,40 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D41">
-        <v>16.87</v>
+        <v>38.55</v>
       </c>
       <c r="E41">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G41">
-        <v>16.87</v>
+        <v>38.55</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K41">
-        <v>1207.6</v>
+        <v>4319.4</v>
       </c>
       <c r="L41">
-        <v>1168.18</v>
+        <v>4129.06</v>
       </c>
       <c r="M41">
-        <v>1286.44</v>
+        <v>4700.09</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2456,40 +2513,40 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="D42">
-        <v>14.46</v>
+        <v>35.3</v>
       </c>
       <c r="E42">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="G42">
-        <v>21.69</v>
+        <v>35.3</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K42">
-        <v>5081.9</v>
+        <v>48515</v>
       </c>
       <c r="L42">
-        <v>4916.12</v>
+        <v>46848.16</v>
       </c>
       <c r="M42">
-        <v>5413.45</v>
+        <v>51848.67</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2500,40 +2557,40 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="D43">
-        <v>13.25</v>
+        <v>34.1</v>
       </c>
       <c r="E43">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="G43">
-        <v>63.86</v>
+        <v>34.1</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K43">
-        <v>2451.8</v>
+        <v>378.1</v>
       </c>
       <c r="L43">
-        <v>2414.24</v>
+        <v>368.79</v>
       </c>
       <c r="M43">
-        <v>2526.92</v>
+        <v>396.72</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2544,40 +2601,40 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D44">
-        <v>10.84</v>
+        <v>33.92</v>
       </c>
       <c r="E44">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G44">
-        <v>15.66</v>
+        <v>33.92</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K44">
-        <v>3485.8</v>
+        <v>1738.6</v>
       </c>
       <c r="L44">
-        <v>3356.66</v>
+        <v>1691.13</v>
       </c>
       <c r="M44">
-        <v>3744.09</v>
+        <v>1833.54</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2588,40 +2645,40 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D45">
-        <v>10.84</v>
+        <v>31.33</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F45" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="G45">
-        <v>19.28</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J45" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K45">
-        <v>1295.4</v>
+        <v>9560</v>
       </c>
       <c r="L45">
-        <v>1263.72</v>
+        <v>8808.57</v>
       </c>
       <c r="M45">
-        <v>1358.76</v>
+        <v>11062.86</v>
       </c>
       <c r="N45">
         <v>2</v>
@@ -2632,40 +2689,40 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D46">
-        <v>9.640000000000001</v>
+        <v>30.12</v>
       </c>
       <c r="E46">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F46" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="G46">
-        <v>31.33</v>
+        <v>38.55</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K46">
-        <v>7459</v>
+        <v>1792.5</v>
       </c>
       <c r="L46">
-        <v>7272.64</v>
+        <v>1727.07</v>
       </c>
       <c r="M46">
-        <v>7831.71</v>
+        <v>1923.36</v>
       </c>
       <c r="N46">
         <v>2</v>
@@ -2676,40 +2733,40 @@
         <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D47">
-        <v>9.640000000000001</v>
+        <v>26.51</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="G47">
-        <v>9.640000000000001</v>
+        <v>26.51</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="K47">
-        <v>4245.4</v>
+        <v>418.6</v>
       </c>
       <c r="L47">
-        <v>4070.26</v>
+        <v>408.29</v>
       </c>
       <c r="M47">
-        <v>4595.68</v>
+        <v>439.22</v>
       </c>
       <c r="N47">
         <v>2</v>
@@ -2720,42 +2777,746 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48">
+        <v>25.3</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>103</v>
+      </c>
+      <c r="G48">
+        <v>25.3</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>108</v>
+      </c>
+      <c r="K48">
+        <v>13350</v>
+      </c>
+      <c r="L48">
+        <v>13115.74</v>
+      </c>
+      <c r="M48">
+        <v>13818.52</v>
+      </c>
+      <c r="N48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" t="s">
         <v>61</v>
       </c>
-      <c r="C48" t="s">
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49">
+        <v>25.3</v>
+      </c>
+      <c r="E49">
+        <v>18</v>
+      </c>
+      <c r="F49" t="s">
+        <v>91</v>
+      </c>
+      <c r="G49">
+        <v>25.3</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49" t="s">
+        <v>108</v>
+      </c>
+      <c r="K49">
+        <v>2817</v>
+      </c>
+      <c r="L49">
+        <v>2722.56</v>
+      </c>
+      <c r="M49">
+        <v>3005.88</v>
+      </c>
+      <c r="N49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50">
+        <v>22.89</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>97</v>
+      </c>
+      <c r="G50">
+        <v>22.89</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50" t="s">
+        <v>108</v>
+      </c>
+      <c r="K50">
+        <v>191.46</v>
+      </c>
+      <c r="L50">
+        <v>181.22</v>
+      </c>
+      <c r="M50">
+        <v>211.94</v>
+      </c>
+      <c r="N50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51">
+        <v>19.28</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+      <c r="F51" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51">
+        <v>39.76</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>108</v>
+      </c>
+      <c r="K51">
+        <v>530.2</v>
+      </c>
+      <c r="L51">
+        <v>512.74</v>
+      </c>
+      <c r="M51">
+        <v>565.13</v>
+      </c>
+      <c r="N51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52">
+        <v>19.28</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52">
+        <v>19.28</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52" t="s">
+        <v>108</v>
+      </c>
+      <c r="K52">
+        <v>749.5</v>
+      </c>
+      <c r="L52">
+        <v>757.0599999999999</v>
+      </c>
+      <c r="M52">
+        <v>734.39</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53">
+        <v>19.28</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53">
+        <v>19.28</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>108</v>
+      </c>
+      <c r="K53">
+        <v>5527</v>
+      </c>
+      <c r="L53">
+        <v>5481.89</v>
+      </c>
+      <c r="M53">
+        <v>5617.21</v>
+      </c>
+      <c r="N53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54">
+        <v>15.66</v>
+      </c>
+      <c r="E54">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G54">
+        <v>26.51</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54" t="s">
+        <v>108</v>
+      </c>
+      <c r="K54">
+        <v>196.6</v>
+      </c>
+      <c r="L54">
+        <v>187.5</v>
+      </c>
+      <c r="M54">
+        <v>214.81</v>
+      </c>
+      <c r="N54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55">
+        <v>14.46</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>91</v>
+      </c>
+      <c r="G55">
+        <v>14.46</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>108</v>
+      </c>
+      <c r="K55">
+        <v>577.35</v>
+      </c>
+      <c r="L55">
+        <v>564.6</v>
+      </c>
+      <c r="M55">
+        <v>602.86</v>
+      </c>
+      <c r="N55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56">
+        <v>14.46</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56">
+        <v>20.48</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>108</v>
+      </c>
+      <c r="K56">
+        <v>3570.6</v>
+      </c>
+      <c r="L56">
+        <v>3477.36</v>
+      </c>
+      <c r="M56">
+        <v>3757.08</v>
+      </c>
+      <c r="N56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57">
+        <v>13.25</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G57">
+        <v>13.25</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>108</v>
+      </c>
+      <c r="K57">
+        <v>1835</v>
+      </c>
+      <c r="L57">
+        <v>1731</v>
+      </c>
+      <c r="M57">
+        <v>2043.01</v>
+      </c>
+      <c r="N57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58">
+        <v>12.05</v>
+      </c>
+      <c r="E58">
+        <v>38</v>
+      </c>
+      <c r="F58" t="s">
+        <v>100</v>
+      </c>
+      <c r="G58">
+        <v>58.19</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>108</v>
+      </c>
+      <c r="K58">
+        <v>3098.5</v>
+      </c>
+      <c r="L58">
+        <v>2942.52</v>
+      </c>
+      <c r="M58">
+        <v>3410.46</v>
+      </c>
+      <c r="N58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59">
+        <v>12.05</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>97</v>
+      </c>
+      <c r="G59">
+        <v>12.05</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>108</v>
+      </c>
+      <c r="K59">
+        <v>4207.4</v>
+      </c>
+      <c r="L59">
+        <v>4045.1</v>
+      </c>
+      <c r="M59">
+        <v>4532</v>
+      </c>
+      <c r="N59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60">
+        <v>12.05</v>
+      </c>
+      <c r="E60">
+        <v>78</v>
+      </c>
+      <c r="F60" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60">
+        <v>61.99</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>108</v>
+      </c>
+      <c r="K60">
+        <v>16789</v>
+      </c>
+      <c r="L60">
+        <v>16137.57</v>
+      </c>
+      <c r="M60">
+        <v>18091.86</v>
+      </c>
+      <c r="N60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
         <v>73</v>
       </c>
-      <c r="D48">
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="E61">
+        <v>43</v>
+      </c>
+      <c r="F61" t="s">
+        <v>91</v>
+      </c>
+      <c r="G61">
+        <v>60.24</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61" t="s">
+        <v>108</v>
+      </c>
+      <c r="K61">
+        <v>522.3</v>
+      </c>
+      <c r="L61">
+        <v>508.85</v>
+      </c>
+      <c r="M61">
+        <v>549.2</v>
+      </c>
+      <c r="N61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62">
+        <v>8.43</v>
+      </c>
+      <c r="E62">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
+        <v>91</v>
+      </c>
+      <c r="G62">
+        <v>16.87</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>108</v>
+      </c>
+      <c r="K62">
+        <v>178.66</v>
+      </c>
+      <c r="L62">
+        <v>174.62</v>
+      </c>
+      <c r="M62">
+        <v>186.73</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63">
         <v>4.82</v>
       </c>
-      <c r="E48">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E63">
+        <v>27</v>
+      </c>
+      <c r="F63" t="s">
+        <v>91</v>
+      </c>
+      <c r="G63">
+        <v>39.76</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>108</v>
+      </c>
+      <c r="K63">
+        <v>1334.8</v>
+      </c>
+      <c r="L63">
+        <v>1270.45</v>
+      </c>
+      <c r="M63">
+        <v>1463.49</v>
+      </c>
+      <c r="N63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" t="s">
         <v>76</v>
       </c>
-      <c r="G48">
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64">
+        <v>4.82</v>
+      </c>
+      <c r="E64">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>91</v>
+      </c>
+      <c r="G64">
         <v>14.46</v>
       </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48" t="s">
-        <v>89</v>
-      </c>
-      <c r="K48">
-        <v>996</v>
-      </c>
-      <c r="L48">
-        <v>967.0599999999999</v>
-      </c>
-      <c r="M48">
-        <v>1053.88</v>
-      </c>
-      <c r="N48">
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>108</v>
+      </c>
+      <c r="K64">
+        <v>996.05</v>
+      </c>
+      <c r="L64">
+        <v>969.08</v>
+      </c>
+      <c r="M64">
+        <v>1049.98</v>
+      </c>
+      <c r="N64">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix July 30 volume data and correct volume participation values
- Fixed July 30 volume breadth showing as 0 (now 14.17%)
- Corrected volume participation calculation for July 28-30
- Volume participation = high_volume/total_stocks (as ratio)
- July 28: 9.26% breadth, 0.0926 participation
- July 29: 11.79% breadth, 0.1179 participation
- July 30: 14.17% breadth, 0.1417 participation

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="117">
   <si>
     <t>Ticker</t>
   </si>
@@ -58,61 +58,91 @@
     <t>Risk_Reward</t>
   </si>
   <si>
+    <t>AMBER</t>
+  </si>
+  <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>EIDPARRY</t>
+  </si>
+  <si>
+    <t>GSFC</t>
+  </si>
+  <si>
+    <t>SUMICHEM</t>
+  </si>
+  <si>
+    <t>CRAFTSMAN</t>
+  </si>
+  <si>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>VISHNU</t>
+  </si>
+  <si>
+    <t>GATEWAY</t>
+  </si>
+  <si>
+    <t>COROMANDEL</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>PGHH</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>POWERINDIA</t>
+  </si>
+  <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
     <t>BOSCHLTD</t>
   </si>
   <si>
-    <t>AMBER</t>
-  </si>
-  <si>
-    <t>TORNTPHARM</t>
-  </si>
-  <si>
-    <t>CIPLA</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
-    <t>COROMANDEL</t>
+    <t>SYRMA</t>
+  </si>
+  <si>
+    <t>OLECTRA</t>
+  </si>
+  <si>
+    <t>NUVOCO</t>
   </si>
   <si>
     <t>TATACHEM</t>
   </si>
   <si>
-    <t>EIDPARRY</t>
-  </si>
-  <si>
-    <t>SUMICHEM</t>
-  </si>
-  <si>
-    <t>CRAFTSMAN</t>
-  </si>
-  <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>GATEWAY</t>
-  </si>
-  <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
-  </si>
-  <si>
-    <t>TI</t>
+    <t>RAMCOCEM</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>GRANULES</t>
   </si>
   <si>
     <t>ETERNAL</t>
   </si>
   <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
+    <t>PCBL</t>
   </si>
   <si>
     <t>UPL</t>
@@ -124,30 +154,21 @@
     <t>ANANDRATHI</t>
   </si>
   <si>
+    <t>JGCHEM</t>
+  </si>
+  <si>
     <t>PATANJALI</t>
   </si>
   <si>
-    <t>JGCHEM</t>
-  </si>
-  <si>
-    <t>AGI</t>
-  </si>
-  <si>
-    <t>NUVOCO</t>
-  </si>
-  <si>
-    <t>PCBL</t>
-  </si>
-  <si>
-    <t>EPACK</t>
-  </si>
-  <si>
     <t>VIPIND</t>
   </si>
   <si>
     <t>METROPOLIS</t>
   </si>
   <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
@@ -160,102 +181,105 @@
     <t>STARHEALTH</t>
   </si>
   <si>
+    <t>WELCORP</t>
+  </si>
+  <si>
+    <t>NIACL</t>
+  </si>
+  <si>
+    <t>CAPLIPOINT</t>
+  </si>
+  <si>
     <t>GODFRYPHLP</t>
   </si>
   <si>
-    <t>VISHNU</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>POWERINDIA</t>
+    <t>PAGEIND</t>
+  </si>
+  <si>
+    <t>MPHASIS</t>
+  </si>
+  <si>
+    <t>PIIND</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>BSOFT</t>
+  </si>
+  <si>
+    <t>SUNPHARMA</t>
+  </si>
+  <si>
+    <t>DMART</t>
   </si>
   <si>
     <t>DBL</t>
   </si>
   <si>
-    <t>PIIND</t>
-  </si>
-  <si>
-    <t>PAGEIND</t>
-  </si>
-  <si>
-    <t>BLS</t>
-  </si>
-  <si>
-    <t>SUNPHARMA</t>
-  </si>
-  <si>
     <t>APARINDS</t>
   </si>
   <si>
     <t>JBCHEPHARM</t>
   </si>
   <si>
-    <t>BSOFT</t>
-  </si>
-  <si>
-    <t>PGHH</t>
-  </si>
-  <si>
-    <t>MPHASIS</t>
-  </si>
-  <si>
-    <t>NIACL</t>
+    <t>ABBOTINDIA</t>
+  </si>
+  <si>
+    <t>TMB</t>
+  </si>
+  <si>
+    <t>FLUOROCHEM</t>
+  </si>
+  <si>
+    <t>AARTIIND</t>
+  </si>
+  <si>
+    <t>NAVINFLUOR</t>
+  </si>
+  <si>
+    <t>AUBANK</t>
+  </si>
+  <si>
+    <t>BALKRISIND</t>
   </si>
   <si>
     <t>HEG</t>
   </si>
   <si>
-    <t>AUBANK</t>
-  </si>
-  <si>
-    <t>EICHERMOT</t>
+    <t>GMMPFAUDLR</t>
+  </si>
+  <si>
+    <t>INDIGOPNTS</t>
+  </si>
+  <si>
+    <t>LALPATHLAB</t>
+  </si>
+  <si>
+    <t>DIXON</t>
   </si>
   <si>
     <t>GPIL</t>
   </si>
   <si>
-    <t>BERGEPAINT</t>
-  </si>
-  <si>
-    <t>FLUOROCHEM</t>
-  </si>
-  <si>
-    <t>ERIS</t>
-  </si>
-  <si>
-    <t>LALPATHLAB</t>
-  </si>
-  <si>
-    <t>DMART</t>
-  </si>
-  <si>
-    <t>DIXON</t>
+    <t>KALYANKJIL</t>
   </si>
   <si>
     <t>DABUR</t>
   </si>
   <si>
-    <t>CESC</t>
-  </si>
-  <si>
-    <t>GMMPFAUDLR</t>
-  </si>
-  <si>
     <t>ZYDUSLIFE</t>
   </si>
   <si>
     <t>Consumer Cyclical</t>
   </si>
   <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
     <t>Unknown</t>
   </si>
   <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
     <t>Basic Materials</t>
   </si>
   <si>
@@ -271,9 +295,6 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>Utilities</t>
-  </si>
-  <si>
     <t>Building_G</t>
   </si>
   <si>
@@ -292,30 +313,36 @@
     <t>2025-07-07</t>
   </si>
   <si>
+    <t>2025-07-25</t>
+  </si>
+  <si>
     <t>2025-07-15</t>
   </si>
   <si>
-    <t>2025-07-25</t>
+    <t>2025-07-24</t>
+  </si>
+  <si>
+    <t>2025-07-16</t>
+  </si>
+  <si>
+    <t>2025-07-30</t>
   </si>
   <si>
     <t>2025-07-29</t>
   </si>
   <si>
+    <t>2025-07-17</t>
+  </si>
+  <si>
+    <t>2025-07-11</t>
+  </si>
+  <si>
     <t>2025-07-22</t>
   </si>
   <si>
-    <t>2025-07-16</t>
-  </si>
-  <si>
-    <t>2025-07-30</t>
-  </si>
-  <si>
     <t>2025-07-08</t>
   </si>
   <si>
-    <t>2025-07-11</t>
-  </si>
-  <si>
     <t>2025-07-09</t>
   </si>
   <si>
@@ -323,9 +350,6 @@
   </si>
   <si>
     <t>2025-07-18</t>
-  </si>
-  <si>
-    <t>2025-07-17</t>
   </si>
   <si>
     <t>G PATTERN DEVELOPING - DOUBLE POSITION (50%)</t>
@@ -698,7 +722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -753,19 +777,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D2">
-        <v>97.11</v>
+        <v>82.47</v>
       </c>
       <c r="E2">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -774,19 +798,19 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K2">
-        <v>40395</v>
+        <v>8022.5</v>
       </c>
       <c r="L2">
-        <v>38442.86</v>
+        <v>7451.93</v>
       </c>
       <c r="M2">
-        <v>44299.29</v>
+        <v>9163.639999999999</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -797,40 +821,40 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D3">
-        <v>64.04000000000001</v>
+        <v>49.4</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G3">
-        <v>79.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K3">
-        <v>8012.5</v>
+        <v>1559.9</v>
       </c>
       <c r="L3">
-        <v>7452.29</v>
+        <v>1506.06</v>
       </c>
       <c r="M3">
-        <v>9132.93</v>
+        <v>1667.59</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -841,19 +865,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="D4">
-        <v>54.22</v>
+        <v>49.4</v>
       </c>
       <c r="E4">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -865,16 +889,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K4">
-        <v>3739</v>
+        <v>3724.8</v>
       </c>
       <c r="L4">
-        <v>3593.57</v>
+        <v>3579.3</v>
       </c>
       <c r="M4">
-        <v>4029.86</v>
+        <v>4015.8</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -885,40 +909,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D5">
-        <v>49.4</v>
+        <v>60.78</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>60.78</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="K5">
-        <v>1560.2</v>
+        <v>1235.3</v>
       </c>
       <c r="L5">
-        <v>1507.49</v>
+        <v>1165.57</v>
       </c>
       <c r="M5">
-        <v>1665.63</v>
+        <v>1374.76</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -929,40 +953,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D6">
-        <v>68.01000000000001</v>
+        <v>53.37</v>
       </c>
       <c r="E6">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>53.37</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="K6">
-        <v>722.55</v>
+        <v>207.6</v>
       </c>
       <c r="L6">
-        <v>680.96</v>
+        <v>200.89</v>
       </c>
       <c r="M6">
-        <v>805.74</v>
+        <v>221.02</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -973,40 +997,40 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D7">
-        <v>68.01000000000001</v>
+        <v>94.88</v>
       </c>
       <c r="E7">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G7">
-        <v>68.01000000000001</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="K7">
-        <v>2612.6</v>
+        <v>649.6</v>
       </c>
       <c r="L7">
-        <v>2446.41</v>
+        <v>606.42</v>
       </c>
       <c r="M7">
-        <v>2944.97</v>
+        <v>735.96</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1017,22 +1041,22 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D8">
-        <v>55.96</v>
+        <v>92.47</v>
       </c>
       <c r="E8">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G8">
-        <v>75.23999999999999</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1041,16 +1065,16 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="K8">
-        <v>1006.1</v>
+        <v>6740</v>
       </c>
       <c r="L8">
-        <v>950.14</v>
+        <v>6269.43</v>
       </c>
       <c r="M8">
-        <v>1118.01</v>
+        <v>7681.14</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1061,40 +1085,40 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D9">
-        <v>53.55</v>
+        <v>92.47</v>
       </c>
       <c r="E9">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="G9">
-        <v>53.55</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="K9">
-        <v>1227.4</v>
+        <v>522.5</v>
       </c>
       <c r="L9">
-        <v>1158.96</v>
+        <v>496.41</v>
       </c>
       <c r="M9">
-        <v>1364.29</v>
+        <v>574.6900000000001</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1105,22 +1129,22 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D10">
-        <v>94.88</v>
+        <v>91.27</v>
       </c>
       <c r="E10">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>91.27</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1129,16 +1153,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K10">
-        <v>638.5</v>
+        <v>570.5</v>
       </c>
       <c r="L10">
-        <v>596.04</v>
+        <v>531.85</v>
       </c>
       <c r="M10">
-        <v>723.4299999999999</v>
+        <v>647.8</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1149,22 +1173,22 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D11">
-        <v>94.88</v>
+        <v>88.86</v>
       </c>
       <c r="E11">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>91.27</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1173,16 +1197,16 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K11">
-        <v>6796</v>
+        <v>71.34</v>
       </c>
       <c r="L11">
-        <v>6325.43</v>
+        <v>66.7</v>
       </c>
       <c r="M11">
-        <v>7737.14</v>
+        <v>80.63</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1193,40 +1217,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D12">
-        <v>92.47</v>
+        <v>86.45</v>
       </c>
       <c r="E12">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K12">
-        <v>521.35</v>
+        <v>2658.8</v>
       </c>
       <c r="L12">
-        <v>495.26</v>
+        <v>2487.47</v>
       </c>
       <c r="M12">
-        <v>573.54</v>
+        <v>3001.46</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1237,22 +1261,22 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D13">
-        <v>91.27</v>
+        <v>82.83</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G13">
-        <v>91.27</v>
+        <v>82.83</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1261,16 +1285,16 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K13">
-        <v>73.09</v>
+        <v>3666</v>
       </c>
       <c r="L13">
-        <v>68.45</v>
+        <v>3546.61</v>
       </c>
       <c r="M13">
-        <v>82.38</v>
+        <v>3904.77</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1281,40 +1305,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D14">
-        <v>38.55</v>
+        <v>81.63</v>
       </c>
       <c r="E14">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="G14">
-        <v>89.88</v>
+        <v>81.63</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K14">
-        <v>887.75</v>
+        <v>13815</v>
       </c>
       <c r="L14">
-        <v>839.9400000000001</v>
+        <v>13273.57</v>
       </c>
       <c r="M14">
-        <v>983.38</v>
+        <v>14897.86</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1325,19 +1349,19 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D15">
-        <v>37.35</v>
+        <v>81.63</v>
       </c>
       <c r="E15">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -1346,19 +1370,19 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K15">
-        <v>986.45</v>
+        <v>722</v>
       </c>
       <c r="L15">
-        <v>930.16</v>
+        <v>680.41</v>
       </c>
       <c r="M15">
-        <v>1099.04</v>
+        <v>805.1900000000001</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1369,40 +1393,40 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D16">
-        <v>31.33</v>
+        <v>53.37</v>
       </c>
       <c r="E16">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K16">
-        <v>753.2</v>
+        <v>20810</v>
       </c>
       <c r="L16">
-        <v>695.8099999999999</v>
+        <v>19117.86</v>
       </c>
       <c r="M16">
-        <v>867.99</v>
+        <v>24194.29</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1413,40 +1437,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D17">
-        <v>30.12</v>
+        <v>37.35</v>
       </c>
       <c r="E17">
         <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G17">
         <v>100</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K17">
-        <v>494</v>
+        <v>985.75</v>
       </c>
       <c r="L17">
-        <v>433.16</v>
+        <v>928.87</v>
       </c>
       <c r="M17">
-        <v>615.6900000000001</v>
+        <v>1099.51</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1457,22 +1481,22 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D18">
-        <v>24.1</v>
+        <v>37.35</v>
       </c>
       <c r="E18">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G18">
-        <v>92.47</v>
+        <v>100</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1481,16 +1505,16 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K18">
-        <v>306.8</v>
+        <v>499.95</v>
       </c>
       <c r="L18">
-        <v>285.73</v>
+        <v>439.11</v>
       </c>
       <c r="M18">
-        <v>348.94</v>
+        <v>621.64</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1501,40 +1525,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D19">
-        <v>21.69</v>
+        <v>36.14</v>
       </c>
       <c r="E19">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G19">
-        <v>82.83</v>
+        <v>89.88</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K19">
-        <v>837.6</v>
+        <v>878</v>
       </c>
       <c r="L19">
-        <v>802.6</v>
+        <v>828.79</v>
       </c>
       <c r="M19">
-        <v>907.61</v>
+        <v>976.4299999999999</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1545,16 +1569,16 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D20">
-        <v>20.48</v>
+        <v>34.94</v>
       </c>
       <c r="E20">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
         <v>98</v>
@@ -1563,22 +1587,22 @@
         <v>100</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K20">
-        <v>5661.5</v>
+        <v>39985</v>
       </c>
       <c r="L20">
-        <v>5426.36</v>
+        <v>38032.86</v>
       </c>
       <c r="M20">
-        <v>6131.79</v>
+        <v>43889.29</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1589,40 +1613,40 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D21">
-        <v>19.28</v>
+        <v>33.73</v>
       </c>
       <c r="E21">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G21">
-        <v>85.23999999999999</v>
+        <v>100</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K21">
-        <v>721.95</v>
+        <v>762.7</v>
       </c>
       <c r="L21">
-        <v>690.23</v>
+        <v>704.77</v>
       </c>
       <c r="M21">
-        <v>785.39</v>
+        <v>878.5599999999999</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1633,40 +1657,40 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D22">
-        <v>16.87</v>
+        <v>31.33</v>
       </c>
       <c r="E22">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="G22">
-        <v>86.45</v>
+        <v>90.06</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K22">
-        <v>2065.3</v>
+        <v>1424</v>
       </c>
       <c r="L22">
-        <v>1929.87</v>
+        <v>1296.93</v>
       </c>
       <c r="M22">
-        <v>2336.16</v>
+        <v>1678.14</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1677,22 +1701,22 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D23">
-        <v>16.87</v>
+        <v>28.92</v>
       </c>
       <c r="E23">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="G23">
-        <v>96.08</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1701,16 +1725,16 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K23">
-        <v>2686.4</v>
+        <v>424.95</v>
       </c>
       <c r="L23">
-        <v>2464.09</v>
+        <v>391.94</v>
       </c>
       <c r="M23">
-        <v>3131.03</v>
+        <v>490.98</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1721,40 +1745,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D24">
-        <v>14.46</v>
+        <v>25.3</v>
       </c>
       <c r="E24">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>75.23999999999999</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K24">
-        <v>1902</v>
+        <v>1004.1</v>
       </c>
       <c r="L24">
-        <v>1797.45</v>
+        <v>948.14</v>
       </c>
       <c r="M24">
-        <v>2111.1</v>
+        <v>1116.01</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1765,22 +1789,22 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D25">
-        <v>14.46</v>
+        <v>22.89</v>
       </c>
       <c r="E25">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G25">
-        <v>86.45</v>
+        <v>70.42</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1789,16 +1813,16 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K25">
-        <v>501.8</v>
+        <v>1205.1</v>
       </c>
       <c r="L25">
-        <v>468.74</v>
+        <v>1130.61</v>
       </c>
       <c r="M25">
-        <v>567.9299999999999</v>
+        <v>1354.07</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1809,19 +1833,19 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D26">
-        <v>14.46</v>
+        <v>20.48</v>
       </c>
       <c r="E26">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G26">
         <v>100</v>
@@ -1833,16 +1857,16 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K26">
-        <v>962.75</v>
+        <v>5670</v>
       </c>
       <c r="L26">
-        <v>875.5700000000001</v>
+        <v>5432.71</v>
       </c>
       <c r="M26">
-        <v>1137.11</v>
+        <v>6144.57</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1853,40 +1877,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D27">
-        <v>14.46</v>
+        <v>20.48</v>
       </c>
       <c r="E27">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G27">
-        <v>84.04000000000001</v>
+        <v>82.83</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K27">
-        <v>418.55</v>
+        <v>841.95</v>
       </c>
       <c r="L27">
-        <v>387.16</v>
+        <v>802.99</v>
       </c>
       <c r="M27">
-        <v>481.32</v>
+        <v>919.88</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1897,43 +1921,43 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D28">
-        <v>13.25</v>
+        <v>20.48</v>
       </c>
       <c r="E28">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G28">
-        <v>70.78</v>
+        <v>76.45</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K28">
-        <v>394.2</v>
+        <v>492.35</v>
       </c>
       <c r="L28">
-        <v>399.29</v>
+        <v>478.7</v>
       </c>
       <c r="M28">
-        <v>384.01</v>
+        <v>519.64</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1941,40 +1965,40 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D29">
-        <v>13.25</v>
+        <v>20.48</v>
       </c>
       <c r="E29">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G29">
-        <v>71.98999999999999</v>
+        <v>92.47</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K29">
-        <v>370.35</v>
+        <v>303.35</v>
       </c>
       <c r="L29">
-        <v>354.18</v>
+        <v>282.11</v>
       </c>
       <c r="M29">
-        <v>402.69</v>
+        <v>345.82</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -1985,22 +2009,22 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D30">
-        <v>13.25</v>
+        <v>19.28</v>
       </c>
       <c r="E30">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G30">
-        <v>71.98999999999999</v>
+        <v>70.78</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -2009,19 +2033,19 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K30">
-        <v>464.45</v>
+        <v>397.3</v>
       </c>
       <c r="L30">
-        <v>440.62</v>
+        <v>399.48</v>
       </c>
       <c r="M30">
-        <v>512.12</v>
+        <v>392.93</v>
       </c>
       <c r="N30">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2029,40 +2053,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D31">
-        <v>12.05</v>
+        <v>19.28</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G31">
-        <v>72.29000000000001</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K31">
-        <v>2020.5</v>
+        <v>721.85</v>
       </c>
       <c r="L31">
-        <v>1890.26</v>
+        <v>690.14</v>
       </c>
       <c r="M31">
-        <v>2280.98</v>
+        <v>785.26</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2073,40 +2097,40 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D32">
-        <v>10.84</v>
+        <v>16.87</v>
       </c>
       <c r="E32">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G32">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K32">
-        <v>981.75</v>
+        <v>2059.9</v>
       </c>
       <c r="L32">
-        <v>955.4</v>
+        <v>1927.72</v>
       </c>
       <c r="M32">
-        <v>1034.46</v>
+        <v>2324.25</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2117,40 +2141,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D33">
-        <v>8.43</v>
+        <v>16.87</v>
       </c>
       <c r="E33">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G33">
-        <v>81.27</v>
+        <v>96.08</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K33">
-        <v>71.98999999999999</v>
+        <v>2679.1</v>
       </c>
       <c r="L33">
-        <v>70.03</v>
+        <v>2456.79</v>
       </c>
       <c r="M33">
-        <v>75.91</v>
+        <v>3123.73</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2161,40 +2185,40 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D34">
-        <v>7.23</v>
+        <v>14.46</v>
       </c>
       <c r="E34">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G34">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="K34">
-        <v>617.75</v>
+        <v>503.95</v>
       </c>
       <c r="L34">
-        <v>597.6900000000001</v>
+        <v>468.94</v>
       </c>
       <c r="M34">
-        <v>657.86</v>
+        <v>573.97</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2205,40 +2229,40 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D35">
-        <v>44.94</v>
+        <v>14.46</v>
       </c>
       <c r="E35">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G35">
-        <v>44.94</v>
+        <v>100</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="K35">
-        <v>445.5</v>
+        <v>1898</v>
       </c>
       <c r="L35">
-        <v>426.18</v>
+        <v>1797.07</v>
       </c>
       <c r="M35">
-        <v>484.15</v>
+        <v>2099.86</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2249,40 +2273,40 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D36">
-        <v>40.12</v>
+        <v>13.25</v>
       </c>
       <c r="E36">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="G36">
-        <v>90.06</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="K36">
-        <v>9434.5</v>
+        <v>463.4</v>
       </c>
       <c r="L36">
-        <v>8740.809999999999</v>
+        <v>440.52</v>
       </c>
       <c r="M36">
-        <v>10821.89</v>
+        <v>509.17</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2293,40 +2317,40 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D37">
-        <v>91.27</v>
+        <v>12.05</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G37">
-        <v>91.27</v>
+        <v>72.29000000000001</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K37">
-        <v>579.6</v>
+        <v>2020</v>
       </c>
       <c r="L37">
-        <v>540.95</v>
+        <v>1889.86</v>
       </c>
       <c r="M37">
-        <v>656.9</v>
+        <v>2280.28</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2337,40 +2361,40 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D38">
-        <v>82.83</v>
+        <v>10.84</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="F38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G38">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K38">
-        <v>3660.1</v>
+        <v>398</v>
       </c>
       <c r="L38">
-        <v>3544.04</v>
+        <v>380.36</v>
       </c>
       <c r="M38">
-        <v>3892.21</v>
+        <v>433.28</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2381,22 +2405,22 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D39">
-        <v>53.37</v>
+        <v>10.84</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="G39">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2405,16 +2429,16 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K39">
-        <v>20810</v>
+        <v>983</v>
       </c>
       <c r="L39">
-        <v>19117.86</v>
+        <v>955.51</v>
       </c>
       <c r="M39">
-        <v>24194.29</v>
+        <v>1037.97</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2425,40 +2449,40 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D40">
-        <v>38.92</v>
+        <v>8.43</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="G40">
-        <v>38.92</v>
+        <v>81.27</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K40">
-        <v>485.55</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="L40">
-        <v>479.65</v>
+        <v>70.03</v>
       </c>
       <c r="M40">
-        <v>497.35</v>
+        <v>76.23</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2469,40 +2493,40 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D41">
-        <v>38.55</v>
+        <v>7.23</v>
       </c>
       <c r="E41">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F41" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G41">
-        <v>38.55</v>
+        <v>100</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="K41">
-        <v>4319.4</v>
+        <v>617.2</v>
       </c>
       <c r="L41">
-        <v>4129.06</v>
+        <v>596.89</v>
       </c>
       <c r="M41">
-        <v>4700.09</v>
+        <v>657.83</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2513,22 +2537,22 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D42">
-        <v>35.3</v>
+        <v>44.94</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F42" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="G42">
-        <v>35.3</v>
+        <v>44.94</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -2537,16 +2561,16 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K42">
-        <v>48515</v>
+        <v>447.85</v>
       </c>
       <c r="L42">
-        <v>46848.16</v>
+        <v>426.24</v>
       </c>
       <c r="M42">
-        <v>51848.67</v>
+        <v>491.07</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2557,40 +2581,40 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D43">
-        <v>34.1</v>
+        <v>44.94</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G43">
-        <v>34.1</v>
+        <v>44.94</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K43">
-        <v>378.1</v>
+        <v>943.8</v>
       </c>
       <c r="L43">
-        <v>368.79</v>
+        <v>898.01</v>
       </c>
       <c r="M43">
-        <v>396.72</v>
+        <v>1035.37</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2601,40 +2625,40 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D44">
-        <v>33.92</v>
+        <v>44.58</v>
       </c>
       <c r="E44">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F44" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G44">
-        <v>33.92</v>
+        <v>44.58</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K44">
-        <v>1738.6</v>
+        <v>206.59</v>
       </c>
       <c r="L44">
-        <v>1691.13</v>
+        <v>194.25</v>
       </c>
       <c r="M44">
-        <v>1833.54</v>
+        <v>231.27</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2645,40 +2669,40 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D45">
-        <v>31.33</v>
+        <v>42.53</v>
       </c>
       <c r="E45">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G45">
-        <v>65.59999999999999</v>
+        <v>42.53</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K45">
-        <v>9560</v>
+        <v>2150.2</v>
       </c>
       <c r="L45">
-        <v>8808.57</v>
+        <v>2050.95</v>
       </c>
       <c r="M45">
-        <v>11062.86</v>
+        <v>2348.71</v>
       </c>
       <c r="N45">
         <v>2</v>
@@ -2689,40 +2713,40 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D46">
-        <v>30.12</v>
+        <v>40.12</v>
       </c>
       <c r="E46">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46">
-        <v>38.55</v>
+        <v>90.06</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K46">
-        <v>1792.5</v>
+        <v>9390</v>
       </c>
       <c r="L46">
-        <v>1727.07</v>
+        <v>8736.57</v>
       </c>
       <c r="M46">
-        <v>1923.36</v>
+        <v>10696.86</v>
       </c>
       <c r="N46">
         <v>2</v>
@@ -2733,22 +2757,22 @@
         <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D47">
-        <v>26.51</v>
+        <v>40.12</v>
       </c>
       <c r="E47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G47">
-        <v>26.51</v>
+        <v>40.12</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2757,16 +2781,16 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K47">
-        <v>418.6</v>
+        <v>48385</v>
       </c>
       <c r="L47">
-        <v>408.29</v>
+        <v>46834.36</v>
       </c>
       <c r="M47">
-        <v>439.22</v>
+        <v>51486.29</v>
       </c>
       <c r="N47">
         <v>2</v>
@@ -2777,40 +2801,40 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D48">
-        <v>25.3</v>
+        <v>40.12</v>
       </c>
       <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G48">
+        <v>40.12</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <v>4</v>
       </c>
-      <c r="F48" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48">
-        <v>25.3</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
       <c r="J48" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="K48">
-        <v>13350</v>
+        <v>2810.3</v>
       </c>
       <c r="L48">
-        <v>13115.74</v>
+        <v>2720.53</v>
       </c>
       <c r="M48">
-        <v>13818.52</v>
+        <v>2989.84</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -2821,40 +2845,40 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D49">
-        <v>25.3</v>
+        <v>52.17</v>
       </c>
       <c r="E49">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G49">
-        <v>25.3</v>
+        <v>52.17</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J49" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K49">
-        <v>2817</v>
+        <v>4324</v>
       </c>
       <c r="L49">
-        <v>2722.56</v>
+        <v>4133.51</v>
       </c>
       <c r="M49">
-        <v>3005.88</v>
+        <v>4704.97</v>
       </c>
       <c r="N49">
         <v>2</v>
@@ -2865,40 +2889,40 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D50">
-        <v>22.89</v>
+        <v>38.92</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G50">
-        <v>22.89</v>
+        <v>38.92</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K50">
-        <v>191.46</v>
+        <v>377.6</v>
       </c>
       <c r="L50">
-        <v>181.22</v>
+        <v>368.74</v>
       </c>
       <c r="M50">
-        <v>211.94</v>
+        <v>395.32</v>
       </c>
       <c r="N50">
         <v>2</v>
@@ -2909,40 +2933,40 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D51">
-        <v>19.28</v>
+        <v>34.1</v>
       </c>
       <c r="E51">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="G51">
-        <v>39.76</v>
+        <v>34.1</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K51">
-        <v>530.2</v>
+        <v>414.15</v>
       </c>
       <c r="L51">
-        <v>512.74</v>
+        <v>407.87</v>
       </c>
       <c r="M51">
-        <v>565.13</v>
+        <v>426.72</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -2953,43 +2977,43 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D52">
-        <v>19.28</v>
+        <v>33.92</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F52" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G52">
-        <v>19.28</v>
+        <v>33.92</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I52">
         <v>0</v>
       </c>
       <c r="J52" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K52">
-        <v>749.5</v>
+        <v>1733.1</v>
       </c>
       <c r="L52">
-        <v>757.0599999999999</v>
+        <v>1685.59</v>
       </c>
       <c r="M52">
-        <v>734.39</v>
+        <v>1828.13</v>
       </c>
       <c r="N52">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -2997,40 +3021,40 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D53">
-        <v>19.28</v>
+        <v>33.73</v>
       </c>
       <c r="E53">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F53" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G53">
-        <v>19.28</v>
+        <v>33.73</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K53">
-        <v>5527</v>
+        <v>4295.9</v>
       </c>
       <c r="L53">
-        <v>5481.89</v>
+        <v>4096.49</v>
       </c>
       <c r="M53">
-        <v>5617.21</v>
+        <v>4694.73</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -3041,40 +3065,40 @@
         <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D54">
-        <v>15.66</v>
+        <v>32.89</v>
       </c>
       <c r="E54">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F54" t="s">
         <v>103</v>
       </c>
       <c r="G54">
-        <v>26.51</v>
+        <v>38.92</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K54">
-        <v>196.6</v>
+        <v>481.7</v>
       </c>
       <c r="L54">
-        <v>187.5</v>
+        <v>479.28</v>
       </c>
       <c r="M54">
-        <v>214.81</v>
+        <v>486.54</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -3085,40 +3109,40 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D55">
-        <v>14.46</v>
+        <v>31.33</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F55" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="G55">
-        <v>14.46</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J55" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K55">
-        <v>577.35</v>
+        <v>9589</v>
       </c>
       <c r="L55">
-        <v>564.6</v>
+        <v>8826.360000000001</v>
       </c>
       <c r="M55">
-        <v>602.86</v>
+        <v>11114.29</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -3129,40 +3153,40 @@
         <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D56">
-        <v>14.46</v>
+        <v>27.71</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="G56">
-        <v>20.48</v>
+        <v>38.55</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K56">
-        <v>3570.6</v>
+        <v>1782.8</v>
       </c>
       <c r="L56">
-        <v>3477.36</v>
+        <v>1716.8</v>
       </c>
       <c r="M56">
-        <v>3757.08</v>
+        <v>1914.8</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -3173,40 +3197,40 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D57">
-        <v>13.25</v>
+        <v>22.89</v>
       </c>
       <c r="E57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57">
-        <v>13.25</v>
+        <v>22.89</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K57">
-        <v>1835</v>
+        <v>35100</v>
       </c>
       <c r="L57">
-        <v>1731</v>
+        <v>33731.42</v>
       </c>
       <c r="M57">
-        <v>2043.01</v>
+        <v>37837.16</v>
       </c>
       <c r="N57">
         <v>2</v>
@@ -3217,40 +3241,40 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D58">
-        <v>12.05</v>
+        <v>21.69</v>
       </c>
       <c r="E58">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F58" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G58">
-        <v>58.19</v>
+        <v>41.14</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J58" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K58">
-        <v>3098.5</v>
+        <v>460.05</v>
       </c>
       <c r="L58">
-        <v>2942.52</v>
+        <v>448.45</v>
       </c>
       <c r="M58">
-        <v>3410.46</v>
+        <v>483.24</v>
       </c>
       <c r="N58">
         <v>2</v>
@@ -3261,40 +3285,40 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D59">
-        <v>12.05</v>
+        <v>20.48</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G59">
-        <v>12.05</v>
+        <v>20.48</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K59">
-        <v>4207.4</v>
+        <v>3596</v>
       </c>
       <c r="L59">
-        <v>4045.1</v>
+        <v>3479.44</v>
       </c>
       <c r="M59">
-        <v>4532</v>
+        <v>3829.12</v>
       </c>
       <c r="N59">
         <v>2</v>
@@ -3305,40 +3329,40 @@
         <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D60">
-        <v>12.05</v>
+        <v>20.48</v>
       </c>
       <c r="E60">
-        <v>78</v>
+        <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G60">
-        <v>61.99</v>
+        <v>20.48</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K60">
-        <v>16789</v>
+        <v>447.75</v>
       </c>
       <c r="L60">
-        <v>16137.57</v>
+        <v>440.3</v>
       </c>
       <c r="M60">
-        <v>18091.86</v>
+        <v>462.65</v>
       </c>
       <c r="N60">
         <v>2</v>
@@ -3349,40 +3373,40 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D61">
-        <v>9.640000000000001</v>
+        <v>19.28</v>
       </c>
       <c r="E61">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="F61" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G61">
-        <v>60.24</v>
+        <v>66.81</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I61">
         <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K61">
-        <v>522.3</v>
+        <v>5183.5</v>
       </c>
       <c r="L61">
-        <v>508.85</v>
+        <v>4922.85</v>
       </c>
       <c r="M61">
-        <v>549.2</v>
+        <v>5704.8</v>
       </c>
       <c r="N61">
         <v>2</v>
@@ -3393,22 +3417,22 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D62">
-        <v>8.43</v>
+        <v>19.28</v>
       </c>
       <c r="E62">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F62" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G62">
-        <v>16.87</v>
+        <v>19.28</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -3417,19 +3441,19 @@
         <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K62">
-        <v>178.66</v>
+        <v>745.6</v>
       </c>
       <c r="L62">
-        <v>174.62</v>
+        <v>756.66</v>
       </c>
       <c r="M62">
-        <v>186.73</v>
+        <v>723.48</v>
       </c>
       <c r="N62">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3437,40 +3461,40 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D63">
-        <v>4.82</v>
+        <v>19.28</v>
       </c>
       <c r="E63">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F63" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G63">
-        <v>39.76</v>
+        <v>43.37</v>
       </c>
       <c r="H63">
         <v>0</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="K63">
-        <v>1334.8</v>
+        <v>2758.8</v>
       </c>
       <c r="L63">
-        <v>1270.45</v>
+        <v>2641.59</v>
       </c>
       <c r="M63">
-        <v>1463.49</v>
+        <v>2993.21</v>
       </c>
       <c r="N63">
         <v>2</v>
@@ -3481,42 +3505,394 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D64">
+        <v>19.28</v>
+      </c>
+      <c r="E64">
+        <v>32</v>
+      </c>
+      <c r="F64" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64">
+        <v>39.76</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>116</v>
+      </c>
+      <c r="K64">
+        <v>534.9</v>
+      </c>
+      <c r="L64">
+        <v>513.0700000000001</v>
+      </c>
+      <c r="M64">
+        <v>578.5700000000001</v>
+      </c>
+      <c r="N64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65">
+        <v>18.07</v>
+      </c>
+      <c r="E65">
+        <v>29</v>
+      </c>
+      <c r="F65" t="s">
+        <v>98</v>
+      </c>
+      <c r="G65">
+        <v>39.76</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65" t="s">
+        <v>116</v>
+      </c>
+      <c r="K65">
+        <v>1349.4</v>
+      </c>
+      <c r="L65">
+        <v>1278.49</v>
+      </c>
+      <c r="M65">
+        <v>1491.23</v>
+      </c>
+      <c r="N65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" t="s">
         <v>78</v>
       </c>
-      <c r="C64" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64">
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66">
+        <v>15.66</v>
+      </c>
+      <c r="E66">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G66">
+        <v>21.69</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>2</v>
+      </c>
+      <c r="J66" t="s">
+        <v>116</v>
+      </c>
+      <c r="K66">
+        <v>1207.1</v>
+      </c>
+      <c r="L66">
+        <v>1170.53</v>
+      </c>
+      <c r="M66">
+        <v>1280.23</v>
+      </c>
+      <c r="N66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="D67">
+        <v>12.05</v>
+      </c>
+      <c r="E67">
+        <v>40</v>
+      </c>
+      <c r="F67" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67">
+        <v>58.19</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>116</v>
+      </c>
+      <c r="K67">
+        <v>3101.3</v>
+      </c>
+      <c r="L67">
+        <v>2944.09</v>
+      </c>
+      <c r="M67">
+        <v>3415.73</v>
+      </c>
+      <c r="N67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68">
+        <v>12.05</v>
+      </c>
+      <c r="E68">
+        <v>80</v>
+      </c>
+      <c r="F68" t="s">
+        <v>109</v>
+      </c>
+      <c r="G68">
+        <v>61.99</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>116</v>
+      </c>
+      <c r="K68">
+        <v>16793</v>
+      </c>
+      <c r="L68">
+        <v>16141.57</v>
+      </c>
+      <c r="M68">
+        <v>18095.86</v>
+      </c>
+      <c r="N68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69">
+        <v>10.84</v>
+      </c>
+      <c r="E69">
+        <v>10</v>
+      </c>
+      <c r="F69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69">
+        <v>26.51</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69">
+        <v>195.53</v>
+      </c>
+      <c r="L69">
+        <v>187.39</v>
+      </c>
+      <c r="M69">
+        <v>211.8</v>
+      </c>
+      <c r="N69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="E70">
+        <v>30</v>
+      </c>
+      <c r="F70" t="s">
+        <v>98</v>
+      </c>
+      <c r="G70">
+        <v>30.12</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>116</v>
+      </c>
+      <c r="K70">
+        <v>607.35</v>
+      </c>
+      <c r="L70">
+        <v>582.41</v>
+      </c>
+      <c r="M70">
+        <v>657.23</v>
+      </c>
+      <c r="N70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="E71">
+        <v>45</v>
+      </c>
+      <c r="F71" t="s">
+        <v>98</v>
+      </c>
+      <c r="G71">
+        <v>60.24</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>116</v>
+      </c>
+      <c r="K71">
+        <v>522.7</v>
+      </c>
+      <c r="L71">
+        <v>508.88</v>
+      </c>
+      <c r="M71">
+        <v>550.34</v>
+      </c>
+      <c r="N71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72">
         <v>4.82</v>
       </c>
-      <c r="E64">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
-        <v>91</v>
-      </c>
-      <c r="G64">
+      <c r="E72">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s">
+        <v>98</v>
+      </c>
+      <c r="G72">
         <v>14.46</v>
       </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-      <c r="J64" t="s">
-        <v>108</v>
-      </c>
-      <c r="K64">
-        <v>996.05</v>
-      </c>
-      <c r="L64">
-        <v>969.08</v>
-      </c>
-      <c r="M64">
-        <v>1049.98</v>
-      </c>
-      <c r="N64">
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>116</v>
+      </c>
+      <c r="K72">
+        <v>995</v>
+      </c>
+      <c r="L72">
+        <v>968.98</v>
+      </c>
+      <c r="M72">
+        <v>1047.03</v>
+      </c>
+      <c r="N72">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix dashboard data population issues - restart services with correct log dates
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="115">
   <si>
     <t>Ticker</t>
   </si>
@@ -73,12 +73,12 @@
     <t>GSFC</t>
   </si>
   <si>
+    <t>CRAFTSMAN</t>
+  </si>
+  <si>
     <t>SUMICHEM</t>
   </si>
   <si>
-    <t>CRAFTSMAN</t>
-  </si>
-  <si>
     <t>VBL</t>
   </si>
   <si>
@@ -94,33 +94,30 @@
     <t>LT</t>
   </si>
   <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
     <t>PGHH</t>
   </si>
   <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
     <t>POWERINDIA</t>
   </si>
   <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
     <t>SHYAMMETL</t>
   </si>
   <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
     <t>TI</t>
   </si>
   <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
     <t>SYRMA</t>
   </si>
   <si>
-    <t>OLECTRA</t>
-  </si>
-  <si>
     <t>NUVOCO</t>
   </si>
   <si>
@@ -133,27 +130,27 @@
     <t>HDFCAMC</t>
   </si>
   <si>
+    <t>ETERNAL</t>
+  </si>
+  <si>
+    <t>GRANULES</t>
+  </si>
+  <si>
     <t>FORTIS</t>
   </si>
   <si>
-    <t>GRANULES</t>
-  </si>
-  <si>
-    <t>ETERNAL</t>
-  </si>
-  <si>
     <t>PCBL</t>
   </si>
   <si>
     <t>UPL</t>
   </si>
   <si>
+    <t>ANANDRATHI</t>
+  </si>
+  <si>
     <t>GLAND</t>
   </si>
   <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
     <t>JGCHEM</t>
   </si>
   <si>
@@ -166,16 +163,16 @@
     <t>METROPOLIS</t>
   </si>
   <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
+    <t>AMBUJACEM</t>
+  </si>
+  <si>
     <t>NMDC</t>
   </si>
   <si>
-    <t>AMBUJACEM</t>
+    <t>CAPLIPOINT</t>
   </si>
   <si>
     <t>STARHEALTH</t>
@@ -187,9 +184,6 @@
     <t>NIACL</t>
   </si>
   <si>
-    <t>CAPLIPOINT</t>
-  </si>
-  <si>
     <t>GODFRYPHLP</t>
   </si>
   <si>
@@ -205,21 +199,21 @@
     <t>BLS</t>
   </si>
   <si>
+    <t>APARINDS</t>
+  </si>
+  <si>
     <t>BSOFT</t>
   </si>
   <si>
     <t>SUNPHARMA</t>
   </si>
   <si>
+    <t>DBL</t>
+  </si>
+  <si>
     <t>DMART</t>
   </si>
   <si>
-    <t>DBL</t>
-  </si>
-  <si>
-    <t>APARINDS</t>
-  </si>
-  <si>
     <t>JBCHEPHARM</t>
   </si>
   <si>
@@ -229,30 +223,27 @@
     <t>TMB</t>
   </si>
   <si>
+    <t>NAVINFLUOR</t>
+  </si>
+  <si>
+    <t>AUBANK</t>
+  </si>
+  <si>
     <t>FLUOROCHEM</t>
   </si>
   <si>
+    <t>HEG</t>
+  </si>
+  <si>
+    <t>BALKRISIND</t>
+  </si>
+  <si>
+    <t>GMMPFAUDLR</t>
+  </si>
+  <si>
     <t>AARTIIND</t>
   </si>
   <si>
-    <t>NAVINFLUOR</t>
-  </si>
-  <si>
-    <t>AUBANK</t>
-  </si>
-  <si>
-    <t>BALKRISIND</t>
-  </si>
-  <si>
-    <t>HEG</t>
-  </si>
-  <si>
-    <t>GMMPFAUDLR</t>
-  </si>
-  <si>
-    <t>INDIGOPNTS</t>
-  </si>
-  <si>
     <t>LALPATHLAB</t>
   </si>
   <si>
@@ -262,13 +253,16 @@
     <t>GPIL</t>
   </si>
   <si>
+    <t>DABUR</t>
+  </si>
+  <si>
+    <t>BALAMINES</t>
+  </si>
+  <si>
+    <t>ZYDUSLIFE</t>
+  </si>
+  <si>
     <t>KALYANKJIL</t>
-  </si>
-  <si>
-    <t>DABUR</t>
-  </si>
-  <si>
-    <t>ZYDUSLIFE</t>
   </si>
   <si>
     <t>Consumer Cyclical</t>
@@ -722,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -777,19 +771,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2">
-        <v>82.47</v>
+        <v>100</v>
       </c>
       <c r="E2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -801,16 +795,16 @@
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K2">
-        <v>8022.5</v>
+        <v>8040.5</v>
       </c>
       <c r="L2">
-        <v>7451.93</v>
+        <v>7469.93</v>
       </c>
       <c r="M2">
-        <v>9163.639999999999</v>
+        <v>9181.639999999999</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -821,19 +815,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3">
         <v>49.4</v>
       </c>
       <c r="E3">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -845,16 +839,16 @@
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K3">
-        <v>1559.9</v>
+        <v>1559.4</v>
       </c>
       <c r="L3">
-        <v>1506.06</v>
+        <v>1505.56</v>
       </c>
       <c r="M3">
-        <v>1667.59</v>
+        <v>1667.09</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -865,19 +859,19 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4">
         <v>49.4</v>
       </c>
       <c r="E4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -889,16 +883,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K4">
-        <v>3724.8</v>
+        <v>3730.6</v>
       </c>
       <c r="L4">
-        <v>3579.3</v>
+        <v>3585.1</v>
       </c>
       <c r="M4">
-        <v>4015.8</v>
+        <v>4021.6</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -909,19 +903,19 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5">
         <v>60.78</v>
       </c>
       <c r="E5">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5">
         <v>60.78</v>
@@ -933,16 +927,16 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K5">
-        <v>1235.3</v>
+        <v>1236.2</v>
       </c>
       <c r="L5">
-        <v>1165.57</v>
+        <v>1166.47</v>
       </c>
       <c r="M5">
-        <v>1374.76</v>
+        <v>1375.66</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -953,19 +947,19 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6">
         <v>53.37</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G6">
         <v>53.37</v>
@@ -977,16 +971,16 @@
         <v>3</v>
       </c>
       <c r="J6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K6">
-        <v>207.6</v>
+        <v>207.58</v>
       </c>
       <c r="L6">
         <v>200.89</v>
       </c>
       <c r="M6">
-        <v>221.02</v>
+        <v>220.96</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -997,19 +991,19 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D7">
         <v>94.88</v>
       </c>
       <c r="E7">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -1018,19 +1012,19 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K7">
-        <v>649.6</v>
+        <v>6863.5</v>
       </c>
       <c r="L7">
-        <v>606.42</v>
+        <v>6390.36</v>
       </c>
       <c r="M7">
-        <v>735.96</v>
+        <v>7809.79</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1044,16 +1038,16 @@
         <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8">
-        <v>92.47</v>
+        <v>94.88</v>
       </c>
       <c r="E8">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G8">
         <v>100</v>
@@ -1062,19 +1056,19 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K8">
-        <v>6740</v>
+        <v>652.25</v>
       </c>
       <c r="L8">
-        <v>6269.43</v>
+        <v>607.64</v>
       </c>
       <c r="M8">
-        <v>7681.14</v>
+        <v>741.48</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1085,19 +1079,19 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9">
         <v>92.47</v>
       </c>
       <c r="E9">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>100</v>
@@ -1109,16 +1103,16 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K9">
-        <v>522.5</v>
+        <v>522.1</v>
       </c>
       <c r="L9">
-        <v>496.41</v>
+        <v>496.01</v>
       </c>
       <c r="M9">
-        <v>574.6900000000001</v>
+        <v>574.29</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1129,19 +1123,19 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D10">
         <v>91.27</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G10">
         <v>91.27</v>
@@ -1153,16 +1147,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K10">
-        <v>570.5</v>
+        <v>564.35</v>
       </c>
       <c r="L10">
-        <v>531.85</v>
+        <v>525.7</v>
       </c>
       <c r="M10">
-        <v>647.8</v>
+        <v>641.65</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1173,19 +1167,19 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D11">
         <v>88.86</v>
       </c>
       <c r="E11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G11">
         <v>91.27</v>
@@ -1197,16 +1191,16 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K11">
-        <v>71.34</v>
+        <v>71.29000000000001</v>
       </c>
       <c r="L11">
-        <v>66.7</v>
+        <v>66.65000000000001</v>
       </c>
       <c r="M11">
-        <v>80.63</v>
+        <v>80.58</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1217,19 +1211,19 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D12">
         <v>86.45</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G12">
         <v>86.45</v>
@@ -1241,16 +1235,16 @@
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K12">
-        <v>2658.8</v>
+        <v>2652.7</v>
       </c>
       <c r="L12">
-        <v>2487.47</v>
+        <v>2481.09</v>
       </c>
       <c r="M12">
-        <v>3001.46</v>
+        <v>2995.93</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1261,19 +1255,19 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D13">
         <v>82.83</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G13">
         <v>82.83</v>
@@ -1285,16 +1279,16 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K13">
-        <v>3666</v>
+        <v>3665.1</v>
       </c>
       <c r="L13">
-        <v>3546.61</v>
+        <v>3545.71</v>
       </c>
       <c r="M13">
-        <v>3904.77</v>
+        <v>3903.87</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1305,40 +1299,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D14">
         <v>81.63</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G14">
-        <v>81.63</v>
+        <v>100</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K14">
-        <v>13815</v>
+        <v>722.05</v>
       </c>
       <c r="L14">
-        <v>13273.57</v>
+        <v>680.46</v>
       </c>
       <c r="M14">
-        <v>14897.86</v>
+        <v>805.24</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1349,40 +1343,40 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15">
         <v>81.63</v>
       </c>
       <c r="E15">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G15">
-        <v>100</v>
+        <v>81.63</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K15">
-        <v>722</v>
+        <v>13805</v>
       </c>
       <c r="L15">
-        <v>680.41</v>
+        <v>13263.57</v>
       </c>
       <c r="M15">
-        <v>805.1900000000001</v>
+        <v>14887.86</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1393,19 +1387,19 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D16">
         <v>53.37</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16">
         <v>84.04000000000001</v>
@@ -1417,16 +1411,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K16">
-        <v>20810</v>
+        <v>20825</v>
       </c>
       <c r="L16">
-        <v>19117.86</v>
+        <v>19132.86</v>
       </c>
       <c r="M16">
-        <v>24194.29</v>
+        <v>24209.29</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1437,40 +1431,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17">
+        <v>38.55</v>
+      </c>
+      <c r="E17">
         <v>87</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>96</v>
       </c>
-      <c r="D17">
-        <v>37.35</v>
-      </c>
-      <c r="E17">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
-        <v>102</v>
-      </c>
       <c r="G17">
-        <v>100</v>
+        <v>89.88</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K17">
-        <v>985.75</v>
+        <v>881.45</v>
       </c>
       <c r="L17">
-        <v>928.87</v>
+        <v>832.17</v>
       </c>
       <c r="M17">
-        <v>1099.51</v>
+        <v>980.01</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1481,40 +1475,40 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D18">
         <v>37.35</v>
       </c>
       <c r="E18">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G18">
         <v>100</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K18">
-        <v>499.95</v>
+        <v>985.6</v>
       </c>
       <c r="L18">
-        <v>439.11</v>
+        <v>928.72</v>
       </c>
       <c r="M18">
-        <v>621.64</v>
+        <v>1099.36</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1525,40 +1519,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19">
+        <v>34.94</v>
+      </c>
+      <c r="E19">
+        <v>85</v>
+      </c>
+      <c r="F19" t="s">
         <v>96</v>
       </c>
-      <c r="D19">
-        <v>36.14</v>
-      </c>
-      <c r="E19">
-        <v>86</v>
-      </c>
-      <c r="F19" t="s">
-        <v>98</v>
-      </c>
       <c r="G19">
-        <v>89.88</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K19">
-        <v>878</v>
+        <v>40060</v>
       </c>
       <c r="L19">
-        <v>828.79</v>
+        <v>38107.86</v>
       </c>
       <c r="M19">
-        <v>976.4299999999999</v>
+        <v>43964.29</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1572,37 +1566,37 @@
         <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D20">
         <v>34.94</v>
       </c>
       <c r="E20">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>100</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K20">
-        <v>39985</v>
+        <v>498.3</v>
       </c>
       <c r="L20">
-        <v>38032.86</v>
+        <v>437.46</v>
       </c>
       <c r="M20">
-        <v>43889.29</v>
+        <v>619.99</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1613,19 +1607,19 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D21">
         <v>33.73</v>
       </c>
       <c r="E21">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -1637,16 +1631,16 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K21">
-        <v>762.7</v>
+        <v>762.95</v>
       </c>
       <c r="L21">
-        <v>704.77</v>
+        <v>704.66</v>
       </c>
       <c r="M21">
-        <v>878.5599999999999</v>
+        <v>879.52</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1657,40 +1651,40 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D22">
-        <v>31.33</v>
+        <v>28.92</v>
       </c>
       <c r="E22">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G22">
-        <v>90.06</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K22">
-        <v>1424</v>
+        <v>424.95</v>
       </c>
       <c r="L22">
-        <v>1296.93</v>
+        <v>391.94</v>
       </c>
       <c r="M22">
-        <v>1678.14</v>
+        <v>490.98</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1701,40 +1695,40 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23">
-        <v>28.92</v>
+        <v>25.3</v>
       </c>
       <c r="E23">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23">
-        <v>84.04000000000001</v>
+        <v>75.23999999999999</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K23">
-        <v>424.95</v>
+        <v>1001.35</v>
       </c>
       <c r="L23">
-        <v>391.94</v>
+        <v>945.39</v>
       </c>
       <c r="M23">
-        <v>490.98</v>
+        <v>1113.26</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1745,40 +1739,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D24">
-        <v>25.3</v>
+        <v>24.1</v>
       </c>
       <c r="E24">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G24">
-        <v>75.23999999999999</v>
+        <v>70.42</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K24">
-        <v>1004.1</v>
+        <v>1201.4</v>
       </c>
       <c r="L24">
-        <v>948.14</v>
+        <v>1127.76</v>
       </c>
       <c r="M24">
-        <v>1116.01</v>
+        <v>1348.68</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1789,40 +1783,40 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
       </c>
       <c r="D25">
-        <v>22.89</v>
+        <v>20.48</v>
       </c>
       <c r="E25">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="G25">
-        <v>70.42</v>
+        <v>100</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K25">
-        <v>1205.1</v>
+        <v>5670</v>
       </c>
       <c r="L25">
-        <v>1130.61</v>
+        <v>5432.71</v>
       </c>
       <c r="M25">
-        <v>1354.07</v>
+        <v>6144.57</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1833,40 +1827,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26">
         <v>20.48</v>
       </c>
       <c r="E26">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>92.47</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K26">
-        <v>5670</v>
+        <v>303.45</v>
       </c>
       <c r="L26">
-        <v>5432.71</v>
+        <v>282.21</v>
       </c>
       <c r="M26">
-        <v>6144.57</v>
+        <v>345.92</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1877,22 +1871,22 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D27">
         <v>20.48</v>
       </c>
       <c r="E27">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G27">
-        <v>82.83</v>
+        <v>76.45</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1901,16 +1895,16 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K27">
-        <v>841.95</v>
+        <v>492.15</v>
       </c>
       <c r="L27">
-        <v>802.99</v>
+        <v>478.68</v>
       </c>
       <c r="M27">
-        <v>919.88</v>
+        <v>519.08</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1921,22 +1915,22 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28">
         <v>20.48</v>
       </c>
       <c r="E28">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G28">
-        <v>76.45</v>
+        <v>82.83</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1945,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K28">
-        <v>492.35</v>
+        <v>842.7</v>
       </c>
       <c r="L28">
-        <v>478.7</v>
+        <v>803.0599999999999</v>
       </c>
       <c r="M28">
-        <v>519.64</v>
+        <v>921.98</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1965,43 +1959,43 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D29">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E29">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
         <v>107</v>
       </c>
       <c r="G29">
-        <v>92.47</v>
+        <v>70.78</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K29">
-        <v>303.35</v>
+        <v>398.25</v>
       </c>
       <c r="L29">
-        <v>282.11</v>
+        <v>399.57</v>
       </c>
       <c r="M29">
-        <v>345.82</v>
+        <v>395.6</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2009,43 +2003,43 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30">
         <v>19.28</v>
       </c>
       <c r="E30">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G30">
-        <v>70.78</v>
+        <v>85.23999999999999</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K30">
-        <v>397.3</v>
+        <v>721.9</v>
       </c>
       <c r="L30">
-        <v>399.48</v>
+        <v>690.15</v>
       </c>
       <c r="M30">
-        <v>392.93</v>
+        <v>785.4</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2053,40 +2047,40 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D31">
-        <v>19.28</v>
+        <v>16.87</v>
       </c>
       <c r="E31">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
         <v>98</v>
       </c>
       <c r="G31">
-        <v>85.23999999999999</v>
+        <v>96.08</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K31">
-        <v>721.85</v>
+        <v>2671.4</v>
       </c>
       <c r="L31">
-        <v>690.14</v>
+        <v>2449.09</v>
       </c>
       <c r="M31">
-        <v>785.26</v>
+        <v>3116.03</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2097,19 +2091,19 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32">
         <v>16.87</v>
       </c>
       <c r="E32">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G32">
         <v>86.45</v>
@@ -2121,16 +2115,16 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K32">
-        <v>2059.9</v>
+        <v>2060.7</v>
       </c>
       <c r="L32">
-        <v>1927.72</v>
+        <v>1927.8</v>
       </c>
       <c r="M32">
-        <v>2324.25</v>
+        <v>2326.5</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2141,40 +2135,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D33">
-        <v>16.87</v>
+        <v>14.46</v>
       </c>
       <c r="E33">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G33">
-        <v>96.08</v>
+        <v>86.45</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K33">
-        <v>2679.1</v>
+        <v>503.55</v>
       </c>
       <c r="L33">
-        <v>2456.79</v>
+        <v>468.9</v>
       </c>
       <c r="M33">
-        <v>3123.73</v>
+        <v>572.84</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2185,40 +2179,40 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <v>14.46</v>
       </c>
       <c r="E34">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="F34" t="s">
         <v>98</v>
       </c>
       <c r="G34">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K34">
-        <v>503.95</v>
+        <v>1899.9</v>
       </c>
       <c r="L34">
-        <v>468.94</v>
+        <v>1797.25</v>
       </c>
       <c r="M34">
-        <v>573.97</v>
+        <v>2105.2</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2229,40 +2223,40 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D35">
-        <v>14.46</v>
+        <v>13.25</v>
       </c>
       <c r="E35">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G35">
-        <v>100</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K35">
-        <v>1898</v>
+        <v>463.35</v>
       </c>
       <c r="L35">
-        <v>1797.07</v>
+        <v>440.51</v>
       </c>
       <c r="M35">
-        <v>2099.86</v>
+        <v>509.03</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2273,22 +2267,22 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36">
-        <v>13.25</v>
+        <v>12.05</v>
       </c>
       <c r="E36">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G36">
-        <v>71.98999999999999</v>
+        <v>72.29000000000001</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2297,16 +2291,16 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K36">
-        <v>463.4</v>
+        <v>2020.1</v>
       </c>
       <c r="L36">
-        <v>440.52</v>
+        <v>1889.87</v>
       </c>
       <c r="M36">
-        <v>509.17</v>
+        <v>2280.57</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2317,40 +2311,40 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37">
-        <v>12.05</v>
+        <v>10.84</v>
       </c>
       <c r="E37">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G37">
-        <v>72.29000000000001</v>
+        <v>100</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K37">
-        <v>2020</v>
+        <v>982.85</v>
       </c>
       <c r="L37">
-        <v>1889.86</v>
+        <v>955.49</v>
       </c>
       <c r="M37">
-        <v>2280.28</v>
+        <v>1037.57</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2364,16 +2358,16 @@
         <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38">
-        <v>10.84</v>
+        <v>8.43</v>
       </c>
       <c r="E38">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G38">
         <v>100</v>
@@ -2385,16 +2379,16 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K38">
-        <v>398</v>
+        <v>617.85</v>
       </c>
       <c r="L38">
-        <v>380.36</v>
+        <v>597.51</v>
       </c>
       <c r="M38">
-        <v>433.28</v>
+        <v>658.54</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2405,40 +2399,40 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D39">
-        <v>10.84</v>
+        <v>8.43</v>
       </c>
       <c r="E39">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G39">
-        <v>100</v>
+        <v>81.27</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K39">
-        <v>983</v>
+        <v>72.06</v>
       </c>
       <c r="L39">
-        <v>955.51</v>
+        <v>70.03</v>
       </c>
       <c r="M39">
-        <v>1037.97</v>
+        <v>76.12</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2449,40 +2443,40 @@
         <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D40">
-        <v>8.43</v>
+        <v>47.35</v>
       </c>
       <c r="E40">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="G40">
-        <v>81.27</v>
+        <v>47.35</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K40">
-        <v>72.09999999999999</v>
+        <v>2145.8</v>
       </c>
       <c r="L40">
-        <v>70.03</v>
+        <v>2050.53</v>
       </c>
       <c r="M40">
-        <v>76.23</v>
+        <v>2336.34</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2493,40 +2487,40 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D41">
-        <v>7.23</v>
+        <v>44.94</v>
       </c>
       <c r="E41">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G41">
-        <v>100</v>
+        <v>44.94</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K41">
-        <v>617.2</v>
+        <v>447.8</v>
       </c>
       <c r="L41">
-        <v>596.89</v>
+        <v>426.24</v>
       </c>
       <c r="M41">
-        <v>657.83</v>
+        <v>490.93</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2537,19 +2531,19 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42">
         <v>44.94</v>
       </c>
       <c r="E42">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G42">
         <v>44.94</v>
@@ -2558,19 +2552,19 @@
         <v>1</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K42">
-        <v>447.85</v>
+        <v>941.6</v>
       </c>
       <c r="L42">
-        <v>426.24</v>
+        <v>897.79</v>
       </c>
       <c r="M42">
-        <v>491.07</v>
+        <v>1029.23</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2581,40 +2575,40 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43">
-        <v>44.94</v>
+        <v>44.58</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G43">
-        <v>44.94</v>
+        <v>44.58</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>2</v>
       </c>
       <c r="J43" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K43">
-        <v>943.8</v>
+        <v>204.35</v>
       </c>
       <c r="L43">
-        <v>898.01</v>
+        <v>191.91</v>
       </c>
       <c r="M43">
-        <v>1035.37</v>
+        <v>229.23</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2625,40 +2619,40 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D44">
-        <v>44.58</v>
+        <v>40.12</v>
       </c>
       <c r="E44">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G44">
-        <v>44.58</v>
+        <v>90.06</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K44">
-        <v>206.59</v>
+        <v>9390.5</v>
       </c>
       <c r="L44">
-        <v>194.25</v>
+        <v>8736.620000000001</v>
       </c>
       <c r="M44">
-        <v>231.27</v>
+        <v>10698.27</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2669,22 +2663,22 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D45">
-        <v>42.53</v>
+        <v>40.12</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G45">
-        <v>42.53</v>
+        <v>40.12</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2693,16 +2687,16 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K45">
-        <v>2150.2</v>
+        <v>48315</v>
       </c>
       <c r="L45">
-        <v>2050.95</v>
+        <v>46827.69</v>
       </c>
       <c r="M45">
-        <v>2348.71</v>
+        <v>51289.62</v>
       </c>
       <c r="N45">
         <v>2</v>
@@ -2713,40 +2707,40 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D46">
         <v>40.12</v>
       </c>
       <c r="E46">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G46">
-        <v>90.06</v>
+        <v>40.12</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K46">
-        <v>9390</v>
+        <v>2806.6</v>
       </c>
       <c r="L46">
-        <v>8736.57</v>
+        <v>2720.18</v>
       </c>
       <c r="M46">
-        <v>10696.86</v>
+        <v>2979.45</v>
       </c>
       <c r="N46">
         <v>2</v>
@@ -2757,40 +2751,40 @@
         <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D47">
-        <v>40.12</v>
+        <v>52.17</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G47">
-        <v>40.12</v>
+        <v>52.17</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K47">
-        <v>48385</v>
+        <v>4324.2</v>
       </c>
       <c r="L47">
-        <v>46834.36</v>
+        <v>4133.43</v>
       </c>
       <c r="M47">
-        <v>51486.29</v>
+        <v>4705.74</v>
       </c>
       <c r="N47">
         <v>2</v>
@@ -2804,37 +2798,37 @@
         <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D48">
-        <v>40.12</v>
+        <v>38.92</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G48">
-        <v>40.12</v>
+        <v>38.92</v>
       </c>
       <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K48">
-        <v>2810.3</v>
+        <v>377.25</v>
       </c>
       <c r="L48">
-        <v>2720.53</v>
+        <v>368.71</v>
       </c>
       <c r="M48">
-        <v>2989.84</v>
+        <v>394.33</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -2851,34 +2845,34 @@
         <v>95</v>
       </c>
       <c r="D49">
-        <v>52.17</v>
+        <v>36.14</v>
       </c>
       <c r="E49">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="F49" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G49">
-        <v>52.17</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49">
         <v>2</v>
       </c>
       <c r="J49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K49">
-        <v>4324</v>
+        <v>9669.5</v>
       </c>
       <c r="L49">
-        <v>4133.51</v>
+        <v>8906.860000000001</v>
       </c>
       <c r="M49">
-        <v>4704.97</v>
+        <v>11194.79</v>
       </c>
       <c r="N49">
         <v>2</v>
@@ -2889,40 +2883,40 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D50">
-        <v>38.92</v>
+        <v>34.1</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G50">
-        <v>38.92</v>
+        <v>34.1</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K50">
-        <v>377.6</v>
+        <v>414.75</v>
       </c>
       <c r="L50">
-        <v>368.74</v>
+        <v>407.92</v>
       </c>
       <c r="M50">
-        <v>395.32</v>
+        <v>428.4</v>
       </c>
       <c r="N50">
         <v>2</v>
@@ -2933,40 +2927,40 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
         <v>92</v>
       </c>
-      <c r="C51" t="s">
-        <v>94</v>
-      </c>
       <c r="D51">
-        <v>34.1</v>
+        <v>33.92</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G51">
-        <v>34.1</v>
+        <v>33.92</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K51">
-        <v>414.15</v>
+        <v>1733.8</v>
       </c>
       <c r="L51">
-        <v>407.87</v>
+        <v>1686.21</v>
       </c>
       <c r="M51">
-        <v>426.72</v>
+        <v>1828.97</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -2980,37 +2974,37 @@
         <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D52">
-        <v>33.92</v>
+        <v>32.89</v>
       </c>
       <c r="E52">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F52" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G52">
-        <v>33.92</v>
+        <v>38.92</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K52">
-        <v>1733.1</v>
+        <v>481.25</v>
       </c>
       <c r="L52">
-        <v>1685.59</v>
+        <v>479.24</v>
       </c>
       <c r="M52">
-        <v>1828.13</v>
+        <v>485.27</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -3021,19 +3015,19 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D53">
-        <v>33.73</v>
+        <v>27.71</v>
       </c>
       <c r="E53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G53">
         <v>33.73</v>
@@ -3045,16 +3039,16 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K53">
-        <v>4295.9</v>
+        <v>4281.4</v>
       </c>
       <c r="L53">
-        <v>4096.49</v>
+        <v>4081.99</v>
       </c>
       <c r="M53">
-        <v>4694.73</v>
+        <v>4680.23</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -3065,40 +3059,40 @@
         <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
         <v>94</v>
       </c>
       <c r="D54">
-        <v>32.89</v>
+        <v>27.71</v>
       </c>
       <c r="E54">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G54">
-        <v>38.92</v>
+        <v>38.55</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K54">
-        <v>481.7</v>
+        <v>1782.6</v>
       </c>
       <c r="L54">
-        <v>479.28</v>
+        <v>1716.57</v>
       </c>
       <c r="M54">
-        <v>486.54</v>
+        <v>1914.66</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -3109,40 +3103,40 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D55">
-        <v>31.33</v>
+        <v>22.89</v>
       </c>
       <c r="E55">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G55">
-        <v>65.59999999999999</v>
+        <v>22.89</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K55">
-        <v>9589</v>
+        <v>35195</v>
       </c>
       <c r="L55">
-        <v>8826.360000000001</v>
+        <v>33732.97</v>
       </c>
       <c r="M55">
-        <v>11114.29</v>
+        <v>38119.07</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -3153,40 +3147,40 @@
         <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D56">
-        <v>27.71</v>
+        <v>21.69</v>
       </c>
       <c r="E56">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F56" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G56">
-        <v>38.55</v>
+        <v>41.14</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K56">
-        <v>1782.8</v>
+        <v>460.05</v>
       </c>
       <c r="L56">
-        <v>1716.8</v>
+        <v>448.45</v>
       </c>
       <c r="M56">
-        <v>1914.8</v>
+        <v>483.24</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -3197,40 +3191,40 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D57">
-        <v>22.89</v>
+        <v>20.48</v>
       </c>
       <c r="E57">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F57" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G57">
-        <v>22.89</v>
+        <v>66.81</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K57">
-        <v>35100</v>
+        <v>5189.6</v>
       </c>
       <c r="L57">
-        <v>33731.42</v>
+        <v>4923.43</v>
       </c>
       <c r="M57">
-        <v>37837.16</v>
+        <v>5721.94</v>
       </c>
       <c r="N57">
         <v>2</v>
@@ -3241,43 +3235,43 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D58">
-        <v>21.69</v>
+        <v>20.48</v>
       </c>
       <c r="E58">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G58">
-        <v>41.14</v>
+        <v>20.48</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K58">
-        <v>460.05</v>
+        <v>746.3</v>
       </c>
       <c r="L58">
-        <v>448.45</v>
+        <v>756.73</v>
       </c>
       <c r="M58">
-        <v>483.24</v>
+        <v>725.45</v>
       </c>
       <c r="N58">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3285,19 +3279,19 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D59">
         <v>20.48</v>
       </c>
       <c r="E59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G59">
         <v>20.48</v>
@@ -3309,16 +3303,16 @@
         <v>0</v>
       </c>
       <c r="J59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K59">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="L59">
-        <v>3479.44</v>
+        <v>3479.34</v>
       </c>
       <c r="M59">
-        <v>3829.12</v>
+        <v>3826.31</v>
       </c>
       <c r="N59">
         <v>2</v>
@@ -3329,40 +3323,40 @@
         <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D60">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F60" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G60">
-        <v>20.48</v>
+        <v>39.76</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
       <c r="I60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K60">
-        <v>447.75</v>
+        <v>534.25</v>
       </c>
       <c r="L60">
-        <v>440.3</v>
+        <v>513</v>
       </c>
       <c r="M60">
-        <v>462.65</v>
+        <v>576.74</v>
       </c>
       <c r="N60">
         <v>2</v>
@@ -3373,40 +3367,40 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D61">
         <v>19.28</v>
       </c>
       <c r="E61">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="F61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G61">
-        <v>66.81</v>
+        <v>43.37</v>
       </c>
       <c r="H61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K61">
-        <v>5183.5</v>
+        <v>2759.1</v>
       </c>
       <c r="L61">
-        <v>4922.85</v>
+        <v>2641.55</v>
       </c>
       <c r="M61">
-        <v>5704.8</v>
+        <v>2994.2</v>
       </c>
       <c r="N61">
         <v>2</v>
@@ -3417,43 +3411,43 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C62" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D62">
-        <v>19.28</v>
+        <v>18.07</v>
       </c>
       <c r="E62">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G62">
-        <v>19.28</v>
+        <v>39.76</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K62">
-        <v>745.6</v>
+        <v>1356</v>
       </c>
       <c r="L62">
-        <v>756.66</v>
+        <v>1283.04</v>
       </c>
       <c r="M62">
-        <v>723.48</v>
+        <v>1501.91</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3461,40 +3455,40 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C63" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D63">
-        <v>19.28</v>
+        <v>14.46</v>
       </c>
       <c r="E63">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G63">
-        <v>43.37</v>
+        <v>20.48</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63">
         <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K63">
-        <v>2758.8</v>
+        <v>445.5</v>
       </c>
       <c r="L63">
-        <v>2641.59</v>
+        <v>440.09</v>
       </c>
       <c r="M63">
-        <v>2993.21</v>
+        <v>456.32</v>
       </c>
       <c r="N63">
         <v>2</v>
@@ -3505,40 +3499,40 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D64">
-        <v>19.28</v>
+        <v>12.05</v>
       </c>
       <c r="E64">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F64" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="G64">
-        <v>39.76</v>
+        <v>58.19</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K64">
-        <v>534.9</v>
+        <v>3099.1</v>
       </c>
       <c r="L64">
-        <v>513.0700000000001</v>
+        <v>2942.58</v>
       </c>
       <c r="M64">
-        <v>578.5700000000001</v>
+        <v>3412.14</v>
       </c>
       <c r="N64">
         <v>2</v>
@@ -3549,40 +3543,40 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C65" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D65">
-        <v>18.07</v>
+        <v>12.05</v>
       </c>
       <c r="E65">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="F65" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="G65">
-        <v>39.76</v>
+        <v>61.99</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K65">
-        <v>1349.4</v>
+        <v>16765</v>
       </c>
       <c r="L65">
-        <v>1278.49</v>
+        <v>16113.57</v>
       </c>
       <c r="M65">
-        <v>1491.23</v>
+        <v>18067.86</v>
       </c>
       <c r="N65">
         <v>2</v>
@@ -3593,40 +3587,40 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D66">
-        <v>15.66</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E66">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G66">
-        <v>21.69</v>
+        <v>26.51</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K66">
-        <v>1207.1</v>
+        <v>195.37</v>
       </c>
       <c r="L66">
-        <v>1170.53</v>
+        <v>187.38</v>
       </c>
       <c r="M66">
-        <v>1280.23</v>
+        <v>211.35</v>
       </c>
       <c r="N66">
         <v>2</v>
@@ -3637,22 +3631,22 @@
         <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D67">
-        <v>12.05</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="E67">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="G67">
-        <v>58.19</v>
+        <v>60.24</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3661,16 +3655,16 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K67">
-        <v>3101.3</v>
+        <v>522</v>
       </c>
       <c r="L67">
-        <v>2944.09</v>
+        <v>508.81</v>
       </c>
       <c r="M67">
-        <v>3415.73</v>
+        <v>548.38</v>
       </c>
       <c r="N67">
         <v>2</v>
@@ -3681,22 +3675,22 @@
         <v>80</v>
       </c>
       <c r="B68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" t="s">
         <v>92</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68">
+        <v>8.43</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+      <c r="F68" t="s">
         <v>96</v>
       </c>
-      <c r="D68">
-        <v>12.05</v>
-      </c>
-      <c r="E68">
-        <v>80</v>
-      </c>
-      <c r="F68" t="s">
-        <v>109</v>
-      </c>
       <c r="G68">
-        <v>61.99</v>
+        <v>39.76</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -3705,16 +3699,16 @@
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K68">
-        <v>16793</v>
+        <v>1726.4</v>
       </c>
       <c r="L68">
-        <v>16141.57</v>
+        <v>1702.39</v>
       </c>
       <c r="M68">
-        <v>18095.86</v>
+        <v>1774.43</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -3725,40 +3719,40 @@
         <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D69">
-        <v>10.84</v>
+        <v>4.82</v>
       </c>
       <c r="E69">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F69" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G69">
-        <v>26.51</v>
+        <v>14.46</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69">
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K69">
-        <v>195.53</v>
+        <v>995.15</v>
       </c>
       <c r="L69">
-        <v>187.39</v>
+        <v>969</v>
       </c>
       <c r="M69">
-        <v>211.8</v>
+        <v>1047.45</v>
       </c>
       <c r="N69">
         <v>2</v>
@@ -3769,130 +3763,42 @@
         <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D70">
-        <v>9.640000000000001</v>
+        <v>4.82</v>
       </c>
       <c r="E70">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F70" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G70">
         <v>30.12</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70">
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K70">
-        <v>607.35</v>
+        <v>606.65</v>
       </c>
       <c r="L70">
-        <v>582.41</v>
+        <v>582.26</v>
       </c>
       <c r="M70">
-        <v>657.23</v>
+        <v>655.4400000000001</v>
       </c>
       <c r="N70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
-      <c r="A71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" t="s">
-        <v>91</v>
-      </c>
-      <c r="C71" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71">
-        <v>9.640000000000001</v>
-      </c>
-      <c r="E71">
-        <v>45</v>
-      </c>
-      <c r="F71" t="s">
-        <v>98</v>
-      </c>
-      <c r="G71">
-        <v>60.24</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="J71" t="s">
-        <v>116</v>
-      </c>
-      <c r="K71">
-        <v>522.7</v>
-      </c>
-      <c r="L71">
-        <v>508.88</v>
-      </c>
-      <c r="M71">
-        <v>550.34</v>
-      </c>
-      <c r="N71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
-      <c r="A72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" t="s">
-        <v>87</v>
-      </c>
-      <c r="C72" t="s">
-        <v>97</v>
-      </c>
-      <c r="D72">
-        <v>4.82</v>
-      </c>
-      <c r="E72">
-        <v>17</v>
-      </c>
-      <c r="F72" t="s">
-        <v>98</v>
-      </c>
-      <c r="G72">
-        <v>14.46</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72" t="s">
-        <v>116</v>
-      </c>
-      <c r="K72">
-        <v>995</v>
-      </c>
-      <c r="L72">
-        <v>968.98</v>
-      </c>
-      <c r="M72">
-        <v>1047.03</v>
-      </c>
-      <c r="N72">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add comprehensive market regime correlation analysis with clear direction rules
</commit_message>
<xml_diff>
--- a/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
+++ b/Daily/G_Pattern_Master/G_Pattern_Master_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="113">
   <si>
     <t>Ticker</t>
   </si>
@@ -58,190 +58,193 @@
     <t>Risk_Reward</t>
   </si>
   <si>
+    <t>HEG</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>PAGEIND</t>
+  </si>
+  <si>
     <t>AMBER</t>
   </si>
   <si>
     <t>CIPLA</t>
   </si>
   <si>
-    <t>TORNTPHARM</t>
+    <t>GMMPFAUDLR</t>
+  </si>
+  <si>
+    <t>NUVOCO</t>
+  </si>
+  <si>
+    <t>GREAVESCOT</t>
+  </si>
+  <si>
+    <t>VBL</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>COROMANDEL</t>
+  </si>
+  <si>
+    <t>GATEWAY</t>
+  </si>
+  <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>SYRMA</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
+    <t>NAVA</t>
+  </si>
+  <si>
+    <t>EPACK</t>
+  </si>
+  <si>
+    <t>CRAFTSMAN</t>
+  </si>
+  <si>
+    <t>THERMAX</t>
+  </si>
+  <si>
+    <t>PGHH</t>
+  </si>
+  <si>
+    <t>ETERNAL</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>RRKABEL</t>
+  </si>
+  <si>
+    <t>PAYTM</t>
+  </si>
+  <si>
+    <t>FORTIS</t>
+  </si>
+  <si>
+    <t>GODREJCP</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>CUMMINSIND</t>
+  </si>
+  <si>
+    <t>AMBUJACEM</t>
+  </si>
+  <si>
+    <t>GLENMARK</t>
+  </si>
+  <si>
+    <t>RBLBANK</t>
+  </si>
+  <si>
+    <t>GRAPHITE</t>
+  </si>
+  <si>
+    <t>NIACL</t>
+  </si>
+  <si>
+    <t>VISHNU</t>
+  </si>
+  <si>
+    <t>SUMICHEM</t>
+  </si>
+  <si>
+    <t>JUBLINGREA</t>
+  </si>
+  <si>
+    <t>KAYNES</t>
+  </si>
+  <si>
+    <t>DEEPINDS</t>
+  </si>
+  <si>
+    <t>EMAMILTD</t>
+  </si>
+  <si>
+    <t>ALKYLAMINE</t>
+  </si>
+  <si>
+    <t>BALAMINES</t>
+  </si>
+  <si>
+    <t>FLUOROCHEM</t>
+  </si>
+  <si>
+    <t>HINDUNILVR</t>
+  </si>
+  <si>
+    <t>DMART</t>
+  </si>
+  <si>
+    <t>APLAPOLLO</t>
+  </si>
+  <si>
+    <t>ACI</t>
   </si>
   <si>
     <t>EIDPARRY</t>
   </si>
   <si>
-    <t>GSFC</t>
-  </si>
-  <si>
-    <t>CRAFTSMAN</t>
-  </si>
-  <si>
-    <t>SUMICHEM</t>
-  </si>
-  <si>
-    <t>VBL</t>
-  </si>
-  <si>
-    <t>VISHNU</t>
-  </si>
-  <si>
-    <t>GATEWAY</t>
-  </si>
-  <si>
-    <t>COROMANDEL</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>SYNGENE</t>
-  </si>
-  <si>
-    <t>PGHH</t>
-  </si>
-  <si>
-    <t>POWERINDIA</t>
-  </si>
-  <si>
-    <t>LAURUSLABS</t>
-  </si>
-  <si>
-    <t>SHYAMMETL</t>
-  </si>
-  <si>
-    <t>BOSCHLTD</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>SYRMA</t>
-  </si>
-  <si>
-    <t>NUVOCO</t>
-  </si>
-  <si>
-    <t>TATACHEM</t>
-  </si>
-  <si>
-    <t>RAMCOCEM</t>
-  </si>
-  <si>
-    <t>HDFCAMC</t>
-  </si>
-  <si>
-    <t>ETERNAL</t>
-  </si>
-  <si>
-    <t>GRANULES</t>
-  </si>
-  <si>
-    <t>FORTIS</t>
-  </si>
-  <si>
-    <t>PCBL</t>
-  </si>
-  <si>
-    <t>UPL</t>
-  </si>
-  <si>
-    <t>ANANDRATHI</t>
-  </si>
-  <si>
-    <t>GLAND</t>
-  </si>
-  <si>
-    <t>JGCHEM</t>
-  </si>
-  <si>
-    <t>PATANJALI</t>
-  </si>
-  <si>
-    <t>VIPIND</t>
-  </si>
-  <si>
-    <t>METROPOLIS</t>
-  </si>
-  <si>
-    <t>JINDALSTEL</t>
-  </si>
-  <si>
-    <t>AMBUJACEM</t>
-  </si>
-  <si>
-    <t>NMDC</t>
-  </si>
-  <si>
-    <t>CAPLIPOINT</t>
-  </si>
-  <si>
-    <t>STARHEALTH</t>
-  </si>
-  <si>
-    <t>WELCORP</t>
-  </si>
-  <si>
-    <t>NIACL</t>
-  </si>
-  <si>
-    <t>GODFRYPHLP</t>
-  </si>
-  <si>
-    <t>PAGEIND</t>
-  </si>
-  <si>
-    <t>MPHASIS</t>
-  </si>
-  <si>
-    <t>PIIND</t>
-  </si>
-  <si>
-    <t>BLS</t>
-  </si>
-  <si>
-    <t>APARINDS</t>
-  </si>
-  <si>
-    <t>BSOFT</t>
-  </si>
-  <si>
-    <t>SUNPHARMA</t>
-  </si>
-  <si>
-    <t>DBL</t>
-  </si>
-  <si>
-    <t>DMART</t>
+    <t>JIOFIN</t>
+  </si>
+  <si>
+    <t>BRITANNIA</t>
+  </si>
+  <si>
+    <t>MAHLIFE</t>
   </si>
   <si>
     <t>JBCHEPHARM</t>
   </si>
   <si>
-    <t>ABBOTINDIA</t>
-  </si>
-  <si>
-    <t>TMB</t>
-  </si>
-  <si>
-    <t>NAVINFLUOR</t>
-  </si>
-  <si>
-    <t>AUBANK</t>
-  </si>
-  <si>
-    <t>FLUOROCHEM</t>
-  </si>
-  <si>
-    <t>HEG</t>
-  </si>
-  <si>
-    <t>BALKRISIND</t>
-  </si>
-  <si>
-    <t>GMMPFAUDLR</t>
-  </si>
-  <si>
-    <t>AARTIIND</t>
+    <t>MARICO</t>
+  </si>
+  <si>
+    <t>AWHCL</t>
+  </si>
+  <si>
+    <t>COLPAL</t>
+  </si>
+  <si>
+    <t>INFY</t>
+  </si>
+  <si>
+    <t>CGCL</t>
+  </si>
+  <si>
+    <t>ICICIBANK</t>
+  </si>
+  <si>
+    <t>ICICIGI</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>TECHM</t>
   </si>
   <si>
     <t>LALPATHLAB</t>
@@ -250,19 +253,13 @@
     <t>DIXON</t>
   </si>
   <si>
-    <t>GPIL</t>
-  </si>
-  <si>
-    <t>DABUR</t>
-  </si>
-  <si>
-    <t>BALAMINES</t>
-  </si>
-  <si>
-    <t>ZYDUSLIFE</t>
-  </si>
-  <si>
-    <t>KALYANKJIL</t>
+    <t>JKCEMENT</t>
+  </si>
+  <si>
+    <t>Industrials</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
   <si>
     <t>Consumer Cyclical</t>
@@ -271,21 +268,18 @@
     <t>Healthcare</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Basic Materials</t>
   </si>
   <si>
-    <t>Industrials</t>
-  </si>
-  <si>
     <t>Financial Services</t>
   </si>
   <si>
     <t>Consumer Defensive</t>
   </si>
   <si>
+    <t>Energy</t>
+  </si>
+  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -304,16 +298,16 @@
     <t>Early_Setup</t>
   </si>
   <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
     <t>2025-07-07</t>
   </si>
   <si>
     <t>2025-07-25</t>
   </si>
   <si>
-    <t>2025-07-15</t>
-  </si>
-  <si>
-    <t>2025-07-24</t>
+    <t>2025-07-11</t>
   </si>
   <si>
     <t>2025-07-16</t>
@@ -328,22 +322,22 @@
     <t>2025-07-17</t>
   </si>
   <si>
-    <t>2025-07-11</t>
-  </si>
-  <si>
     <t>2025-07-22</t>
   </si>
   <si>
     <t>2025-07-08</t>
   </si>
   <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
     <t>2025-07-09</t>
   </si>
   <si>
+    <t>2025-07-10</t>
+  </si>
+  <si>
     <t>2025-07-21</t>
-  </si>
-  <si>
-    <t>2025-07-18</t>
   </si>
   <si>
     <t>G PATTERN DEVELOPING - DOUBLE POSITION (50%)</t>
@@ -716,7 +710,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -771,19 +765,19 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -792,19 +786,19 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K2">
-        <v>8040.5</v>
+        <v>608.45</v>
       </c>
       <c r="L2">
-        <v>7469.93</v>
+        <v>559.1</v>
       </c>
       <c r="M2">
-        <v>9181.639999999999</v>
+        <v>707.15</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -815,19 +809,19 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3">
-        <v>49.4</v>
+        <v>51.81</v>
       </c>
       <c r="E3">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -836,19 +830,19 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K3">
-        <v>1559.4</v>
+        <v>3730.4</v>
       </c>
       <c r="L3">
-        <v>1505.56</v>
+        <v>3586.77</v>
       </c>
       <c r="M3">
-        <v>1667.09</v>
+        <v>4017.66</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -859,22 +853,22 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4">
-        <v>49.4</v>
+        <v>50.78</v>
       </c>
       <c r="E4">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G4">
-        <v>100</v>
+        <v>50.78</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -883,16 +877,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K4">
-        <v>3730.6</v>
+        <v>49025</v>
       </c>
       <c r="L4">
-        <v>3585.1</v>
+        <v>46965.07</v>
       </c>
       <c r="M4">
-        <v>4021.6</v>
+        <v>53144.86</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -903,40 +897,40 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5">
-        <v>60.78</v>
+        <v>50.6</v>
       </c>
       <c r="E5">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5">
-        <v>60.78</v>
+        <v>100</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K5">
-        <v>1236.2</v>
+        <v>7989</v>
       </c>
       <c r="L5">
-        <v>1166.47</v>
+        <v>7452.93</v>
       </c>
       <c r="M5">
-        <v>1375.66</v>
+        <v>9061.139999999999</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -947,40 +941,40 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D6">
-        <v>53.37</v>
+        <v>39.76</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G6">
-        <v>53.37</v>
+        <v>100</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K6">
-        <v>207.58</v>
+        <v>1556.1</v>
       </c>
       <c r="L6">
-        <v>200.89</v>
+        <v>1501.93</v>
       </c>
       <c r="M6">
-        <v>220.96</v>
+        <v>1664.44</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -991,22 +985,22 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <v>94.88</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="E7">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1015,16 +1009,16 @@
         <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K7">
-        <v>6863.5</v>
+        <v>1381.4</v>
       </c>
       <c r="L7">
-        <v>6390.36</v>
+        <v>1300.4</v>
       </c>
       <c r="M7">
-        <v>7809.79</v>
+        <v>1543.4</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -1035,40 +1029,40 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D8">
-        <v>94.88</v>
+        <v>53.55</v>
       </c>
       <c r="E8">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G8">
-        <v>100</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K8">
-        <v>652.25</v>
+        <v>434.75</v>
       </c>
       <c r="L8">
-        <v>607.64</v>
+        <v>400.59</v>
       </c>
       <c r="M8">
-        <v>741.48</v>
+        <v>503.06</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1079,22 +1073,22 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9">
-        <v>92.47</v>
+        <v>91.27</v>
       </c>
       <c r="E9">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>91.27</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1103,16 +1097,16 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K9">
-        <v>522.1</v>
+        <v>233.15</v>
       </c>
       <c r="L9">
-        <v>496.01</v>
+        <v>214.33</v>
       </c>
       <c r="M9">
-        <v>574.29</v>
+        <v>270.79</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -1123,40 +1117,40 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10">
-        <v>91.27</v>
+        <v>39.76</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G10">
-        <v>91.27</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K10">
-        <v>564.35</v>
+        <v>522.45</v>
       </c>
       <c r="L10">
-        <v>525.7</v>
+        <v>496.23</v>
       </c>
       <c r="M10">
-        <v>641.65</v>
+        <v>574.89</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -1167,22 +1161,22 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11">
-        <v>88.86</v>
+        <v>33.73</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G11">
-        <v>91.27</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1191,16 +1185,16 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K11">
-        <v>71.29000000000001</v>
+        <v>40315</v>
       </c>
       <c r="L11">
-        <v>66.65000000000001</v>
+        <v>38387.86</v>
       </c>
       <c r="M11">
-        <v>80.58</v>
+        <v>44169.29</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -1211,40 +1205,40 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12">
-        <v>86.45</v>
+        <v>33.73</v>
       </c>
       <c r="E12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G12">
-        <v>86.45</v>
+        <v>82.83</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K12">
-        <v>2652.7</v>
+        <v>3660.4</v>
       </c>
       <c r="L12">
-        <v>2481.09</v>
+        <v>3542.01</v>
       </c>
       <c r="M12">
-        <v>2995.93</v>
+        <v>3897.17</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -1255,22 +1249,22 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>93</v>
       </c>
       <c r="D13">
-        <v>82.83</v>
+        <v>31.33</v>
       </c>
       <c r="E13">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G13">
-        <v>82.83</v>
+        <v>100</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1279,16 +1273,16 @@
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K13">
-        <v>3665.1</v>
+        <v>715.15</v>
       </c>
       <c r="L13">
-        <v>3545.71</v>
+        <v>672.61</v>
       </c>
       <c r="M13">
-        <v>3903.87</v>
+        <v>800.22</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -1299,40 +1293,40 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14">
-        <v>81.63</v>
+        <v>31.33</v>
       </c>
       <c r="E14">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G14">
-        <v>100</v>
+        <v>86.45</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K14">
-        <v>722.05</v>
+        <v>2644.1</v>
       </c>
       <c r="L14">
-        <v>680.46</v>
+        <v>2470.94</v>
       </c>
       <c r="M14">
-        <v>805.24</v>
+        <v>2990.41</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -1343,22 +1337,22 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>93</v>
       </c>
       <c r="D15">
-        <v>81.63</v>
+        <v>31.33</v>
       </c>
       <c r="E15">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G15">
-        <v>81.63</v>
+        <v>91.27</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1367,16 +1361,16 @@
         <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K15">
-        <v>13805</v>
+        <v>71.20999999999999</v>
       </c>
       <c r="L15">
-        <v>13263.57</v>
+        <v>66.26000000000001</v>
       </c>
       <c r="M15">
-        <v>14887.86</v>
+        <v>81.11</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -1387,22 +1381,22 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>93</v>
       </c>
       <c r="D16">
-        <v>53.37</v>
+        <v>28.92</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G16">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1411,16 +1405,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K16">
-        <v>20825</v>
+        <v>987.6</v>
       </c>
       <c r="L16">
-        <v>19132.86</v>
+        <v>926.95</v>
       </c>
       <c r="M16">
-        <v>24209.29</v>
+        <v>1108.9</v>
       </c>
       <c r="N16">
         <v>2</v>
@@ -1431,40 +1425,40 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D17">
-        <v>38.55</v>
+        <v>28.92</v>
       </c>
       <c r="E17">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17">
-        <v>89.88</v>
+        <v>100</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K17">
-        <v>881.45</v>
+        <v>758.5</v>
       </c>
       <c r="L17">
-        <v>832.17</v>
+        <v>700.35</v>
       </c>
       <c r="M17">
-        <v>980.01</v>
+        <v>874.8</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -1475,40 +1469,40 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18">
-        <v>37.35</v>
+        <v>26.51</v>
       </c>
       <c r="E18">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G18">
-        <v>100</v>
+        <v>89.88</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K18">
-        <v>985.6</v>
+        <v>871</v>
       </c>
       <c r="L18">
-        <v>928.72</v>
+        <v>821.01</v>
       </c>
       <c r="M18">
-        <v>1099.36</v>
+        <v>970.99</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -1519,40 +1513,40 @@
         <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19">
-        <v>34.94</v>
+        <v>26.51</v>
       </c>
       <c r="E19">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>75.42</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K19">
-        <v>40060</v>
+        <v>629.9</v>
       </c>
       <c r="L19">
-        <v>38107.86</v>
+        <v>595.02</v>
       </c>
       <c r="M19">
-        <v>43964.29</v>
+        <v>699.65</v>
       </c>
       <c r="N19">
         <v>2</v>
@@ -1563,22 +1557,22 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20">
-        <v>34.94</v>
+        <v>26.51</v>
       </c>
       <c r="E20">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G20">
-        <v>100</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1587,16 +1581,16 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K20">
-        <v>498.3</v>
+        <v>390</v>
       </c>
       <c r="L20">
-        <v>437.46</v>
+        <v>357.81</v>
       </c>
       <c r="M20">
-        <v>619.99</v>
+        <v>454.37</v>
       </c>
       <c r="N20">
         <v>2</v>
@@ -1607,40 +1601,40 @@
         <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21">
-        <v>33.73</v>
+        <v>22.89</v>
       </c>
       <c r="E21">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21">
         <v>100</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K21">
-        <v>762.95</v>
+        <v>6652.5</v>
       </c>
       <c r="L21">
-        <v>704.66</v>
+        <v>6163.21</v>
       </c>
       <c r="M21">
-        <v>879.52</v>
+        <v>7631.07</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -1651,40 +1645,40 @@
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D22">
-        <v>28.92</v>
+        <v>22.89</v>
       </c>
       <c r="E22">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G22">
-        <v>84.04000000000001</v>
+        <v>100</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K22">
-        <v>424.95</v>
+        <v>3885.5</v>
       </c>
       <c r="L22">
-        <v>391.94</v>
+        <v>3647.01</v>
       </c>
       <c r="M22">
-        <v>490.98</v>
+        <v>4362.48</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -1695,40 +1689,40 @@
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D23">
-        <v>25.3</v>
+        <v>22.89</v>
       </c>
       <c r="E23">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G23">
-        <v>75.23999999999999</v>
+        <v>81.63</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K23">
-        <v>1001.35</v>
+        <v>13696</v>
       </c>
       <c r="L23">
-        <v>945.39</v>
+        <v>13155.89</v>
       </c>
       <c r="M23">
-        <v>1113.26</v>
+        <v>14776.22</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -1739,40 +1733,40 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
         <v>92</v>
       </c>
       <c r="D24">
-        <v>24.1</v>
+        <v>22.89</v>
       </c>
       <c r="E24">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="G24">
-        <v>70.42</v>
+        <v>92.47</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K24">
-        <v>1201.4</v>
+        <v>309.4</v>
       </c>
       <c r="L24">
-        <v>1127.76</v>
+        <v>287.35</v>
       </c>
       <c r="M24">
-        <v>1348.68</v>
+        <v>353.5</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -1783,19 +1777,19 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D25">
         <v>20.48</v>
       </c>
       <c r="E25">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F25" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G25">
         <v>100</v>
@@ -1807,16 +1801,16 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K25">
-        <v>5670</v>
+        <v>5692</v>
       </c>
       <c r="L25">
-        <v>5432.71</v>
+        <v>5455.5</v>
       </c>
       <c r="M25">
-        <v>6144.57</v>
+        <v>6165</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -1827,40 +1821,40 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D26">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E26">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G26">
-        <v>92.47</v>
+        <v>100</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K26">
-        <v>303.45</v>
+        <v>1438</v>
       </c>
       <c r="L26">
-        <v>282.21</v>
+        <v>1372.09</v>
       </c>
       <c r="M26">
-        <v>345.92</v>
+        <v>1569.83</v>
       </c>
       <c r="N26">
         <v>2</v>
@@ -1871,40 +1865,40 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27">
-        <v>20.48</v>
+        <v>16.87</v>
       </c>
       <c r="E27">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
+        <v>97</v>
+      </c>
+      <c r="G27">
         <v>100</v>
       </c>
-      <c r="G27">
-        <v>76.45</v>
-      </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K27">
-        <v>492.15</v>
+        <v>1084.75</v>
       </c>
       <c r="L27">
-        <v>478.68</v>
+        <v>1006.84</v>
       </c>
       <c r="M27">
-        <v>519.08</v>
+        <v>1240.56</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -1915,40 +1909,40 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <v>15.66</v>
+      </c>
+      <c r="E28">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
         <v>95</v>
-      </c>
-      <c r="D28">
-        <v>20.48</v>
-      </c>
-      <c r="E28">
-        <v>48</v>
-      </c>
-      <c r="F28" t="s">
-        <v>96</v>
       </c>
       <c r="G28">
         <v>82.83</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K28">
-        <v>842.7</v>
+        <v>851.25</v>
       </c>
       <c r="L28">
-        <v>803.0599999999999</v>
+        <v>811.08</v>
       </c>
       <c r="M28">
-        <v>921.98</v>
+        <v>931.59</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -1959,22 +1953,22 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29">
-        <v>19.28</v>
+        <v>14.46</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G29">
-        <v>70.78</v>
+        <v>100</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1983,19 +1977,19 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K29">
-        <v>398.25</v>
+        <v>1260.1</v>
       </c>
       <c r="L29">
-        <v>399.57</v>
+        <v>1222.77</v>
       </c>
       <c r="M29">
-        <v>395.6</v>
+        <v>1334.76</v>
       </c>
       <c r="N29">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2003,40 +1997,40 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D30">
-        <v>19.28</v>
+        <v>14.46</v>
       </c>
       <c r="E30">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G30">
-        <v>85.23999999999999</v>
+        <v>100</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K30">
-        <v>721.9</v>
+        <v>972.9</v>
       </c>
       <c r="L30">
-        <v>690.15</v>
+        <v>883.46</v>
       </c>
       <c r="M30">
-        <v>785.4</v>
+        <v>1151.79</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -2047,22 +2041,22 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31">
-        <v>16.87</v>
+        <v>14.46</v>
       </c>
       <c r="E31">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F31" t="s">
         <v>98</v>
       </c>
       <c r="G31">
-        <v>96.08</v>
+        <v>100</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2071,16 +2065,16 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K31">
-        <v>2671.4</v>
+        <v>489.75</v>
       </c>
       <c r="L31">
-        <v>2449.09</v>
+        <v>427.88</v>
       </c>
       <c r="M31">
-        <v>3116.03</v>
+        <v>613.49</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -2091,22 +2085,22 @@
         <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D32">
-        <v>16.87</v>
+        <v>13.25</v>
       </c>
       <c r="E32">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G32">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -2115,16 +2109,16 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K32">
-        <v>2060.7</v>
+        <v>3594</v>
       </c>
       <c r="L32">
-        <v>1927.8</v>
+        <v>3482.9</v>
       </c>
       <c r="M32">
-        <v>2326.5</v>
+        <v>3816.2</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -2135,40 +2129,40 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33">
+        <v>7.23</v>
+      </c>
+      <c r="E33">
         <v>85</v>
       </c>
-      <c r="C33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33">
-        <v>14.46</v>
-      </c>
-      <c r="E33">
-        <v>20</v>
-      </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33">
-        <v>86.45</v>
+        <v>100</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K33">
-        <v>503.55</v>
+        <v>619.2</v>
       </c>
       <c r="L33">
-        <v>468.9</v>
+        <v>598.4299999999999</v>
       </c>
       <c r="M33">
-        <v>572.84</v>
+        <v>660.74</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -2179,22 +2173,22 @@
         <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34">
+        <v>4.82</v>
+      </c>
+      <c r="E34">
+        <v>65</v>
+      </c>
+      <c r="F34" t="s">
         <v>95</v>
       </c>
-      <c r="D34">
-        <v>14.46</v>
-      </c>
-      <c r="E34">
-        <v>66</v>
-      </c>
-      <c r="F34" t="s">
-        <v>98</v>
-      </c>
       <c r="G34">
-        <v>100</v>
+        <v>73.01000000000001</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2203,16 +2197,16 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K34">
-        <v>1899.9</v>
+        <v>2150.6</v>
       </c>
       <c r="L34">
-        <v>1797.25</v>
+        <v>2046.61</v>
       </c>
       <c r="M34">
-        <v>2105.2</v>
+        <v>2358.58</v>
       </c>
       <c r="N34">
         <v>2</v>
@@ -2223,40 +2217,40 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35">
-        <v>13.25</v>
+        <v>44.94</v>
       </c>
       <c r="E35">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G35">
-        <v>71.98999999999999</v>
+        <v>49.4</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K35">
-        <v>463.35</v>
+        <v>270</v>
       </c>
       <c r="L35">
-        <v>440.51</v>
+        <v>253.13</v>
       </c>
       <c r="M35">
-        <v>509.03</v>
+        <v>303.75</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -2267,40 +2261,40 @@
         <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D36">
-        <v>12.05</v>
+        <v>44.94</v>
       </c>
       <c r="E36">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G36">
-        <v>72.29000000000001</v>
+        <v>44.94</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K36">
-        <v>2020.1</v>
+        <v>586.85</v>
       </c>
       <c r="L36">
-        <v>1889.87</v>
+        <v>553.28</v>
       </c>
       <c r="M36">
-        <v>2280.57</v>
+        <v>654</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -2311,40 +2305,40 @@
         <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D37">
-        <v>10.84</v>
+        <v>43.37</v>
       </c>
       <c r="E37">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G37">
-        <v>100</v>
+        <v>90.06</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K37">
-        <v>982.85</v>
+        <v>205.9</v>
       </c>
       <c r="L37">
-        <v>955.49</v>
+        <v>191.19</v>
       </c>
       <c r="M37">
-        <v>1037.57</v>
+        <v>235.32</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -2355,40 +2349,40 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D38">
-        <v>8.43</v>
+        <v>42.17</v>
       </c>
       <c r="E38">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G38">
-        <v>100</v>
+        <v>91.27</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K38">
-        <v>617.85</v>
+        <v>574.85</v>
       </c>
       <c r="L38">
-        <v>597.51</v>
+        <v>532.21</v>
       </c>
       <c r="M38">
-        <v>658.54</v>
+        <v>660.14</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -2399,40 +2393,40 @@
         <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
         <v>92</v>
       </c>
       <c r="D39">
-        <v>8.43</v>
+        <v>40.96</v>
       </c>
       <c r="E39">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G39">
-        <v>81.27</v>
+        <v>100</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K39">
-        <v>72.06</v>
+        <v>648.5</v>
       </c>
       <c r="L39">
-        <v>70.03</v>
+        <v>601.87</v>
       </c>
       <c r="M39">
-        <v>76.12</v>
+        <v>741.76</v>
       </c>
       <c r="N39">
         <v>2</v>
@@ -2446,37 +2440,37 @@
         <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D40">
-        <v>47.35</v>
+        <v>63.19</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G40">
-        <v>47.35</v>
+        <v>63.19</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I40">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K40">
-        <v>2145.8</v>
+        <v>835.15</v>
       </c>
       <c r="L40">
-        <v>2050.53</v>
+        <v>788.1</v>
       </c>
       <c r="M40">
-        <v>2336.34</v>
+        <v>929.26</v>
       </c>
       <c r="N40">
         <v>2</v>
@@ -2487,40 +2481,40 @@
         <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41">
-        <v>44.94</v>
+        <v>52.17</v>
       </c>
       <c r="E41">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G41">
-        <v>44.94</v>
+        <v>88.86</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K41">
-        <v>447.8</v>
+        <v>6183.5</v>
       </c>
       <c r="L41">
-        <v>426.24</v>
+        <v>5780.36</v>
       </c>
       <c r="M41">
-        <v>490.93</v>
+        <v>6989.79</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -2531,40 +2525,40 @@
         <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D42">
-        <v>44.94</v>
+        <v>34.94</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F42" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G42">
-        <v>44.94</v>
+        <v>34.94</v>
       </c>
       <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K42">
-        <v>941.6</v>
+        <v>489</v>
       </c>
       <c r="L42">
-        <v>897.79</v>
+        <v>449.87</v>
       </c>
       <c r="M42">
-        <v>1029.23</v>
+        <v>567.26</v>
       </c>
       <c r="N42">
         <v>2</v>
@@ -2575,40 +2569,40 @@
         <v>55</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D43">
-        <v>44.58</v>
+        <v>34.1</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G43">
-        <v>44.58</v>
+        <v>40.96</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K43">
-        <v>204.35</v>
+        <v>593.5</v>
       </c>
       <c r="L43">
-        <v>191.91</v>
+        <v>571.3200000000001</v>
       </c>
       <c r="M43">
-        <v>229.23</v>
+        <v>637.87</v>
       </c>
       <c r="N43">
         <v>2</v>
@@ -2619,40 +2613,40 @@
         <v>56</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D44">
-        <v>40.12</v>
+        <v>33.92</v>
       </c>
       <c r="E44">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F44" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G44">
-        <v>90.06</v>
+        <v>33.92</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K44">
-        <v>9390.5</v>
+        <v>2355.1</v>
       </c>
       <c r="L44">
-        <v>8736.620000000001</v>
+        <v>2214.54</v>
       </c>
       <c r="M44">
-        <v>10698.27</v>
+        <v>2636.21</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2663,40 +2657,40 @@
         <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D45">
-        <v>40.12</v>
+        <v>32.71</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G45">
-        <v>40.12</v>
+        <v>39.76</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K45">
-        <v>48315</v>
+        <v>1797.5</v>
       </c>
       <c r="L45">
-        <v>46827.69</v>
+        <v>1707.29</v>
       </c>
       <c r="M45">
-        <v>51289.62</v>
+        <v>1977.92</v>
       </c>
       <c r="N45">
         <v>2</v>
@@ -2707,40 +2701,40 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D46">
-        <v>40.12</v>
+        <v>32.71</v>
       </c>
       <c r="E46">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G46">
-        <v>40.12</v>
+        <v>32.71</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K46">
-        <v>2806.6</v>
+        <v>3610.6</v>
       </c>
       <c r="L46">
-        <v>2720.18</v>
+        <v>3485.35</v>
       </c>
       <c r="M46">
-        <v>2979.45</v>
+        <v>3861.11</v>
       </c>
       <c r="N46">
         <v>2</v>
@@ -2751,40 +2745,40 @@
         <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D47">
-        <v>52.17</v>
+        <v>30.12</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G47">
-        <v>52.17</v>
+        <v>63.86</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K47">
-        <v>4324.2</v>
+        <v>2541</v>
       </c>
       <c r="L47">
-        <v>4133.43</v>
+        <v>2457.97</v>
       </c>
       <c r="M47">
-        <v>4705.74</v>
+        <v>2707.06</v>
       </c>
       <c r="N47">
         <v>2</v>
@@ -2795,40 +2789,40 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D48">
-        <v>38.92</v>
+        <v>28.92</v>
       </c>
       <c r="E48">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G48">
-        <v>38.92</v>
+        <v>36.14</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48">
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K48">
-        <v>377.25</v>
+        <v>4297.3</v>
       </c>
       <c r="L48">
-        <v>368.71</v>
+        <v>4102.49</v>
       </c>
       <c r="M48">
-        <v>394.33</v>
+        <v>4686.93</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -2839,43 +2833,43 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D49">
-        <v>36.14</v>
+        <v>26.51</v>
       </c>
       <c r="E49">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="F49" t="s">
         <v>104</v>
       </c>
       <c r="G49">
-        <v>65.59999999999999</v>
+        <v>26.51</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <v>2</v>
       </c>
       <c r="J49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K49">
-        <v>9669.5</v>
+        <v>1601</v>
       </c>
       <c r="L49">
-        <v>8906.860000000001</v>
+        <v>1625.51</v>
       </c>
       <c r="M49">
-        <v>11194.79</v>
+        <v>1551.98</v>
       </c>
       <c r="N49">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -2883,40 +2877,40 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s">
         <v>90</v>
       </c>
-      <c r="C50" t="s">
-        <v>92</v>
-      </c>
       <c r="D50">
-        <v>34.1</v>
+        <v>26.51</v>
       </c>
       <c r="E50">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G50">
-        <v>34.1</v>
+        <v>58.19</v>
       </c>
       <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K50">
-        <v>414.75</v>
+        <v>672.65</v>
       </c>
       <c r="L50">
-        <v>407.92</v>
+        <v>654.7</v>
       </c>
       <c r="M50">
-        <v>428.4</v>
+        <v>708.55</v>
       </c>
       <c r="N50">
         <v>2</v>
@@ -2927,40 +2921,40 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
         <v>92</v>
       </c>
       <c r="D51">
-        <v>33.92</v>
+        <v>24.1</v>
       </c>
       <c r="E51">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="F51" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G51">
-        <v>33.92</v>
+        <v>60.78</v>
       </c>
       <c r="H51">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K51">
-        <v>1733.8</v>
+        <v>1236.1</v>
       </c>
       <c r="L51">
-        <v>1686.21</v>
+        <v>1169.13</v>
       </c>
       <c r="M51">
-        <v>1828.97</v>
+        <v>1370.04</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -2971,40 +2965,40 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D52">
-        <v>32.89</v>
+        <v>22.89</v>
       </c>
       <c r="E52">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G52">
-        <v>38.92</v>
+        <v>22.89</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K52">
-        <v>481.25</v>
+        <v>330.15</v>
       </c>
       <c r="L52">
-        <v>479.24</v>
+        <v>314.56</v>
       </c>
       <c r="M52">
-        <v>485.27</v>
+        <v>361.34</v>
       </c>
       <c r="N52">
         <v>2</v>
@@ -3015,40 +3009,40 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D53">
-        <v>27.71</v>
+        <v>21.69</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G53">
-        <v>33.73</v>
+        <v>21.69</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K53">
-        <v>4281.4</v>
+        <v>5814</v>
       </c>
       <c r="L53">
-        <v>4081.99</v>
+        <v>5674.27</v>
       </c>
       <c r="M53">
-        <v>4680.23</v>
+        <v>6093.46</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -3059,40 +3053,40 @@
         <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D54">
-        <v>27.71</v>
+        <v>21.69</v>
       </c>
       <c r="E54">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F54" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G54">
-        <v>38.55</v>
+        <v>34.94</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54">
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K54">
-        <v>1782.6</v>
+        <v>364.15</v>
       </c>
       <c r="L54">
-        <v>1716.57</v>
+        <v>360.24</v>
       </c>
       <c r="M54">
-        <v>1914.66</v>
+        <v>371.97</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -3103,40 +3097,40 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D55">
-        <v>22.89</v>
+        <v>19.28</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="F55" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G55">
-        <v>22.89</v>
+        <v>38.55</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55">
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K55">
-        <v>35195</v>
+        <v>1773.9</v>
       </c>
       <c r="L55">
-        <v>33732.97</v>
+        <v>1705.49</v>
       </c>
       <c r="M55">
-        <v>38119.07</v>
+        <v>1910.73</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -3147,40 +3141,40 @@
         <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56">
+        <v>19.28</v>
+      </c>
+      <c r="E56">
+        <v>14</v>
+      </c>
+      <c r="F56" t="s">
         <v>95</v>
       </c>
-      <c r="D56">
-        <v>21.69</v>
-      </c>
-      <c r="E56">
-        <v>51</v>
-      </c>
-      <c r="F56" t="s">
-        <v>100</v>
-      </c>
       <c r="G56">
-        <v>41.14</v>
+        <v>22.89</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K56">
-        <v>460.05</v>
+        <v>712.65</v>
       </c>
       <c r="L56">
-        <v>448.45</v>
+        <v>706.16</v>
       </c>
       <c r="M56">
-        <v>483.24</v>
+        <v>725.62</v>
       </c>
       <c r="N56">
         <v>2</v>
@@ -3191,40 +3185,40 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D57">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E57">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G57">
-        <v>66.81</v>
+        <v>19.28</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K57">
-        <v>5189.6</v>
+        <v>623.6</v>
       </c>
       <c r="L57">
-        <v>4923.43</v>
+        <v>617.79</v>
       </c>
       <c r="M57">
-        <v>5721.94</v>
+        <v>635.23</v>
       </c>
       <c r="N57">
         <v>2</v>
@@ -3235,22 +3229,22 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D58">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E58">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G58">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -3259,16 +3253,16 @@
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K58">
-        <v>746.3</v>
+        <v>2255</v>
       </c>
       <c r="L58">
-        <v>756.73</v>
+        <v>2300.65</v>
       </c>
       <c r="M58">
-        <v>725.45</v>
+        <v>2163.7</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -3279,43 +3273,43 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D59">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="E59">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F59" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G59">
-        <v>20.48</v>
+        <v>19.28</v>
       </c>
       <c r="H59">
         <v>1</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K59">
-        <v>3595</v>
+        <v>1522.5</v>
       </c>
       <c r="L59">
-        <v>3479.34</v>
+        <v>1547.32</v>
       </c>
       <c r="M59">
-        <v>3826.31</v>
+        <v>1472.86</v>
       </c>
       <c r="N59">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3323,22 +3317,22 @@
         <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D60">
-        <v>19.28</v>
+        <v>15.66</v>
       </c>
       <c r="E60">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G60">
-        <v>39.76</v>
+        <v>32.53</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -3347,16 +3341,16 @@
         <v>0</v>
       </c>
       <c r="J60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K60">
-        <v>534.25</v>
+        <v>187.88</v>
       </c>
       <c r="L60">
-        <v>513</v>
+        <v>176.67</v>
       </c>
       <c r="M60">
-        <v>576.74</v>
+        <v>210.31</v>
       </c>
       <c r="N60">
         <v>2</v>
@@ -3367,40 +3361,40 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D61">
-        <v>19.28</v>
+        <v>14.46</v>
       </c>
       <c r="E61">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="F61" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="G61">
-        <v>43.37</v>
+        <v>63.37</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K61">
-        <v>2759.1</v>
+        <v>1492.2</v>
       </c>
       <c r="L61">
-        <v>2641.55</v>
+        <v>1455.37</v>
       </c>
       <c r="M61">
-        <v>2994.2</v>
+        <v>1565.86</v>
       </c>
       <c r="N61">
         <v>2</v>
@@ -3411,40 +3405,40 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62">
+        <v>13.25</v>
+      </c>
+      <c r="E62">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
         <v>95</v>
       </c>
-      <c r="D62">
-        <v>18.07</v>
-      </c>
-      <c r="E62">
-        <v>30</v>
-      </c>
-      <c r="F62" t="s">
-        <v>96</v>
-      </c>
       <c r="G62">
-        <v>39.76</v>
+        <v>13.25</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K62">
-        <v>1356</v>
+        <v>1932.9</v>
       </c>
       <c r="L62">
-        <v>1283.04</v>
+        <v>1928.34</v>
       </c>
       <c r="M62">
-        <v>1501.91</v>
+        <v>1942.02</v>
       </c>
       <c r="N62">
         <v>2</v>
@@ -3455,43 +3449,43 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C63" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D63">
-        <v>14.46</v>
+        <v>13.25</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G63">
-        <v>20.48</v>
+        <v>13.25</v>
       </c>
       <c r="H63">
         <v>1</v>
       </c>
       <c r="I63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K63">
-        <v>445.5</v>
+        <v>4562.7</v>
       </c>
       <c r="L63">
-        <v>440.09</v>
+        <v>4666.06</v>
       </c>
       <c r="M63">
-        <v>456.32</v>
+        <v>4355.98</v>
       </c>
       <c r="N63">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3499,43 +3493,43 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D64">
-        <v>12.05</v>
+        <v>13.25</v>
       </c>
       <c r="E64">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G64">
-        <v>58.19</v>
+        <v>13.25</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64">
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K64">
-        <v>3099.1</v>
+        <v>1470.9</v>
       </c>
       <c r="L64">
-        <v>2942.58</v>
+        <v>1517.96</v>
       </c>
       <c r="M64">
-        <v>3412.14</v>
+        <v>1376.79</v>
       </c>
       <c r="N64">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3543,40 +3537,40 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D65">
         <v>12.05</v>
       </c>
       <c r="E65">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="F65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G65">
-        <v>61.99</v>
+        <v>58.19</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K65">
-        <v>16765</v>
+        <v>3104</v>
       </c>
       <c r="L65">
-        <v>16113.57</v>
+        <v>2953.27</v>
       </c>
       <c r="M65">
-        <v>18067.86</v>
+        <v>3405.47</v>
       </c>
       <c r="N65">
         <v>2</v>
@@ -3587,40 +3581,40 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D66">
         <v>9.640000000000001</v>
       </c>
       <c r="E66">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="F66" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G66">
-        <v>26.51</v>
+        <v>61.99</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K66">
-        <v>195.37</v>
+        <v>16887</v>
       </c>
       <c r="L66">
-        <v>187.38</v>
+        <v>16157.57</v>
       </c>
       <c r="M66">
-        <v>211.35</v>
+        <v>18345.86</v>
       </c>
       <c r="N66">
         <v>2</v>
@@ -3631,22 +3625,22 @@
         <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D67">
-        <v>9.640000000000001</v>
+        <v>4.82</v>
       </c>
       <c r="E67">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F67" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="G67">
-        <v>60.24</v>
+        <v>22.89</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3655,150 +3649,18 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K67">
-        <v>522</v>
+        <v>6665</v>
       </c>
       <c r="L67">
-        <v>508.81</v>
+        <v>6350.98</v>
       </c>
       <c r="M67">
-        <v>548.38</v>
+        <v>7293.05</v>
       </c>
       <c r="N67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" t="s">
-        <v>86</v>
-      </c>
-      <c r="C68" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68">
-        <v>8.43</v>
-      </c>
-      <c r="E68">
-        <v>10</v>
-      </c>
-      <c r="F68" t="s">
-        <v>96</v>
-      </c>
-      <c r="G68">
-        <v>39.76</v>
-      </c>
-      <c r="H68">
-        <v>1</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="J68" t="s">
-        <v>114</v>
-      </c>
-      <c r="K68">
-        <v>1726.4</v>
-      </c>
-      <c r="L68">
-        <v>1702.39</v>
-      </c>
-      <c r="M68">
-        <v>1774.43</v>
-      </c>
-      <c r="N68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14">
-      <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" t="s">
-        <v>85</v>
-      </c>
-      <c r="C69" t="s">
-        <v>95</v>
-      </c>
-      <c r="D69">
-        <v>4.82</v>
-      </c>
-      <c r="E69">
-        <v>18</v>
-      </c>
-      <c r="F69" t="s">
-        <v>96</v>
-      </c>
-      <c r="G69">
-        <v>14.46</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69" t="s">
-        <v>114</v>
-      </c>
-      <c r="K69">
-        <v>995.15</v>
-      </c>
-      <c r="L69">
-        <v>969</v>
-      </c>
-      <c r="M69">
-        <v>1047.45</v>
-      </c>
-      <c r="N69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
-      <c r="A70" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" t="s">
-        <v>95</v>
-      </c>
-      <c r="D70">
-        <v>4.82</v>
-      </c>
-      <c r="E70">
-        <v>31</v>
-      </c>
-      <c r="F70" t="s">
-        <v>96</v>
-      </c>
-      <c r="G70">
-        <v>30.12</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70" t="s">
-        <v>114</v>
-      </c>
-      <c r="K70">
-        <v>606.65</v>
-      </c>
-      <c r="L70">
-        <v>582.26</v>
-      </c>
-      <c r="M70">
-        <v>655.4400000000001</v>
-      </c>
-      <c r="N70">
         <v>2</v>
       </c>
     </row>

</xml_diff>